<commit_message>
Output after npm start
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20312"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CEA915-C91B-4603-B145-B58E2285AFA9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934146D2-3464-4DD4-B0E1-1875BA945D38}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1200" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
   <si>
     <t>Class</t>
   </si>
@@ -293,7 +293,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,29 +303,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -340,18 +328,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,8 +370,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D119" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D119" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D37" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D37" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -695,11 +679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,1000 +709,508 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing comments annd unmapping repeated snippets
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20312"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934146D2-3464-4DD4-B0E1-1875BA945D38}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6E37C8-11D2-4D0D-AA20-D1367935E700}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1200" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
   <si>
     <t>Class</t>
   </si>
@@ -98,18 +98,6 @@
   </si>
   <si>
     <t>word-basics-insert-in-different-locations</t>
-  </si>
-  <si>
-    <t>before</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>after</t>
   </si>
   <si>
     <t>replace</t>
@@ -370,8 +358,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D37" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D37" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D33" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -679,22 +667,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,161 +696,161 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -876,7 +864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -890,7 +878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -904,7 +892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -918,7 +906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -932,7 +920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -946,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -960,256 +948,200 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>56</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Word snippet fixes (#223)
* Word snippet fixes

* Adding missing parans

* Adding missing parans

* Fixing merge conflict
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21022"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAA49D4-8094-4FA1-BA52-96BA04CF74CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310204C-FFCD-4CCC-94DD-DF63596FA9C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>Class</t>
   </si>
@@ -52,9 +52,6 @@
     <t>properties</t>
   </si>
   <si>
-    <t>run</t>
-  </si>
-  <si>
     <t>Paragraph</t>
   </si>
   <si>
@@ -275,6 +272,12 @@
   </si>
   <si>
     <t>items</t>
+  </si>
+  <si>
+    <t>addFormattedParagraph</t>
+  </si>
+  <si>
+    <t>addHeader</t>
   </si>
 </sst>
 </file>
@@ -670,19 +673,19 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,452 +699,452 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="3" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="3" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="D25" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Word snippet clean up - folders and descriptions (#226)
* Word snippet organization

* Applying feedback
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21031"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310204C-FFCD-4CCC-94DD-DF63596FA9C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB7D651-1A15-48E3-B672-A6C5457AE3C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1800" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -94,15 +94,9 @@
     <t>alignment</t>
   </si>
   <si>
-    <t>word-basics-insert-in-different-locations</t>
-  </si>
-  <si>
     <t>replace</t>
   </si>
   <si>
-    <t>word-basics-insert-and-get-pictures</t>
-  </si>
-  <si>
     <t>getImage</t>
   </si>
   <si>
@@ -118,12 +112,6 @@
     <t>Section</t>
   </si>
   <si>
-    <t>word-basics-insert-header</t>
-  </si>
-  <si>
-    <t>word-basics-insert-line-and-page-breaks</t>
-  </si>
-  <si>
     <t>insertLineBreak</t>
   </si>
   <si>
@@ -133,9 +121,6 @@
     <t>insertPageBreak</t>
   </si>
   <si>
-    <t>word-basics-insert-formatted-text</t>
-  </si>
-  <si>
     <t>insertParagraph</t>
   </si>
   <si>
@@ -145,18 +130,12 @@
     <t>wildcardSearch</t>
   </si>
   <si>
-    <t>word-basics-search</t>
-  </si>
-  <si>
     <t>search</t>
   </si>
   <si>
     <t>Body</t>
   </si>
   <si>
-    <t>word-basics-basic-doc-assembly</t>
-  </si>
-  <si>
     <t>addParagraphs</t>
   </si>
   <si>
@@ -196,9 +175,6 @@
     <t>modifyContentControls</t>
   </si>
   <si>
-    <t>word-basics-scroll-to-range</t>
-  </si>
-  <si>
     <t>scroll</t>
   </si>
   <si>
@@ -208,9 +184,6 @@
     <t>scrollEnd</t>
   </si>
   <si>
-    <t>word-range-split-words-of-first-paragraph</t>
-  </si>
-  <si>
     <t>highlightWords</t>
   </si>
   <si>
@@ -241,9 +214,6 @@
     <t>startNewList</t>
   </si>
   <si>
-    <t>word-basics-read-write-custom-document-properties</t>
-  </si>
-  <si>
     <t>insertNumericProperty</t>
   </si>
   <si>
@@ -256,9 +226,6 @@
     <t>readCustomDocumentProperties</t>
   </si>
   <si>
-    <t>word-custom-properties-get-built-in-properties</t>
-  </si>
-  <si>
     <t>getProperties</t>
   </si>
   <si>
@@ -278,6 +245,39 @@
   </si>
   <si>
     <t>addHeader</t>
+  </si>
+  <si>
+    <t>word-images-insert-and-get-pictures</t>
+  </si>
+  <si>
+    <t>word-paragraphs-insert-line-and-page-breaks</t>
+  </si>
+  <si>
+    <t>word-paragraphs-insert-formatted-text</t>
+  </si>
+  <si>
+    <t>word-paragraphs-search</t>
+  </si>
+  <si>
+    <t>word-scenarios-basic-doc-assembly</t>
+  </si>
+  <si>
+    <t>word-paragraphs-insert-header-and-footer</t>
+  </si>
+  <si>
+    <t>word-paragraphs-insert-in-different-locations</t>
+  </si>
+  <si>
+    <t>word-ranges-scroll-to-range</t>
+  </si>
+  <si>
+    <t>word-ranges-split-words-of-first-paragraph</t>
+  </si>
+  <si>
+    <t>word-properties-read-write-custom-document-properties</t>
+  </si>
+  <si>
+    <t>word-properties-get-built-in-properties</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,30 +701,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -732,13 +732,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,13 +746,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,55 +760,55 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -816,41 +816,41 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -945,38 +945,38 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -984,13 +984,13 @@
         <v>10</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -998,13 +998,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1012,41 +1012,41 @@
         <v>10</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1054,69 +1054,69 @@
         <v>10</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>7</v>
@@ -1141,10 +1141,10 @@
         <v>6</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pointing snippet at correct method
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD680FB-1F09-4A2E-8C85-BB9A27D6D356}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA85BBFD-A0E0-416D-8E0A-D4BB7ACCA0EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1800" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -319,14 +319,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,7 +672,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,464 +684,464 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="A32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (Range) Point snippet at correct method (#239)
* Pointing snippet at correct method

* Fix spacing
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD680FB-1F09-4A2E-8C85-BB9A27D6D356}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA85BBFD-A0E0-416D-8E0A-D4BB7ACCA0EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1800" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -319,14 +319,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,7 +672,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,464 +684,464 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="A32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Add Get word count snippet
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21514"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA85BBFD-A0E0-416D-8E0A-D4BB7ACCA0EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C616BB08-E0C1-4FB3-BC4B-719167B5F48B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="90">
   <si>
     <t>Class</t>
   </si>
@@ -278,6 +278,18 @@
   </si>
   <si>
     <t>word-scenarios-multiple-property-set</t>
+  </si>
+  <si>
+    <t>word-paragraph-get-word-count</t>
+  </si>
+  <si>
+    <t>paragraphs</t>
+  </si>
+  <si>
+    <t>parseText</t>
+  </si>
+  <si>
+    <t>searchAndCount</t>
   </si>
 </sst>
 </file>
@@ -319,12 +331,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,8 +372,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D33" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D35" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -668,22 +681,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -711,7 +724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -725,7 +738,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -739,7 +752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -753,7 +766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -767,7 +780,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -781,7 +794,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -795,7 +808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -809,7 +822,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -823,7 +836,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -837,7 +850,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -851,7 +864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -865,7 +878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -879,7 +892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -893,7 +906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -907,7 +920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -921,7 +934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -935,7 +948,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -949,7 +962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -963,7 +976,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -977,7 +990,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -991,7 +1004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1005,7 +1018,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +1032,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -1033,7 +1046,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -1047,7 +1060,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1074,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1075,7 +1088,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
@@ -1089,7 +1102,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1103,7 +1116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
@@ -1117,7 +1130,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1131,7 +1144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1143,6 +1156,34 @@
       </c>
       <c r="D33" s="2" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates based on feedback
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C616BB08-E0C1-4FB3-BC4B-719167B5F48B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22DE909-3244-4747-93E6-9B846ED071BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>Class</t>
   </si>
@@ -286,10 +286,7 @@
     <t>paragraphs</t>
   </si>
   <si>
-    <t>parseText</t>
-  </si>
-  <si>
-    <t>searchAndCount</t>
+    <t>run</t>
   </si>
 </sst>
 </file>
@@ -331,13 +328,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,7 +681,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1159,30 +1155,30 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>89</v>
+      <c r="D34" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Add Get word count snippet (#280)
* [Word] Add Get word count snippet

* Update snippet to include setup

* Updates based on feedback

* Minor cleanup

* Include author
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA85BBFD-A0E0-416D-8E0A-D4BB7ACCA0EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22DE909-3244-4747-93E6-9B846ED071BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>Class</t>
   </si>
@@ -278,6 +278,15 @@
   </si>
   <si>
     <t>word-scenarios-multiple-property-set</t>
+  </si>
+  <si>
+    <t>word-paragraph-get-word-count</t>
+  </si>
+  <si>
+    <t>paragraphs</t>
+  </si>
+  <si>
+    <t>run</t>
   </si>
 </sst>
 </file>
@@ -359,8 +368,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D33" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D35" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -668,22 +677,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -711,7 +720,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -725,7 +734,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -739,7 +748,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -753,7 +762,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -767,7 +776,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -781,7 +790,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -795,7 +804,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -809,7 +818,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -823,7 +832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -837,7 +846,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -851,7 +860,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -865,7 +874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -879,7 +888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -893,7 +902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -907,7 +916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -921,7 +930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -935,7 +944,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -949,7 +958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -963,7 +972,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -977,7 +986,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -991,7 +1000,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1005,7 +1014,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +1028,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -1033,7 +1042,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -1047,7 +1056,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1070,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1075,7 +1084,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
@@ -1089,7 +1098,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
@@ -1117,7 +1126,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1131,7 +1140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1143,6 +1152,34 @@
       </c>
       <c r="D33" s="2" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapping snippets to new API Documenter UID format
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22107"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22DE909-3244-4747-93E6-9B846ED071BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDB0C9E-D4EA-4DEF-98D7-6E427BB08340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
   <si>
     <t>Class</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>Member ID (methods only)</t>
   </si>
 </sst>
 </file>
@@ -368,11 +371,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E35" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{C4D3C13D-AC7C-4710-891C-E576D03BABFC}" name="Member ID (methods only)"/>
     <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="0"/>
   </tableColumns>
@@ -677,22 +681,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,485 +705,557 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1"/>
+      <c r="D30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
         <v>86</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>87</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>86</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mapping snippets to new API Documenter UID format (#348)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22107"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22DE909-3244-4747-93E6-9B846ED071BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDB0C9E-D4EA-4DEF-98D7-6E427BB08340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
   <si>
     <t>Class</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>Member ID (methods only)</t>
   </si>
 </sst>
 </file>
@@ -368,11 +371,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E35" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{C4D3C13D-AC7C-4710-891C-E576D03BABFC}" name="Member ID (methods only)"/>
     <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="0"/>
   </tableColumns>
@@ -677,22 +681,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,485 +705,557 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1"/>
+      <c r="D30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
         <v>86</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>87</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>86</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removing unneeded Word snippets
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22608"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EBB303-A601-4285-8792-1E00409E9891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA6B28-17D1-4C1F-A3AB-5E29C4333FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Class</t>
   </si>
@@ -112,9 +112,6 @@
     <t>insertBreak</t>
   </si>
   <si>
-    <t>insertPageBreak</t>
-  </si>
-  <si>
     <t>insertParagraph</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
   </si>
   <si>
     <t>Body</t>
-  </si>
-  <si>
-    <t>addParagraphs</t>
   </si>
   <si>
     <t>addContentControls</t>
@@ -371,10 +365,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E35">
-    <sortCondition ref="A1:A35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E33" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E33">
+    <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -684,11 +678,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -719,155 +713,155 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>55</v>
+      <c r="E5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
         <v>86</v>
       </c>
-      <c r="E6" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="1">
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -876,7 +870,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>62</v>
@@ -884,66 +878,66 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,16 +945,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -968,16 +962,14 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -985,16 +977,14 @@
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,14 +992,14 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="1" t="s">
-        <v>81</v>
+      <c r="D19" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1017,14 +1007,14 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1032,14 +1022,14 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1047,14 +1037,16 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1062,14 +1054,16 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,16 +1071,16 @@
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1094,16 +1088,16 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1111,33 +1105,33 @@
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1145,135 +1139,101 @@
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>85</v>
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>81</v>
+        <v>27</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="2">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing unneeded Word snippets (#397)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22608"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EBB303-A601-4285-8792-1E00409E9891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA6B28-17D1-4C1F-A3AB-5E29C4333FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Class</t>
   </si>
@@ -112,9 +112,6 @@
     <t>insertBreak</t>
   </si>
   <si>
-    <t>insertPageBreak</t>
-  </si>
-  <si>
     <t>insertParagraph</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
   </si>
   <si>
     <t>Body</t>
-  </si>
-  <si>
-    <t>addParagraphs</t>
   </si>
   <si>
     <t>addContentControls</t>
@@ -371,10 +365,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E35">
-    <sortCondition ref="A1:A35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E33" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E33">
+    <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -684,11 +678,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -719,155 +713,155 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>55</v>
+      <c r="E5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
         <v>86</v>
       </c>
-      <c r="E6" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="1">
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -876,7 +870,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>62</v>
@@ -884,66 +878,66 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,16 +945,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -968,16 +962,14 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -985,16 +977,14 @@
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,14 +992,14 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="1" t="s">
-        <v>81</v>
+      <c r="D19" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1017,14 +1007,14 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1032,14 +1022,14 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1047,14 +1037,16 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1062,14 +1054,16 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,16 +1071,16 @@
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1094,16 +1088,16 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1111,33 +1105,33 @@
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1145,135 +1139,101 @@
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>85</v>
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>81</v>
+        <v>27</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="2">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Word] (preview) Footnotes feature
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24809"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA6B28-17D1-4C1F-A3AB-5E29C4333FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A084732C-AB7D-4F1B-9EDC-C13C592D1812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
   <si>
     <t>Class</t>
   </si>
@@ -284,6 +284,63 @@
   </si>
   <si>
     <t>Member ID (methods only)</t>
+  </si>
+  <si>
+    <t>insertFootnote</t>
+  </si>
+  <si>
+    <t>word-manage-footnotes</t>
+  </si>
+  <si>
+    <t>footnotes</t>
+  </si>
+  <si>
+    <t>getFootnotesFromBody</t>
+  </si>
+  <si>
+    <t>NoteItem</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>getReference</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>getFootnoteType</t>
+  </si>
+  <si>
+    <t>getFootnotesFromRange</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>deleteFootnote</t>
+  </si>
+  <si>
+    <t>NoteItemCollection</t>
+  </si>
+  <si>
+    <t>getFirst</t>
+  </si>
+  <si>
+    <t>getFirstFootnote</t>
+  </si>
+  <si>
+    <t>getNext</t>
+  </si>
+  <si>
+    <t>getNextFootnote</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>getFootnoteBody</t>
   </si>
 </sst>
 </file>
@@ -325,12 +382,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,10 +427,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E33" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E33">
-    <sortCondition ref="A1:A33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E42" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E42" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E42">
+    <sortCondition ref="A1:A42"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -678,23 +740,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -728,7 +790,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -745,7 +807,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -762,7 +824,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -779,87 +841,84 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>84</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -873,366 +932,511 @@
         <v>73</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="1"/>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
+      <c r="D16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>20</v>
+      <c r="D18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
+      <c r="D19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>71</v>
+        <v>8</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E34" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1243,4 +1447,10 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Add sample for Comments feature
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24809"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A084732C-AB7D-4F1B-9EDC-C13C592D1812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB5ED5C-8501-460A-89B0-30F0949EC78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="122">
   <si>
     <t>Class</t>
   </si>
@@ -341,6 +341,51 @@
   </si>
   <si>
     <t>getFootnoteBody</t>
+  </si>
+  <si>
+    <t>insertComment</t>
+  </si>
+  <si>
+    <t>word-manage-comments</t>
+  </si>
+  <si>
+    <t>getComments</t>
+  </si>
+  <si>
+    <t>getCommentsInSelection</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>reply</t>
+  </si>
+  <si>
+    <t>replyToFirstCommentInSelection</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>editFirstCommentInSelection</t>
+  </si>
+  <si>
+    <t>resolved</t>
+  </si>
+  <si>
+    <t>resolveFirstCommentInSelection</t>
+  </si>
+  <si>
+    <t>deleteFirstCommentInSelection</t>
+  </si>
+  <si>
+    <t>getRange</t>
+  </si>
+  <si>
+    <t>getFirstCommentRange</t>
+  </si>
+  <si>
+    <t>CommentCollection</t>
   </si>
 </sst>
 </file>
@@ -427,10 +472,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E42" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E42" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E42">
-    <sortCondition ref="A1:A42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E52" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E52" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E52">
+    <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -740,11 +785,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,20 +819,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>31</v>
+      <c r="B2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -804,421 +849,422 @@
         <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>84</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>85</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>84</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>11</v>
+      <c r="A24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>15</v>
+      <c r="A25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>20</v>
+      <c r="A26" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>16</v>
+      <c r="D26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>17</v>
+      <c r="A27" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>17</v>
+      <c r="D27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>21</v>
+      <c r="A28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>18</v>
+      <c r="D28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>13</v>
+      <c r="A29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>22</v>
+      <c r="D29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1226,16 +1272,16 @@
         <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1243,16 +1289,16 @@
         <v>10</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1260,16 +1306,14 @@
         <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>72</v>
+        <v>8</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1277,33 +1321,29 @@
         <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
+      <c r="B34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1311,132 +1351,298 @@
         <v>10</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>88</v>
+      <c r="A38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>97</v>
+      <c r="A39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="1">
+        <v>10</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="2">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="1">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (preview) Footnotes and Comments features (#582)
* [Word] (preview) Footnotes feature

* Add sample for Comments feature

* Updates based on feedback

* Updates based on feedback
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24816"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA6B28-17D1-4C1F-A3AB-5E29C4333FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B529D69-1E4F-4194-B12C-677A7815F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="122">
   <si>
     <t>Class</t>
   </si>
@@ -284,6 +284,108 @@
   </si>
   <si>
     <t>Member ID (methods only)</t>
+  </si>
+  <si>
+    <t>insertFootnote</t>
+  </si>
+  <si>
+    <t>word-manage-footnotes</t>
+  </si>
+  <si>
+    <t>footnotes</t>
+  </si>
+  <si>
+    <t>getFootnotesFromBody</t>
+  </si>
+  <si>
+    <t>NoteItem</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>getReference</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>getFootnoteType</t>
+  </si>
+  <si>
+    <t>getFootnotesFromRange</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>deleteFootnote</t>
+  </si>
+  <si>
+    <t>NoteItemCollection</t>
+  </si>
+  <si>
+    <t>getFirst</t>
+  </si>
+  <si>
+    <t>getFirstFootnote</t>
+  </si>
+  <si>
+    <t>getNext</t>
+  </si>
+  <si>
+    <t>getNextFootnote</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>getFootnoteBody</t>
+  </si>
+  <si>
+    <t>insertComment</t>
+  </si>
+  <si>
+    <t>word-manage-comments</t>
+  </si>
+  <si>
+    <t>getComments</t>
+  </si>
+  <si>
+    <t>getCommentsInSelection</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>reply</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>editFirstCommentInSelection</t>
+  </si>
+  <si>
+    <t>resolved</t>
+  </si>
+  <si>
+    <t>deleteFirstCommentInSelection</t>
+  </si>
+  <si>
+    <t>getRange</t>
+  </si>
+  <si>
+    <t>getFirstCommentRange</t>
+  </si>
+  <si>
+    <t>CommentCollection</t>
+  </si>
+  <si>
+    <t>toggleResolvedStatusOfFirstCommentInSelection</t>
+  </si>
+  <si>
+    <t>replyToFirstActiveCommentInSelection</t>
   </si>
 </sst>
 </file>
@@ -325,12 +427,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,10 +472,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E33" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E33">
-    <sortCondition ref="A1:A33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E52" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E52" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E52">
+    <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -678,23 +785,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,24 +818,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -742,49 +849,52 @@
         <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>84</v>
@@ -793,446 +903,746 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1243,4 +1653,10 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
[Word] Add ChangeTracking snippet
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24912"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B529D69-1E4F-4194-B12C-677A7815F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4F70FC-4F83-4472-B10E-A502E5BF30CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="127">
   <si>
     <t>Class</t>
   </si>
@@ -386,6 +386,21 @@
   </si>
   <si>
     <t>replyToFirstActiveCommentInSelection</t>
+  </si>
+  <si>
+    <t>changeTrackingMode</t>
+  </si>
+  <si>
+    <t>word-manage-change-tracking</t>
+  </si>
+  <si>
+    <t>setChangeTrackingMode</t>
+  </si>
+  <si>
+    <t>getChangeTrackingMode</t>
+  </si>
+  <si>
+    <t>getReviewedText</t>
   </si>
 </sst>
 </file>
@@ -472,10 +487,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E52" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E52" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E52">
-    <sortCondition ref="A1:A52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E55" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E55" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E55">
+    <sortCondition ref="A1:A55"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -785,11 +800,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,69 +1155,65 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1210,14 +1221,16 @@
         <v>92</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
       <c r="D26" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1225,14 +1238,16 @@
         <v>92</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
       <c r="D27" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1240,65 +1255,61 @@
         <v>92</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1306,14 +1317,16 @@
         <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="1" t="s">
-        <v>79</v>
+        <v>29</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1321,14 +1334,16 @@
         <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
       <c r="D33" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1336,14 +1351,14 @@
         <v>10</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>80</v>
+      <c r="D34" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1351,14 +1366,14 @@
         <v>10</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1366,14 +1381,14 @@
         <v>10</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1381,16 +1396,14 @@
         <v>10</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1398,16 +1411,14 @@
         <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1415,16 +1426,16 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C39" s="2">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1432,16 +1443,16 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C40" s="2">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1449,33 +1460,33 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="1">
+      <c r="B42" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="2">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1483,50 +1494,50 @@
         <v>10</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>110</v>
+      <c r="E44" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1534,50 +1545,50 @@
         <v>5</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="4" t="s">
         <v>108</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>36</v>
+      <c r="B47" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C47" s="1">
         <v>1</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>35</v>
+      <c r="D47" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>88</v>
+      <c r="B48" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>88</v>
+      <c r="D48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1585,64 +1596,115 @@
         <v>5</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
       <c r="D49" s="3" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2" t="s">
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Remap snippet to Body.insertParagraph
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24922"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B529D69-1E4F-4194-B12C-677A7815F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A765B4C8-8A44-482A-8F38-F93409DD71AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -789,7 +789,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,78 +874,78 @@
         <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>84</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>85</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>84</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -953,7 +953,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -962,7 +962,7 @@
         <v>108</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -979,7 +979,7 @@
         <v>108</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -987,13 +987,16 @@
         <v>111</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1001,30 +1004,27 @@
         <v>111</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,79 +1032,79 @@
         <v>119</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>101</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1121,71 +1121,71 @@
         <v>73</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1193,7 +1193,7 @@
         <v>92</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -1202,7 +1202,7 @@
         <v>89</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1210,14 +1210,16 @@
         <v>92</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
       <c r="D26" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1225,14 +1227,14 @@
         <v>92</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1240,48 +1242,46 @@
         <v>92</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1289,16 +1289,16 @@
         <v>10</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Word] Remap snippet to Body.insertParagraph (#588)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24922"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B529D69-1E4F-4194-B12C-677A7815F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A765B4C8-8A44-482A-8F38-F93409DD71AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -789,7 +789,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,78 +874,78 @@
         <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>84</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>85</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>84</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -953,7 +953,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -962,7 +962,7 @@
         <v>108</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -979,7 +979,7 @@
         <v>108</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -987,13 +987,16 @@
         <v>111</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1001,30 +1004,27 @@
         <v>111</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,79 +1032,79 @@
         <v>119</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>101</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1121,71 +1121,71 @@
         <v>73</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1193,7 +1193,7 @@
         <v>92</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -1202,7 +1202,7 @@
         <v>89</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1210,14 +1210,16 @@
         <v>92</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
       <c r="D26" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1225,14 +1227,14 @@
         <v>92</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1240,48 +1242,46 @@
         <v>92</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1289,16 +1289,16 @@
         <v>10</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Word] (content controls) How to work with onDeleted event (#597)
* [Word] (content controls) How to work with events

* Minor cleanup

* Add track statement

* Rename sample

* Update samples/word/99-preview-apis/content-control-ondeleted-event.yaml

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>

* Map snippet

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24922"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25022"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A765B4C8-8A44-482A-8F38-F93409DD71AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E41246-125E-4FC5-85F7-089C07FE83F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="129">
   <si>
     <t>Class</t>
   </si>
@@ -386,6 +386,27 @@
   </si>
   <si>
     <t>replyToFirstActiveCommentInSelection</t>
+  </si>
+  <si>
+    <t>onDeleted</t>
+  </si>
+  <si>
+    <t>word-content-control-ondeleted-event</t>
+  </si>
+  <si>
+    <t>registerEventHandlers</t>
+  </si>
+  <si>
+    <t>contentControlDeleted</t>
+  </si>
+  <si>
+    <t>deleteContentControl</t>
+  </si>
+  <si>
+    <t>ContentControlEventArgs</t>
+  </si>
+  <si>
+    <t>contentControl</t>
   </si>
 </sst>
 </file>
@@ -472,10 +493,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E52" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E52" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E52">
-    <sortCondition ref="A1:A52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E56" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E56" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E56">
+    <sortCondition ref="A1:A56"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -785,11 +806,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,19 +840,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>109</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -921,16 +942,16 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" t="s">
         <v>91</v>
       </c>
     </row>
@@ -949,112 +970,112 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>98</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>117</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>112</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>101</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1062,288 +1083,286 @@
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>42</v>
+      <c r="B17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>46</v>
+      <c r="B18" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>4</v>
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>60</v>
+      <c r="D20" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="2">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>64</v>
+      <c r="A23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E30" s="2" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="1" t="s">
-        <v>79</v>
+      <c r="D32" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
       <c r="D34" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1351,14 +1370,16 @@
         <v>10</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
       <c r="D35" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1366,14 +1387,14 @@
         <v>10</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>80</v>
+      <c r="D36" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1381,16 +1402,14 @@
         <v>10</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1398,16 +1417,14 @@
         <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1415,16 +1432,14 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="2">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1432,16 +1447,14 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1449,33 +1462,33 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="1">
+      <c r="B42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="2">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1483,166 +1496,234 @@
         <v>10</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>110</v>
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>107</v>
+      <c r="A46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>107</v>
+      <c r="D46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+      <c r="B48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>97</v>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>78</v>
+      <c r="D50" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" s="2">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="1">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Add ChangeTracking snippet (#585)
* [Word] Add ChangeTracking snippet

* Tweak messages

* Reorder options

* run yarn start

* Display current reviewed text as well

* Apply suggestions from code review

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>

* Updates based on feedback

* Tweak

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E41246-125E-4FC5-85F7-089C07FE83F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AFE11F-78A4-475D-91E7-B478BD9834CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="136">
   <si>
     <t>Class</t>
   </si>
@@ -388,6 +388,18 @@
     <t>replyToFirstActiveCommentInSelection</t>
   </si>
   <si>
+    <t>changeTrackingMode</t>
+  </si>
+  <si>
+    <t>word-manage-change-tracking</t>
+  </si>
+  <si>
+    <t>getChangeTrackingMode</t>
+  </si>
+  <si>
+    <t>getReviewedText</t>
+  </si>
+  <si>
     <t>onDeleted</t>
   </si>
   <si>
@@ -407,13 +419,22 @@
   </si>
   <si>
     <t>contentControl</t>
+  </si>
+  <si>
+    <t>ChangeTrackingMode</t>
+  </si>
+  <si>
+    <t>ChangeTrackingVersion</t>
+  </si>
+  <si>
+    <t>enum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,13 +448,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FFE2EFDA"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -448,17 +482,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +528,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E56" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E56" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E56">
-    <sortCondition ref="A1:A56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E60" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E60" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E60">
+    <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -806,11 +841,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,10 +929,10 @@
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -971,36 +1006,30 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" t="s">
-        <v>116</v>
+        <v>133</v>
+      </c>
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" t="s">
-        <v>118</v>
+        <v>134</v>
+      </c>
+      <c r="C11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1008,7 +1037,7 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1017,7 +1046,7 @@
         <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1025,13 +1054,16 @@
         <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1039,283 +1071,281 @@
         <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>108</v>
       </c>
       <c r="E14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
         <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="D16" t="s">
         <v>108</v>
       </c>
       <c r="E16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>126</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
+      <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="2">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>62</v>
+        <v>127</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="1"/>
+      <c r="B26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="2" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
       <c r="D31" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1323,14 +1353,16 @@
         <v>92</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1338,78 +1370,78 @@
         <v>92</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
       <c r="D33" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="2">
-        <v>1</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="1" t="s">
-        <v>79</v>
+      <c r="D36" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
       <c r="D37" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1417,14 +1449,16 @@
         <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
       <c r="D38" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1432,14 +1466,14 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>80</v>
+      <c r="D39" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1447,14 +1481,14 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1462,16 +1496,14 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1479,16 +1511,14 @@
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1496,16 +1526,14 @@
         <v>10</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1513,16 +1541,16 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1530,33 +1558,33 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C45" s="2">
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="1">
+      <c r="B46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="2">
         <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1564,67 +1592,67 @@
         <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C47" s="2">
         <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C48" s="1">
+        <v>10</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="2">
         <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>79</v>
+      <c r="D49" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>108</v>
+        <v>10</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1632,16 +1660,16 @@
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1649,16 +1677,16 @@
         <v>5</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>89</v>
+      <c r="D52" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1666,64 +1694,132 @@
         <v>5</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
       <c r="D53" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>78</v>
+      <c r="D54" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="2">
+        <v>5</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="1">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="2" t="s">
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Map snippet for Word.Style enum
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25109"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AFE11F-78A4-475D-91E7-B478BD9834CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E17A0C8-27B2-4EF5-BA15-746481B2945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
   <si>
     <t>Class</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t>enum</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>addPreStyledFormattedText</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -492,6 +498,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -528,10 +538,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E60" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E60" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E60">
-    <sortCondition ref="A1:A60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E61" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E61" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E61">
+    <sortCondition ref="A1:A61"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -841,11 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,19 +1817,34 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Map snippet for Word.Style enum (#607)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25109"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AFE11F-78A4-475D-91E7-B478BD9834CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E17A0C8-27B2-4EF5-BA15-746481B2945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
   <si>
     <t>Class</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t>enum</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>addPreStyledFormattedText</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -492,6 +498,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -528,10 +538,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E60" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E60" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E60">
-    <sortCondition ref="A1:A60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E61" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E61" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E61">
+    <sortCondition ref="A1:A61"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -841,11 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,19 +1817,34 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[admin] main -> prod (#611)
* [Word] Map snippet for Word.Style enum (#607)

* moves GAed samples out of preview section of PPT

Co-authored-by: Rick Kirkham <rickeeee@msn.com>
Co-authored-by: Rick Kirkham <Rick-Kirkham@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25109"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AFE11F-78A4-475D-91E7-B478BD9834CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E17A0C8-27B2-4EF5-BA15-746481B2945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
   <si>
     <t>Class</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t>enum</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>addPreStyledFormattedText</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -492,6 +498,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -528,10 +538,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E60" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E60" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E60">
-    <sortCondition ref="A1:A60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E61" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E61" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E61">
+    <sortCondition ref="A1:A61"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -841,11 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,19 +1817,34 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (preview) How to get fields
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25229"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E17A0C8-27B2-4EF5-BA15-746481B2945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF5111D-F3B5-48DF-8384-AF5A86CFC40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-9855" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="140">
   <si>
     <t>Class</t>
   </si>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>addPreStyledFormattedText</t>
+  </si>
+  <si>
+    <t>fields</t>
+  </si>
+  <si>
+    <t>word-manage-fields</t>
   </si>
 </sst>
 </file>
@@ -462,18 +468,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFDA"/>
-        <bgColor rgb="FFE2EFDA"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -488,22 +488,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,10 +530,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E61" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E61" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E61">
-    <sortCondition ref="A1:A61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E62" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E62" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E62">
+    <sortCondition ref="A1:A62"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -851,11 +843,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,33 +898,33 @@
         <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -940,33 +932,33 @@
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -987,17 +979,17 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" t="s">
-        <v>91</v>
+      <c r="B8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1005,32 +997,32 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>124</v>
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
         <v>135</v>
@@ -1039,24 +1031,21 @@
         <v>123</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" t="s">
-        <v>116</v>
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1064,7 +1053,7 @@
         <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1073,7 +1062,7 @@
         <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1081,7 +1070,7 @@
         <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1090,7 +1079,7 @@
         <v>108</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1098,13 +1087,16 @@
         <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1112,30 +1104,27 @@
         <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
         <v>108</v>
       </c>
       <c r="E16" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
         <v>108</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1143,140 +1132,139 @@
         <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>101</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>108</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>127</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>129</v>
+      <c r="E20" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>130</v>
+      <c r="E22" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>46</v>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>129</v>
+        <v>82</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>60</v>
+        <v>127</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1293,86 +1281,86 @@
         <v>73</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="2"/>
+      <c r="B30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="2" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1380,7 +1368,7 @@
         <v>92</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -1389,7 +1377,7 @@
         <v>89</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1397,14 +1385,16 @@
         <v>92</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
       <c r="D34" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1412,14 +1402,14 @@
         <v>92</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1427,48 +1417,46 @@
         <v>92</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1476,14 +1464,16 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="1" t="s">
-        <v>79</v>
+        <v>29</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1491,14 +1481,14 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="2" t="s">
-        <v>80</v>
+      <c r="D40" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1506,14 +1496,14 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1521,14 +1511,14 @@
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1536,14 +1526,14 @@
         <v>10</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1551,16 +1541,14 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1568,16 +1556,16 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C45" s="2">
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1594,7 +1582,7 @@
         <v>71</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1602,16 +1590,16 @@
         <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C47" s="2">
         <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1619,67 +1607,67 @@
         <v>10</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C48" s="2">
         <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="1">
+      <c r="B49" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="2">
         <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="1">
+        <v>10</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="2">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1687,16 +1675,16 @@
         <v>5</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1704,16 +1692,16 @@
         <v>5</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="C53" s="1">
         <v>1</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>79</v>
+      <c r="D53" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1721,16 +1709,16 @@
         <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1738,16 +1726,16 @@
         <v>5</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>82</v>
+      <c r="D55" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1755,16 +1743,16 @@
         <v>5</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="C56" s="1">
         <v>1</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>89</v>
+      <c r="D56" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1772,79 +1760,96 @@
         <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
       <c r="D57" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C58" s="1">
-        <v>1</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>78</v>
+        <v>90</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" s="2">
+      <c r="B59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="1">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E59" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (preview) How to get fields (#627)
* [Word] (preview) How to get fields

* Updates based on feedback

* Updates based on feedback

* Minor update
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25229"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E17A0C8-27B2-4EF5-BA15-746481B2945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BD1B2C-AC61-4E38-9C39-A7907694D63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-9855" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="149">
   <si>
     <t>Class</t>
   </si>
@@ -434,6 +434,39 @@
   </si>
   <si>
     <t>addPreStyledFormattedText</t>
+  </si>
+  <si>
+    <t>fields</t>
+  </si>
+  <si>
+    <t>word-manage-fields</t>
+  </si>
+  <si>
+    <t>getAllFields</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>parentBody</t>
+  </si>
+  <si>
+    <t>getParentBodyOfFirstField</t>
+  </si>
+  <si>
+    <t>getFirstOrNullObject</t>
+  </si>
+  <si>
+    <t>getFirstField</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>FieldCollection</t>
   </si>
 </sst>
 </file>
@@ -462,18 +495,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFDA"/>
-        <bgColor rgb="FFE2EFDA"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -488,18 +515,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -538,10 +560,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E61" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E61" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E61">
-    <sortCondition ref="A1:A61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E67" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E67" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E67">
+    <sortCondition ref="A1:A67"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -851,11 +873,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,33 +928,33 @@
         <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -940,33 +962,33 @@
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -991,13 +1013,13 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1005,32 +1027,32 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>124</v>
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
         <v>135</v>
@@ -1039,24 +1061,21 @@
         <v>123</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" t="s">
-        <v>116</v>
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1064,7 +1083,7 @@
         <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1073,7 +1092,7 @@
         <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1081,7 +1100,7 @@
         <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1090,7 +1109,7 @@
         <v>108</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1098,13 +1117,16 @@
         <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1112,30 +1134,27 @@
         <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
         <v>108</v>
       </c>
       <c r="E16" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
         <v>108</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1143,140 +1162,139 @@
         <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>101</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>108</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>127</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>129</v>
+      <c r="E20" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>130</v>
+      <c r="E22" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>46</v>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>129</v>
+        <v>82</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>60</v>
+        <v>127</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1293,257 +1311,259 @@
         <v>73</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="2"/>
+      <c r="B30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="2" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>98</v>
+      <c r="A32" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>99</v>
+      <c r="D32" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>104</v>
+      <c r="A33" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>105</v>
+      <c r="A34" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>106</v>
+      <c r="D34" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>93</v>
+      <c r="A35" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>94</v>
+      <c r="D35" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>95</v>
+      <c r="A36" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>96</v>
+      <c r="D36" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>102</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="1" t="s">
-        <v>79</v>
+        <v>103</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
       <c r="D43" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1551,16 +1571,16 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1568,16 +1588,14 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="2">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>71</v>
+        <v>8</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1585,16 +1603,14 @@
         <v>10</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1602,16 +1618,14 @@
         <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1619,33 +1633,29 @@
         <v>10</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="2">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1</v>
-      </c>
+      <c r="B49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1653,118 +1663,118 @@
         <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="1">
+        <v>10</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="2">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C52" s="1">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="2">
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>108</v>
+        <v>10</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>89</v>
+        <v>10</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1772,79 +1782,181 @@
         <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1" t="s">
-        <v>89</v>
+        <v>109</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" s="2">
-        <v>1</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>137</v>
+      <c r="A60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" s="2">
+        <v>1</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (Fields) Remap sample from Field to FieldCollection
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25316"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BD1B2C-AC61-4E38-9C39-A7907694D63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4669E0C5-934E-4367-A7FE-243952718419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9855" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -515,17 +515,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,8 +872,8 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,79 +1373,79 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E35" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="5" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="2" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (Fields) Remap sample from Field to FieldCollection (#638)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25316"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BD1B2C-AC61-4E38-9C39-A7907694D63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4669E0C5-934E-4367-A7FE-243952718419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9855" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -515,17 +515,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,8 +872,8 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,79 +1373,79 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E35" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="5" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="2" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (document) How to insert section breaks (#651)
* [Word] (document) How to insert section breaks

* Update samples/word/50-document/insert-section-breaks.yaml

Co-authored-by: David Chesnut <davech@microsoft.com>

* Metadata mapping

Co-authored-by: David Chesnut <davech@microsoft.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25316"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25408"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4669E0C5-934E-4367-A7FE-243952718419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA77E29-655D-4933-B856-3C13A265198F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="154">
   <si>
     <t>Class</t>
   </si>
@@ -289,9 +289,6 @@
     <t>insertFootnote</t>
   </si>
   <si>
-    <t>word-manage-footnotes</t>
-  </si>
-  <si>
     <t>footnotes</t>
   </si>
   <si>
@@ -346,9 +343,6 @@
     <t>insertComment</t>
   </si>
   <si>
-    <t>word-manage-comments</t>
-  </si>
-  <si>
     <t>getComments</t>
   </si>
   <si>
@@ -391,9 +385,6 @@
     <t>changeTrackingMode</t>
   </si>
   <si>
-    <t>word-manage-change-tracking</t>
-  </si>
-  <si>
     <t>getChangeTrackingMode</t>
   </si>
   <si>
@@ -467,6 +458,30 @@
   </si>
   <si>
     <t>FieldCollection</t>
+  </si>
+  <si>
+    <t>word-document-insert-section-breaks</t>
+  </si>
+  <si>
+    <t>addNext</t>
+  </si>
+  <si>
+    <t>SectionCollection</t>
+  </si>
+  <si>
+    <t>addEven</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>word-document-manage-comments</t>
+  </si>
+  <si>
+    <t>word-document-manage-footnotes</t>
+  </si>
+  <si>
+    <t>word-document-manage-change-tracking</t>
   </si>
 </sst>
 </file>
@@ -556,10 +571,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E67" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E67" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E67">
-    <sortCondition ref="A1:A67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E69" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E69" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E69">
+    <sortCondition ref="A1:A69"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -869,11 +884,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,16 +922,16 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1009,13 +1024,13 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1023,13 +1038,13 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
         <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1048,140 +1063,140 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" t="s">
         <v>111</v>
       </c>
-      <c r="B16" t="s">
-        <v>113</v>
-      </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
         <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1189,16 +1204,16 @@
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" t="s">
         <v>127</v>
-      </c>
-      <c r="E20" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1223,13 +1238,13 @@
         <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1237,13 +1252,13 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" t="s">
         <v>126</v>
-      </c>
-      <c r="D23" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1280,17 +1295,17 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1347,14 +1362,14 @@
         <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1374,79 +1389,79 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1468,98 +1483,98 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C39" s="2">
-        <v>1</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1778,16 +1793,16 @@
         <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C57" s="1">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1795,16 +1810,16 @@
         <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1829,16 +1844,16 @@
         <v>5</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1869,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>88</v>
@@ -1880,79 +1895,109 @@
         <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>78</v>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C65" s="2">
+      <c r="B65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" s="1">
         <v>1</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2" t="s">
-        <v>135</v>
+        <v>27</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C67" s="1">
-        <v>1</v>
-      </c>
-      <c r="D67" s="2" t="s">
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (TableCell) Map existing sample
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25414"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA77E29-655D-4933-B856-3C13A265198F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D35BC9D-9A13-43E5-B760-0C7D8D9E9F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="155">
   <si>
     <t>Class</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t>word-document-manage-change-tracking</t>
+  </si>
+  <si>
+    <t>TableCell</t>
   </si>
 </sst>
 </file>
@@ -530,13 +533,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +575,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E69" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E69" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E70" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E70" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E69">
     <sortCondition ref="A1:A69"/>
   </sortState>
@@ -884,11 +888,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2001,6 +2005,21 @@
         <v>54</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" t="s">
+        <v>150</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Word] (TableCell) Map existing sample (#658)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25414"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA77E29-655D-4933-B856-3C13A265198F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D35BC9D-9A13-43E5-B760-0C7D8D9E9F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="155">
   <si>
     <t>Class</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t>word-document-manage-change-tracking</t>
+  </si>
+  <si>
+    <t>TableCell</t>
   </si>
 </sst>
 </file>
@@ -530,13 +533,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +575,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E69" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E69" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E70" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E70" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E69">
     <sortCondition ref="A1:A69"/>
   </sortState>
@@ -884,11 +888,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2001,6 +2005,21 @@
         <v>54</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" t="s">
+        <v>150</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Word] (paragraph) Show how to use other HeaderFooterType options (#657)
* [Word] (paragraph) Show how to use other HeaderFooterType options

* Updates based on feedback

* Add missing word

* Updates per feedback
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25414"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D35BC9D-9A13-43E5-B760-0C7D8D9E9F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191EC940-2021-4C83-AFBE-B561584DE7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="156">
   <si>
     <t>Class</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>TableCell</t>
+  </si>
+  <si>
+    <t>HeaderFooterType</t>
   </si>
 </sst>
 </file>
@@ -533,14 +536,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +581,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E70" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E70" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E69">
-    <sortCondition ref="A1:A69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E71" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E71" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E70">
+    <sortCondition ref="A1:A70"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -888,11 +894,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1469,37 +1475,35 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>23</v>
+      <c r="A37" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1507,7 +1511,7 @@
         <v>91</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C39" s="2">
         <v>1</v>
@@ -1516,7 +1520,7 @@
         <v>152</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1524,14 +1528,16 @@
         <v>91</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
       <c r="D40" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1539,14 +1545,14 @@
         <v>91</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1554,48 +1560,46 @@
         <v>91</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1603,14 +1607,16 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="1" t="s">
-        <v>79</v>
+        <v>29</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1618,14 +1624,14 @@
         <v>10</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="2" t="s">
-        <v>80</v>
+      <c r="D46" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1633,14 +1639,14 @@
         <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1648,14 +1654,14 @@
         <v>10</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1663,14 +1669,14 @@
         <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1678,16 +1684,14 @@
         <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1695,16 +1699,16 @@
         <v>10</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1721,7 +1725,7 @@
         <v>71</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1729,16 +1733,16 @@
         <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C53" s="2">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1746,67 +1750,67 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C54" s="2">
         <v>1</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="1">
+      <c r="B55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="2">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C57" s="1">
+        <v>10</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="2">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>151</v>
+        <v>83</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1814,16 +1818,16 @@
         <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1831,16 +1835,16 @@
         <v>5</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>79</v>
+      <c r="D59" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1848,16 +1852,16 @@
         <v>5</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1865,16 +1869,16 @@
         <v>5</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="C61" s="1">
         <v>1</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>82</v>
+      <c r="D61" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1882,16 +1886,16 @@
         <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>152</v>
+      <c r="D62" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1899,124 +1903,140 @@
         <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C63" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
       <c r="D63" s="1" t="s">
         <v>152</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1" t="s">
-        <v>150</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>78</v>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C66" s="2">
+      <c r="B66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2" t="s">
-        <v>150</v>
+        <v>27</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C69" s="1">
-        <v>1</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B70" s="4"/>
-      <c r="C70" t="s">
-        <v>150</v>
+      <c r="C70" s="1">
+        <v>1</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>52</v>
       </c>
       <c r="E70" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C71" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (enums) Map to existing snippets
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191EC940-2021-4C83-AFBE-B561584DE7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFC1C64-659F-4D49-BBC7-428F591EEF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="163">
   <si>
     <t>Class</t>
   </si>
@@ -488,6 +488,27 @@
   </si>
   <si>
     <t>HeaderFooterType</t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>setup</t>
+  </si>
+  <si>
+    <t>BreakType</t>
+  </si>
+  <si>
+    <t>insertPageBreak</t>
+  </si>
+  <si>
+    <t>InsertLocation</t>
+  </si>
+  <si>
+    <t>addContinuous</t>
+  </si>
+  <si>
+    <t>NoteItemType</t>
   </si>
 </sst>
 </file>
@@ -536,17 +557,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +603,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E71" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E71" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E70">
-    <sortCondition ref="A1:A70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E75" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E75" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E74">
+    <sortCondition ref="A1:A74"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -894,11 +916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,71 +950,69 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>107</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>151</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1009,24 +1029,24 @@
         <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1034,13 +1054,16 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1048,13 +1071,13 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1062,75 +1085,70 @@
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>121</v>
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>131</v>
-      </c>
+      <c r="A12" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" t="s">
         <v>132</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>122</v>
+        <v>75</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1138,7 +1156,7 @@
         <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1147,7 +1165,7 @@
         <v>151</v>
       </c>
       <c r="E15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1155,13 +1173,16 @@
         <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>151</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1169,78 +1190,75 @@
         <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>151</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
         <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
         <v>151</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1248,183 +1266,187 @@
         <v>44</v>
       </c>
       <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>123</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>124</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>126</v>
+        <v>43</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>62</v>
+        <v>124</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="1"/>
       <c r="D32" s="2" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1432,7 +1454,7 @@
         <v>138</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
@@ -1444,115 +1466,111 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>69</v>
+      <c r="A37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="2">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="C40" s="2">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>105</v>
+      <c r="A41" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1560,14 +1578,16 @@
         <v>91</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
       <c r="D42" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1575,93 +1595,93 @@
         <v>91</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
       <c r="D43" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="1" t="s">
-        <v>79</v>
+      <c r="D46" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
       <c r="D47" s="2" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="2"/>
+      <c r="A48" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
       <c r="D48" s="2" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1669,14 +1689,16 @@
         <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
       <c r="D49" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1684,14 +1706,14 @@
         <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="2" t="s">
-        <v>80</v>
+      <c r="D50" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1699,16 +1721,14 @@
         <v>10</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1716,16 +1736,14 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1733,16 +1751,14 @@
         <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C53" s="2">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1750,16 +1766,14 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1767,33 +1781,33 @@
         <v>10</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="1">
+      <c r="B56" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="2">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1801,84 +1815,84 @@
         <v>10</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C57" s="2">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C58" s="1">
+        <v>10</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>151</v>
+        <v>72</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59" s="1">
+        <v>10</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="2">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>79</v>
+      <c r="D60" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1886,16 +1900,16 @@
         <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,16 +1917,16 @@
         <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="C63" s="1">
         <v>1</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>152</v>
+      <c r="D63" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1920,123 +1934,191 @@
         <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C64" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
       <c r="D64" s="1" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1" t="s">
-        <v>150</v>
+        <v>5</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C67" s="2">
-        <v>1</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>146</v>
+        <v>5</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>76</v>
+        <v>27</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" s="2">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>154</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C75" t="s">
         <v>150</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (enums) Map to existing snippets (#662)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191EC940-2021-4C83-AFBE-B561584DE7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFC1C64-659F-4D49-BBC7-428F591EEF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="163">
   <si>
     <t>Class</t>
   </si>
@@ -488,6 +488,27 @@
   </si>
   <si>
     <t>HeaderFooterType</t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>setup</t>
+  </si>
+  <si>
+    <t>BreakType</t>
+  </si>
+  <si>
+    <t>insertPageBreak</t>
+  </si>
+  <si>
+    <t>InsertLocation</t>
+  </si>
+  <si>
+    <t>addContinuous</t>
+  </si>
+  <si>
+    <t>NoteItemType</t>
   </si>
 </sst>
 </file>
@@ -536,17 +557,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +603,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E71" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E71" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E70">
-    <sortCondition ref="A1:A70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E75" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E75" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E74">
+    <sortCondition ref="A1:A74"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -894,11 +916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,71 +950,69 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>107</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>151</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1009,24 +1029,24 @@
         <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1034,13 +1054,16 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1048,13 +1071,13 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1062,75 +1085,70 @@
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>121</v>
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>131</v>
-      </c>
+      <c r="A12" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" t="s">
         <v>132</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>122</v>
+        <v>75</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1138,7 +1156,7 @@
         <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1147,7 +1165,7 @@
         <v>151</v>
       </c>
       <c r="E15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1155,13 +1173,16 @@
         <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>151</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1169,78 +1190,75 @@
         <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>151</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
         <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
         <v>151</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1248,183 +1266,187 @@
         <v>44</v>
       </c>
       <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>123</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>124</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>126</v>
+        <v>43</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>62</v>
+        <v>124</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="1"/>
       <c r="D32" s="2" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1432,7 +1454,7 @@
         <v>138</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
@@ -1444,115 +1466,111 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>69</v>
+      <c r="A37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="2">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="C40" s="2">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>105</v>
+      <c r="A41" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1560,14 +1578,16 @@
         <v>91</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
       <c r="D42" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1575,93 +1595,93 @@
         <v>91</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
       <c r="D43" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="1" t="s">
-        <v>79</v>
+      <c r="D46" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
       <c r="D47" s="2" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="2"/>
+      <c r="A48" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
       <c r="D48" s="2" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1669,14 +1689,16 @@
         <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
       <c r="D49" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1684,14 +1706,14 @@
         <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="2" t="s">
-        <v>80</v>
+      <c r="D50" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1699,16 +1721,14 @@
         <v>10</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1716,16 +1736,14 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1733,16 +1751,14 @@
         <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C53" s="2">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1750,16 +1766,14 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1767,33 +1781,33 @@
         <v>10</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="1">
+      <c r="B56" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="2">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1801,84 +1815,84 @@
         <v>10</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C57" s="2">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C58" s="1">
+        <v>10</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>151</v>
+        <v>72</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59" s="1">
+        <v>10</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="2">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>79</v>
+      <c r="D60" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1886,16 +1900,16 @@
         <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,16 +1917,16 @@
         <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="C63" s="1">
         <v>1</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>152</v>
+      <c r="D63" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1920,123 +1934,191 @@
         <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C64" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
       <c r="D64" s="1" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1" t="s">
-        <v>150</v>
+        <v>5</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C67" s="2">
-        <v>1</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>146</v>
+        <v>5</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>76</v>
+        <v>27</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" s="2">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>154</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C75" t="s">
         <v>150</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Map existing examples to enums
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFC1C64-659F-4D49-BBC7-428F591EEF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5057CCD-6790-4FD3-B79A-EB9DEFDFE550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="166">
   <si>
     <t>Class</t>
   </si>
@@ -509,6 +509,15 @@
   </si>
   <si>
     <t>NoteItemType</t>
+  </si>
+  <si>
+    <t>ContentControlAppearance</t>
+  </si>
+  <si>
+    <t>RangeLocation</t>
+  </si>
+  <si>
+    <t>SelectionMode</t>
   </si>
 </sst>
 </file>
@@ -565,10 +574,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +612,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E75" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E75" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E74">
-    <sortCondition ref="A1:A74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E79" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E79" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
+    <sortCondition ref="A1:A78"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -916,11 +925,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,10 +959,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="4"/>
       <c r="C2" t="s">
         <v>132</v>
       </c>
@@ -1109,17 +1117,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="4"/>
       <c r="C12" t="s">
         <v>132</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1339,52 +1346,50 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
+      <c r="A27" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" t="s">
+        <v>132</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
       <c r="D28" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1401,67 +1406,69 @@
         <v>73</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="1"/>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
       <c r="D31" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="2" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="2"/>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1"/>
       <c r="D33" s="2" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1469,14 +1476,14 @@
         <v>138</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1484,26 +1491,24 @@
         <v>138</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>136</v>
       </c>
@@ -1516,78 +1521,78 @@
         <v>145</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
       <c r="D38" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="2">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" s="2">
-        <v>1</v>
+        <v>160</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>98</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1595,7 +1600,7 @@
         <v>91</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -1604,7 +1609,7 @@
         <v>152</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1612,14 +1617,16 @@
         <v>91</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
       <c r="D44" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,14 +1634,14 @@
         <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1642,78 +1649,77 @@
         <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B48" s="4"/>
-      <c r="C48" t="s">
-        <v>132</v>
+      <c r="A48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="2">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="2"/>
+      <c r="B50" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
       <c r="D50" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>11</v>
+      <c r="E50" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1721,14 +1727,16 @@
         <v>10</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
       <c r="D51" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1736,14 +1744,16 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1</v>
+      </c>
       <c r="D52" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1751,14 +1761,16 @@
         <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C53" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1766,14 +1778,16 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
       <c r="D54" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1781,16 +1795,16 @@
         <v>10</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1798,33 +1812,33 @@
         <v>10</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C56" s="2">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="2">
+      <c r="B57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="1">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1832,16 +1846,16 @@
         <v>10</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1849,33 +1863,29 @@
         <v>10</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
+      <c r="B60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1883,50 +1893,44 @@
         <v>10</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>153</v>
+        <v>10</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1934,16 +1938,16 @@
         <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>79</v>
+      <c r="D64" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1951,16 +1955,16 @@
         <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C65" s="1">
         <v>1</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>151</v>
+      <c r="D65" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1968,16 +1972,16 @@
         <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>82</v>
+      <c r="D66" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1985,16 +1989,16 @@
         <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2002,123 +2006,187 @@
         <v>5</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1" t="s">
-        <v>152</v>
+        <v>36</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1" t="s">
-        <v>150</v>
+        <v>5</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>147</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C71" s="2">
-        <v>1</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>40</v>
+      <c r="A71" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="1">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2" t="s">
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>154</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C79" t="s">
         <v>150</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Map existing examples to enums (#664)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFC1C64-659F-4D49-BBC7-428F591EEF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5057CCD-6790-4FD3-B79A-EB9DEFDFE550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="166">
   <si>
     <t>Class</t>
   </si>
@@ -509,6 +509,15 @@
   </si>
   <si>
     <t>NoteItemType</t>
+  </si>
+  <si>
+    <t>ContentControlAppearance</t>
+  </si>
+  <si>
+    <t>RangeLocation</t>
+  </si>
+  <si>
+    <t>SelectionMode</t>
   </si>
 </sst>
 </file>
@@ -565,10 +574,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +612,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E75" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E75" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E74">
-    <sortCondition ref="A1:A74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E79" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E79" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
+    <sortCondition ref="A1:A78"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -916,11 +925,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,10 +959,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="4"/>
       <c r="C2" t="s">
         <v>132</v>
       </c>
@@ -1109,17 +1117,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="4"/>
       <c r="C12" t="s">
         <v>132</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1339,52 +1346,50 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
+      <c r="A27" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" t="s">
+        <v>132</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
       <c r="D28" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1401,67 +1406,69 @@
         <v>73</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="1"/>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
       <c r="D31" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="2" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="2"/>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1"/>
       <c r="D33" s="2" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1469,14 +1476,14 @@
         <v>138</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1484,26 +1491,24 @@
         <v>138</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>136</v>
       </c>
@@ -1516,78 +1521,78 @@
         <v>145</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
       <c r="D38" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="2">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" s="2">
-        <v>1</v>
+        <v>160</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>98</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1595,7 +1600,7 @@
         <v>91</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -1604,7 +1609,7 @@
         <v>152</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1612,14 +1617,16 @@
         <v>91</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
       <c r="D44" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,14 +1634,14 @@
         <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1642,78 +1649,77 @@
         <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B48" s="4"/>
-      <c r="C48" t="s">
-        <v>132</v>
+      <c r="A48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="2">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="2"/>
+      <c r="B50" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
       <c r="D50" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>11</v>
+      <c r="E50" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1721,14 +1727,16 @@
         <v>10</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
       <c r="D51" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1736,14 +1744,16 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1</v>
+      </c>
       <c r="D52" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1751,14 +1761,16 @@
         <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C53" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1766,14 +1778,16 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
       <c r="D54" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1781,16 +1795,16 @@
         <v>10</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1798,33 +1812,33 @@
         <v>10</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C56" s="2">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="2">
+      <c r="B57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="1">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1832,16 +1846,16 @@
         <v>10</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1849,33 +1863,29 @@
         <v>10</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
+      <c r="B60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1883,50 +1893,44 @@
         <v>10</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>153</v>
+        <v>10</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1934,16 +1938,16 @@
         <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>79</v>
+      <c r="D64" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1951,16 +1955,16 @@
         <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C65" s="1">
         <v>1</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>151</v>
+      <c r="D65" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1968,16 +1972,16 @@
         <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>82</v>
+      <c r="D66" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1985,16 +1989,16 @@
         <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2002,123 +2006,187 @@
         <v>5</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1" t="s">
-        <v>152</v>
+        <v>36</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1" t="s">
-        <v>150</v>
+        <v>5</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>147</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C71" s="2">
-        <v>1</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>40</v>
+      <c r="A71" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="1">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2" t="s">
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>154</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C79" t="s">
         <v>150</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Update existing sample to show EventType
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25506"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25602"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5057CCD-6790-4FD3-B79A-EB9DEFDFE550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28AAF0A-0373-401E-8187-393FFE8922A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="168">
   <si>
     <t>Class</t>
   </si>
@@ -518,6 +518,12 @@
   </si>
   <si>
     <t>SelectionMode</t>
+  </si>
+  <si>
+    <t>eventType</t>
+  </si>
+  <si>
+    <t>EventType</t>
   </si>
 </sst>
 </file>
@@ -566,18 +572,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +613,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E79" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E79" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
-    <sortCondition ref="A1:A78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E81" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E81" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E80">
+    <sortCondition ref="A1:A80"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -925,11 +926,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1346,17 +1347,16 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" t="s">
         <v>163</v>
       </c>
-      <c r="B27" s="4"/>
       <c r="C27" t="s">
         <v>132</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1394,19 +1394,17 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1423,82 +1421,84 @@
         <v>73</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="1"/>
+      <c r="B32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="2" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="2"/>
+      <c r="B34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="1"/>
       <c r="D34" s="2" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="D36" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>140</v>
+        <v>124</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1506,7 +1506,7 @@
         <v>138</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
@@ -1518,115 +1518,111 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2" t="s">
-        <v>132</v>
+        <v>145</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
         <v>132</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>161</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1</v>
+        <v>160</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1634,14 +1630,16 @@
         <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
       <c r="D45" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1649,14 +1647,16 @@
         <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
       <c r="D46" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1664,40 +1664,39 @@
         <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>162</v>
-      </c>
-      <c r="C49" t="s">
-        <v>132</v>
-      </c>
+      <c r="A49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
         <v>152</v>
       </c>
@@ -1706,37 +1705,34 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>115</v>
+      <c r="A50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>12</v>
+      <c r="D50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="2">
-        <v>1</v>
+      <c r="A51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" t="s">
+        <v>132</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1744,16 +1740,16 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="C52" s="2">
         <v>1</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>81</v>
+      <c r="D52" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1761,16 +1757,16 @@
         <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C53" s="2">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1778,16 +1774,16 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C54" s="2">
         <v>1</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1795,16 +1791,16 @@
         <v>10</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1812,33 +1808,33 @@
         <v>10</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C56" s="2">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="1">
+      <c r="B57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" s="2">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1846,31 +1842,33 @@
         <v>10</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C59" s="2"/>
+      <c r="B59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
       <c r="D59" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1878,14 +1876,16 @@
         <v>10</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C60" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
       <c r="D60" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1893,14 +1893,14 @@
         <v>10</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1908,14 +1908,14 @@
         <v>10</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1923,48 +1923,44 @@
         <v>10</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C63" s="2"/>
-      <c r="D63" s="1" t="s">
-        <v>79</v>
+      <c r="D63" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>153</v>
+        <v>10</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1972,16 +1968,16 @@
         <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>79</v>
+      <c r="D66" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1989,16 +1985,16 @@
         <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>151</v>
+      <c r="D67" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2006,16 +2002,16 @@
         <v>5</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C68" s="1">
         <v>1</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>82</v>
+      <c r="D68" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,16 +2019,16 @@
         <v>5</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C69" s="1">
         <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2040,153 +2036,187 @@
         <v>5</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>12</v>
+      <c r="E71" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1" t="s">
-        <v>150</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>78</v>
+        <v>164</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C74" s="2">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>78</v>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2" t="s">
-        <v>150</v>
+        <v>27</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>149</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B76" s="6"/>
-      <c r="C76" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>71</v>
+      <c r="A76" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C78" s="1">
-        <v>1</v>
-      </c>
-      <c r="D78" s="2" t="s">
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>154</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>150</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Update existing sample to show EventType (#682)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25506"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25602"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5057CCD-6790-4FD3-B79A-EB9DEFDFE550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28AAF0A-0373-401E-8187-393FFE8922A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="168">
   <si>
     <t>Class</t>
   </si>
@@ -518,6 +518,12 @@
   </si>
   <si>
     <t>SelectionMode</t>
+  </si>
+  <si>
+    <t>eventType</t>
+  </si>
+  <si>
+    <t>EventType</t>
   </si>
 </sst>
 </file>
@@ -566,18 +572,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +613,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E79" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E79" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
-    <sortCondition ref="A1:A78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E81" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E81" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E80">
+    <sortCondition ref="A1:A80"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -925,11 +926,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1346,17 +1347,16 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" t="s">
         <v>163</v>
       </c>
-      <c r="B27" s="4"/>
       <c r="C27" t="s">
         <v>132</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1394,19 +1394,17 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1423,82 +1421,84 @@
         <v>73</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="1"/>
+      <c r="B32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="2" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="2"/>
+      <c r="B34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="1"/>
       <c r="D34" s="2" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="D36" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>140</v>
+        <v>124</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1506,7 +1506,7 @@
         <v>138</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
@@ -1518,115 +1518,111 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2" t="s">
-        <v>132</v>
+        <v>145</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
         <v>132</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>161</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1</v>
+        <v>160</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1634,14 +1630,16 @@
         <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
       <c r="D45" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1649,14 +1647,16 @@
         <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
       <c r="D46" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1664,40 +1664,39 @@
         <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>162</v>
-      </c>
-      <c r="C49" t="s">
-        <v>132</v>
-      </c>
+      <c r="A49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
         <v>152</v>
       </c>
@@ -1706,37 +1705,34 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>115</v>
+      <c r="A50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>12</v>
+      <c r="D50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="2">
-        <v>1</v>
+      <c r="A51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" t="s">
+        <v>132</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1744,16 +1740,16 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="C52" s="2">
         <v>1</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>81</v>
+      <c r="D52" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1761,16 +1757,16 @@
         <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C53" s="2">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1778,16 +1774,16 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C54" s="2">
         <v>1</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1795,16 +1791,16 @@
         <v>10</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1812,33 +1808,33 @@
         <v>10</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C56" s="2">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="1">
+      <c r="B57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" s="2">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1846,31 +1842,33 @@
         <v>10</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C59" s="2"/>
+      <c r="B59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
       <c r="D59" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1878,14 +1876,16 @@
         <v>10</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C60" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
       <c r="D60" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1893,14 +1893,14 @@
         <v>10</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1908,14 +1908,14 @@
         <v>10</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1923,48 +1923,44 @@
         <v>10</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C63" s="2"/>
-      <c r="D63" s="1" t="s">
-        <v>79</v>
+      <c r="D63" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>153</v>
+        <v>10</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1972,16 +1968,16 @@
         <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>79</v>
+      <c r="D66" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1989,16 +1985,16 @@
         <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>151</v>
+      <c r="D67" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2006,16 +2002,16 @@
         <v>5</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C68" s="1">
         <v>1</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>82</v>
+      <c r="D68" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,16 +2019,16 @@
         <v>5</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C69" s="1">
         <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2040,153 +2036,187 @@
         <v>5</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>12</v>
+      <c r="E71" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1" t="s">
-        <v>150</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>78</v>
+        <v>164</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C74" s="2">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>78</v>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2" t="s">
-        <v>150</v>
+        <v>27</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>149</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B76" s="6"/>
-      <c r="C76" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>71</v>
+      <c r="A76" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C78" s="1">
-        <v>1</v>
-      </c>
-      <c r="D78" s="2" t="s">
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>154</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>150</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (1,4, HiddenDocument 1.4) Promote to GA
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25710"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E42BE97-36F5-430E-B2ED-B3AE75953C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B85E242-42AA-4446-BAF4-22EA200A69E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="171">
   <si>
     <t>Class</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>Word</t>
+  </si>
+  <si>
+    <t>word-document-manage-fields</t>
   </si>
 </sst>
 </file>
@@ -955,20 +958,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A81"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.53125" customWidth="1"/>
-    <col min="3" max="3" width="26.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -988,7 +991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>169</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>169</v>
       </c>
@@ -1125,7 +1128,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>169</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>169</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>169</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -1210,7 +1213,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>169</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>169</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>169</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>169</v>
       </c>
@@ -1287,7 +1290,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>169</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>169</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>169</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>169</v>
       </c>
@@ -1378,7 +1381,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>169</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>169</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>169</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>169</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>169</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>169</v>
       </c>
@@ -1487,7 +1490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>169</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>169</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>169</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>169</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>169</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>169</v>
       </c>
@@ -1617,7 +1620,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>169</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -1647,13 +1650,13 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>169</v>
       </c>
@@ -1665,13 +1668,13 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -1683,13 +1686,13 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>169</v>
       </c>
@@ -1703,13 +1706,13 @@
         <v>1</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>169</v>
       </c>
@@ -1721,13 +1724,13 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>169</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>169</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>169</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>169</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>169</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>169</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>169</v>
       </c>
@@ -1897,7 +1900,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -1914,7 +1917,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>169</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>169</v>
       </c>
@@ -1974,7 +1977,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>169</v>
       </c>
@@ -1994,7 +1997,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>169</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>169</v>
       </c>
@@ -2034,7 +2037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>169</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>169</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>169</v>
       </c>
@@ -2112,7 +2115,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>169</v>
       </c>
@@ -2148,7 +2151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>169</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>169</v>
       </c>
@@ -2184,7 +2187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>169</v>
       </c>
@@ -2204,7 +2207,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>169</v>
       </c>
@@ -2224,7 +2227,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>169</v>
       </c>
@@ -2244,7 +2247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>169</v>
       </c>
@@ -2264,7 +2267,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>169</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>169</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>169</v>
       </c>
@@ -2340,7 +2343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>169</v>
       </c>
@@ -2358,7 +2361,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>169</v>
       </c>
@@ -2378,7 +2381,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>169</v>
       </c>
@@ -2398,7 +2401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>169</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>169</v>
       </c>
@@ -2434,7 +2437,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>169</v>
       </c>
@@ -2452,7 +2455,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>169</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
[Word] Update metadata reference
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E42BE97-36F5-430E-B2ED-B3AE75953C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C93631C-770D-4623-BCFA-D70B19A92A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -954,21 +954,21 @@
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A81"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.53125" customWidth="1"/>
-    <col min="3" max="3" width="26.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -988,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>76</v>
@@ -1045,7 +1045,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>169</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>169</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>169</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>169</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>169</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>169</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>169</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>169</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>169</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>169</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>169</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>169</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>169</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>169</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>169</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>169</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>169</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>169</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>169</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>169</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>169</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>169</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>169</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>169</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>169</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>169</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>169</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>169</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>169</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>169</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>169</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>169</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>169</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>169</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>169</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>169</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>169</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>169</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>169</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>169</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>169</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>169</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>169</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>169</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>169</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>169</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>169</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>169</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>169</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>169</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>169</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>169</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>169</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>169</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>169</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>169</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>169</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>169</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>169</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>169</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>169</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
[Word] Update metadata reference (#700)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E42BE97-36F5-430E-B2ED-B3AE75953C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C93631C-770D-4623-BCFA-D70B19A92A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -954,21 +954,21 @@
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A81"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.53125" customWidth="1"/>
-    <col min="3" max="3" width="26.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -988,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>76</v>
@@ -1045,7 +1045,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>169</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>169</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>169</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>169</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>169</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>169</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>169</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>169</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>169</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>169</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>169</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>169</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>169</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>169</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>169</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>169</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>169</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>169</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>169</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>169</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>169</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>169</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>169</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>169</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>169</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>169</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>169</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>169</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>169</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>169</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>169</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>169</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>169</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>169</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>169</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>169</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>169</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>169</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>169</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>169</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>169</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>169</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>169</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>169</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>169</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>169</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>169</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>169</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>169</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>169</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>169</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>169</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>169</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>169</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>169</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>169</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>169</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>169</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>169</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>169</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>169</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
[Word] (1.4) Promote to GA (#699)
* [Word] (1,4, HiddenDocument 1.4) Promote to GA

* Update fields snippets based on feedback that design changed
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C93631C-770D-4623-BCFA-D70B19A92A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B578329-F858-4666-B6D6-7FB8F58644EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -430,9 +430,6 @@
     <t>fields</t>
   </si>
   <si>
-    <t>word-manage-fields</t>
-  </si>
-  <si>
     <t>getAllFields</t>
   </si>
   <si>
@@ -530,6 +527,9 @@
   </si>
   <si>
     <t>Word</t>
+  </si>
+  <si>
+    <t>word-document-manage-fields</t>
   </si>
 </sst>
 </file>
@@ -955,7 +955,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -970,7 +970,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -990,10 +990,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
         <v>132</v>
@@ -1002,12 +1002,12 @@
         <v>80</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -1019,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" t="s">
         <v>107</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>34</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -1136,15 +1136,15 @@
         <v>135</v>
       </c>
       <c r="E9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" t="s">
         <v>136</v>
-      </c>
-      <c r="F9" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -1153,7 +1153,7 @@
         <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F10" t="s">
         <v>90</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
@@ -1178,10 +1178,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
         <v>132</v>
@@ -1190,12 +1190,12 @@
         <v>75</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
         <v>130</v>
@@ -1204,7 +1204,7 @@
         <v>132</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>121</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
         <v>131</v>
@@ -1221,7 +1221,7 @@
         <v>132</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>122</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
         <v>109</v>
@@ -1241,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15" t="s">
         <v>114</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
         <v>109</v>
@@ -1261,7 +1261,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F16" t="s">
         <v>116</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
         <v>109</v>
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F17" t="s">
         <v>119</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
         <v>109</v>
@@ -1298,7 +1298,7 @@
         <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F18" t="s">
         <v>112</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
         <v>109</v>
@@ -1315,7 +1315,7 @@
         <v>113</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F19" t="s">
         <v>118</v>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
         <v>117</v>
@@ -1335,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F20" t="s">
         <v>116</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
         <v>117</v>
@@ -1352,7 +1352,7 @@
         <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F21" t="s">
         <v>119</v>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
         <v>44</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>44</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>44</v>
@@ -1452,10 +1452,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s">
         <v>132</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>39</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>128</v>
@@ -1507,13 +1507,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
@@ -1525,7 +1525,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>61</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>61</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>61</v>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>65</v>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>121</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>65</v>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
@@ -1637,102 +1637,102 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
@@ -1747,7 +1747,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>25</v>
@@ -1767,25 +1767,25 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>91</v>
@@ -1797,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>98</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>91</v>
@@ -1817,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>103</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>91</v>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>105</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>91</v>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>93</v>
@@ -1861,7 +1861,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>91</v>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>95</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>99</v>
@@ -1891,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>101</v>
@@ -1899,16 +1899,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D51" t="s">
         <v>132</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>95</v>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>10</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>10</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>10</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>10</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>10</v>
@@ -2016,7 +2016,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>10</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>10</v>
@@ -2056,7 +2056,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>10</v>
@@ -2076,7 +2076,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>10</v>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>10</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>10</v>
@@ -2132,7 +2132,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>10</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>10</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>10</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>5</v>
@@ -2198,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>108</v>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>5</v>
@@ -2218,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>122</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>5</v>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
@@ -2258,7 +2258,7 @@
         <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>106</v>
@@ -2266,7 +2266,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>5</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>5</v>
@@ -2298,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>88</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>5</v>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>96</v>
@@ -2324,10 +2324,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
@@ -2342,25 +2342,25 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E74" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>27</v>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>27</v>
@@ -2400,28 +2400,28 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
@@ -2436,7 +2436,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>133</v>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>56</v>
@@ -2474,13 +2474,13 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D81" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
[Word] (Settings) Add sample for SettingCollection
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25804"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B578329-F858-4666-B6D6-7FB8F58644EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF809C40-D846-4146-B33F-8EA51BE6E3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="176">
   <si>
     <t>Class</t>
   </si>
@@ -530,6 +530,24 @@
   </si>
   <si>
     <t>word-document-manage-fields</t>
+  </si>
+  <si>
+    <t>word-document-manage-settings</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>getSettings</t>
+  </si>
+  <si>
+    <t>createSetting</t>
+  </si>
+  <si>
+    <t>deleteAllSettings</t>
+  </si>
+  <si>
+    <t>SettingCollection</t>
   </si>
 </sst>
 </file>
@@ -640,8 +658,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F81" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F81" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F85" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F85" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -951,11 +969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,21 +1636,21 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>126</v>
+        <v>170</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1640,17 +1658,17 @@
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E37" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1661,14 +1679,14 @@
         <v>137</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1679,14 +1697,14 @@
         <v>137</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1694,14 +1712,12 @@
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
         <v>169</v>
       </c>
@@ -1717,14 +1733,16 @@
         <v>144</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1732,17 +1750,17 @@
         <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1750,19 +1768,17 @@
         <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1770,17 +1786,19 @@
         <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
-        <v>132</v>
+        <v>25</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1788,19 +1806,17 @@
         <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,7 +1827,7 @@
         <v>91</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D46" s="2">
         <v>1</v>
@@ -1820,7 +1836,7 @@
         <v>151</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1831,14 +1847,16 @@
         <v>91</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
       <c r="E47" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1849,14 +1867,14 @@
         <v>91</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1867,14 +1885,14 @@
         <v>91</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1882,56 +1900,54 @@
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>168</v>
       </c>
-      <c r="B51" t="s">
-        <v>161</v>
-      </c>
-      <c r="D51" t="s">
-        <v>132</v>
+      <c r="B51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>79</v>
+      <c r="B52" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" t="s">
+        <v>132</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1942,16 +1958,16 @@
         <v>10</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>75</v>
+      <c r="E53" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1962,16 +1978,16 @@
         <v>10</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1982,16 +1998,16 @@
         <v>10</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D55" s="2">
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2011,7 +2027,7 @@
         <v>71</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2022,16 +2038,16 @@
         <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D57" s="2">
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2042,16 +2058,16 @@
         <v>10</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2061,17 +2077,17 @@
       <c r="B59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="1">
+      <c r="C59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="2">
         <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2081,17 +2097,17 @@
       <c r="B60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="1">
         <v>1</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2102,14 +2118,16 @@
         <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
       <c r="E61" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2120,14 +2138,14 @@
         <v>10</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2138,14 +2156,14 @@
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2156,14 +2174,14 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2174,14 +2192,14 @@
         <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D65" s="2"/>
-      <c r="E65" s="1" t="s">
-        <v>79</v>
+      <c r="E65" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2189,19 +2207,17 @@
         <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D66" s="1">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>150</v>
+        <v>10</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2212,16 +2228,16 @@
         <v>5</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D67" s="1">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2232,16 +2248,16 @@
         <v>5</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>79</v>
+      <c r="E68" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2252,16 +2268,16 @@
         <v>5</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2272,16 +2288,16 @@
         <v>5</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="D70" s="1">
         <v>1</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>82</v>
+      <c r="E70" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2292,16 +2308,16 @@
         <v>5</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="D71" s="1">
         <v>1</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>151</v>
+      <c r="E71" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2312,14 +2328,16 @@
         <v>5</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D72" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1</v>
+      </c>
       <c r="E72" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2327,17 +2345,17 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2345,17 +2363,17 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2365,17 +2383,15 @@
       <c r="B75" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D75" s="1">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>78</v>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2385,17 +2401,17 @@
       <c r="B76" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D76" s="2">
+      <c r="C76" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2403,17 +2419,19 @@
         <v>168</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>148</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2421,17 +2439,17 @@
         <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,53 +2457,127 @@
         <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E79" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="1" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D80" s="1">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="s">
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>168</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
         <v>153</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D85" t="s">
         <v>149</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E85" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (Settings) Add sample for SettingCollection (#709)
* [Word] (Settings) Add sample for SettingCollection

* Apply suggestions from code review

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>

* Updates based on feedback

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25806"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B578329-F858-4666-B6D6-7FB8F58644EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC7B33-2245-4C78-9DA5-6ACDF0A65F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="176">
   <si>
     <t>Class</t>
   </si>
@@ -530,6 +530,24 @@
   </si>
   <si>
     <t>word-document-manage-fields</t>
+  </si>
+  <si>
+    <t>word-document-manage-settings</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>deleteAllSettings</t>
+  </si>
+  <si>
+    <t>SettingCollection</t>
+  </si>
+  <si>
+    <t>addEditSetting</t>
+  </si>
+  <si>
+    <t>getAllSettings</t>
   </si>
 </sst>
 </file>
@@ -640,8 +658,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F81" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F81" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F85" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F85" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -951,11 +969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,21 +1636,21 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>126</v>
+        <v>170</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1640,17 +1658,17 @@
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E37" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1661,14 +1679,14 @@
         <v>137</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1679,14 +1697,14 @@
         <v>137</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1694,14 +1712,12 @@
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
         <v>169</v>
       </c>
@@ -1717,14 +1733,16 @@
         <v>144</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1732,17 +1750,17 @@
         <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1750,19 +1768,17 @@
         <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1770,17 +1786,19 @@
         <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
-        <v>132</v>
+        <v>25</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1788,19 +1806,17 @@
         <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,7 +1827,7 @@
         <v>91</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D46" s="2">
         <v>1</v>
@@ -1820,7 +1836,7 @@
         <v>151</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1831,14 +1847,16 @@
         <v>91</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
       <c r="E47" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1849,14 +1867,14 @@
         <v>91</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1867,14 +1885,14 @@
         <v>91</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1882,56 +1900,54 @@
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>168</v>
       </c>
-      <c r="B51" t="s">
-        <v>161</v>
-      </c>
-      <c r="D51" t="s">
-        <v>132</v>
+      <c r="B51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>79</v>
+      <c r="B52" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" t="s">
+        <v>132</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1942,16 +1958,16 @@
         <v>10</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>75</v>
+      <c r="E53" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1962,16 +1978,16 @@
         <v>10</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1982,16 +1998,16 @@
         <v>10</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D55" s="2">
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2011,7 +2027,7 @@
         <v>71</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2022,16 +2038,16 @@
         <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D57" s="2">
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2042,16 +2058,16 @@
         <v>10</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2061,17 +2077,17 @@
       <c r="B59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="1">
+      <c r="C59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="2">
         <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2081,17 +2097,17 @@
       <c r="B60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="1">
         <v>1</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2102,14 +2118,16 @@
         <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
       <c r="E61" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2120,14 +2138,14 @@
         <v>10</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2138,14 +2156,14 @@
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2156,14 +2174,14 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2174,14 +2192,14 @@
         <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D65" s="2"/>
-      <c r="E65" s="1" t="s">
-        <v>79</v>
+      <c r="E65" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2189,19 +2207,17 @@
         <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D66" s="1">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>150</v>
+        <v>10</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2212,16 +2228,16 @@
         <v>5</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D67" s="1">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2232,16 +2248,16 @@
         <v>5</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>79</v>
+      <c r="E68" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2252,16 +2268,16 @@
         <v>5</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2272,16 +2288,16 @@
         <v>5</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="D70" s="1">
         <v>1</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>82</v>
+      <c r="E70" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2292,16 +2308,16 @@
         <v>5</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="D71" s="1">
         <v>1</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>151</v>
+      <c r="E71" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2312,14 +2328,16 @@
         <v>5</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D72" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1</v>
+      </c>
       <c r="E72" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2327,17 +2345,17 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2345,17 +2363,17 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2365,17 +2383,15 @@
       <c r="B75" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D75" s="1">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>78</v>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2385,17 +2401,17 @@
       <c r="B76" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D76" s="2">
+      <c r="C76" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2403,17 +2419,19 @@
         <v>168</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>148</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2421,17 +2439,17 @@
         <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,53 +2457,127 @@
         <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E79" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="1" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D80" s="1">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="s">
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>168</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
         <v>153</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D85" t="s">
         <v>149</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E85" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Add manage-custom-xml-part snippet
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25806"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25808"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC7B33-2245-4C78-9DA5-6ACDF0A65F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4EF970-2F68-4630-9578-C3EDB41DEDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="187">
   <si>
     <t>Class</t>
   </si>
@@ -548,6 +548,39 @@
   </si>
   <si>
     <t>getAllSettings</t>
+  </si>
+  <si>
+    <t>CustomXmlPart</t>
+  </si>
+  <si>
+    <t>getXml</t>
+  </si>
+  <si>
+    <t>getItem</t>
+  </si>
+  <si>
+    <t>word-document-manage-custom-xml-part</t>
+  </si>
+  <si>
+    <t>addCustomXmlPart</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>CustomXmlParts</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>insertAttribute</t>
+  </si>
+  <si>
+    <t>insertElement</t>
+  </si>
+  <si>
+    <t>deleteCustomXmlPart</t>
   </si>
 </sst>
 </file>
@@ -596,13 +629,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +695,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F85" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F85" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F93" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F93" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -969,11 +1006,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1600,149 +1637,161 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>168</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>120</v>
+      <c r="A34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>121</v>
+      <c r="E34" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>168</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>64</v>
+      <c r="A35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>175</v>
+      <c r="B36" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>168</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>126</v>
+      <c r="A37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>141</v>
+      <c r="A38" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>168</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>139</v>
+      <c r="A39" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>168</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>141</v>
+      <c r="A40" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>141</v>
+      <c r="A41" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1750,17 +1799,17 @@
         <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="2" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1768,37 +1817,35 @@
         <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="2">
-        <v>1</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1806,17 +1853,17 @@
         <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>160</v>
+        <v>124</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1824,19 +1871,17 @@
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1844,19 +1889,17 @@
         <v>168</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1864,17 +1907,17 @@
         <v>168</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1882,17 +1925,19 @@
         <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
       <c r="E49" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1900,17 +1945,17 @@
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1918,36 +1963,37 @@
         <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>168</v>
       </c>
-      <c r="B52" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52" t="s">
-        <v>132</v>
+      <c r="B52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1955,19 +2001,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="2">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>79</v>
+        <v>159</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>12</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1975,19 +2019,19 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1995,19 +2039,19 @@
         <v>168</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="D55" s="2">
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2015,19 +2059,17 @@
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2035,19 +2077,17 @@
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,19 +2095,17 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2075,39 +2113,36 @@
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="D59" s="2">
         <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>168</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
+      <c r="B60" t="s">
+        <v>161</v>
+      </c>
+      <c r="D60" t="s">
+        <v>132</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2118,16 +2153,16 @@
         <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>83</v>
+      <c r="E61" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2138,14 +2173,16 @@
         <v>10</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
       <c r="E62" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2156,14 +2193,16 @@
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
       <c r="E63" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2174,14 +2213,16 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
       <c r="E64" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2192,14 +2233,16 @@
         <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
       <c r="E65" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2210,14 +2253,16 @@
         <v>10</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2225,19 +2270,19 @@
         <v>168</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D67" s="1">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2245,19 +2290,19 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2265,19 +2310,19 @@
         <v>168</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2285,19 +2330,17 @@
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D70" s="1">
-        <v>1</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>150</v>
+        <v>10</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2305,19 +2348,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D71" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2325,19 +2366,17 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D72" s="1">
-        <v>1</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2345,17 +2384,17 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2363,17 +2402,17 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="2"/>
       <c r="E74" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2381,17 +2420,19 @@
         <v>168</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,19 +2440,19 @@
         <v>168</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2419,19 +2460,19 @@
         <v>168</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,17 +2480,19 @@
         <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2457,73 +2500,75 @@
         <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>170</v>
+      <c r="E82" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>174</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2531,17 +2576,17 @@
         <v>168</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>76</v>
+        <v>27</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2549,35 +2594,185 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>168</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>168</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>168</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>168</v>
+      </c>
+      <c r="B93" t="s">
         <v>153</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D93" t="s">
         <v>149</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Additional mappings for a couple of enums
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25806"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25812"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC7B33-2245-4C78-9DA5-6ACDF0A65F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A51A6CD-04D3-4BD2-8105-1DBA6C164B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="184">
   <si>
     <t>Class</t>
   </si>
@@ -548,6 +548,30 @@
   </si>
   <si>
     <t>getAllSettings</t>
+  </si>
+  <si>
+    <t>DocumentPropertyType</t>
+  </si>
+  <si>
+    <t>CustomProperty</t>
+  </si>
+  <si>
+    <t>imageFormat</t>
+  </si>
+  <si>
+    <t>ImageFormat</t>
+  </si>
+  <si>
+    <t>inlinePictures</t>
+  </si>
+  <si>
+    <t>insertImage</t>
+  </si>
+  <si>
+    <t>getLast</t>
+  </si>
+  <si>
+    <t>InlinePictureCollection</t>
   </si>
 </sst>
 </file>
@@ -596,13 +620,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +686,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F85" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F85" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F93" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F93" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -969,11 +997,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,20 +1206,21 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" t="s">
-        <v>86</v>
+      <c r="C11" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1199,16 +1228,16 @@
         <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>158</v>
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1216,16 +1245,16 @@
         <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
         <v>132</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>152</v>
+        <v>75</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1233,7 +1262,7 @@
         <v>168</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" t="s">
         <v>132</v>
@@ -1242,7 +1271,7 @@
         <v>152</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1250,19 +1279,16 @@
         <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>150</v>
-      </c>
-      <c r="F15" t="s">
-        <v>114</v>
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1273,7 +1299,7 @@
         <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1282,7 +1308,7 @@
         <v>150</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1293,7 +1319,7 @@
         <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1302,7 +1328,7 @@
         <v>150</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1313,13 +1339,16 @@
         <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>150</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1330,13 +1359,13 @@
         <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
         <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1344,19 +1373,16 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
         <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1367,13 +1393,16 @@
         <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1381,56 +1410,56 @@
         <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>168</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>46</v>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>168</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
-        <v>123</v>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1443,66 +1472,63 @@
       <c r="C25" t="s">
         <v>123</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F25" t="s">
-        <v>126</v>
+      <c r="F25" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>168</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>42</v>
+      <c r="C26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>168</v>
       </c>
-      <c r="B27" t="s">
-        <v>162</v>
-      </c>
-      <c r="D27" t="s">
-        <v>132</v>
-      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F27" t="s">
-        <v>46</v>
+      <c r="F27" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
+      <c r="B28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" t="s">
+        <v>132</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1510,17 +1536,19 @@
         <v>168</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1531,7 +1559,7 @@
         <v>128</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
@@ -1546,39 +1574,35 @@
         <v>168</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1</v>
+      <c r="A32" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1588,15 +1612,17 @@
       <c r="B33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="1"/>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
       <c r="E33" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1604,17 +1630,19 @@
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
       <c r="E34" s="2" t="s">
-        <v>152</v>
+        <v>73</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1622,35 +1650,35 @@
         <v>168</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D36" s="2"/>
+      <c r="C36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1658,53 +1686,53 @@
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>126</v>
+        <v>74</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>168</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D39" s="2"/>
+      <c r="A39" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E39" s="2" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1712,17 +1740,17 @@
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E40" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1730,14 +1758,12 @@
         <v>168</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
         <v>169</v>
       </c>
@@ -1750,17 +1776,17 @@
         <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1768,17 +1794,17 @@
         <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1786,19 +1812,19 @@
         <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="D44" s="2">
         <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1806,17 +1832,17 @@
         <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1824,57 +1850,53 @@
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>168</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1</v>
+      <c r="A47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="2"/>
+      <c r="A48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E48" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1882,72 +1904,73 @@
         <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
       <c r="E49" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>168</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>94</v>
+      <c r="A50" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1</v>
+      <c r="A51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>168</v>
       </c>
-      <c r="B52" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="B52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1955,19 +1978,19 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>79</v>
+      <c r="E53" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1975,19 +1998,19 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1995,19 +2018,17 @@
         <v>168</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2015,19 +2036,17 @@
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2035,19 +2054,17 @@
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,39 +2072,36 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>168</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1</v>
+      <c r="B59" t="s">
+        <v>161</v>
+      </c>
+      <c r="D59" t="s">
+        <v>132</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2097,17 +2111,17 @@
       <c r="B60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>83</v>
+      <c r="C60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2117,17 +2131,17 @@
       <c r="B61" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>6</v>
+      <c r="C61" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2138,14 +2152,16 @@
         <v>10</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
       <c r="E62" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2156,14 +2172,16 @@
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
       <c r="E63" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2174,14 +2192,16 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
       <c r="E64" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2192,14 +2212,16 @@
         <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
       <c r="E65" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2210,14 +2232,16 @@
         <v>10</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2225,19 +2249,19 @@
         <v>168</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D67" s="1">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2245,19 +2269,19 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2265,19 +2289,19 @@
         <v>168</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2285,19 +2309,17 @@
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D70" s="1">
-        <v>1</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>150</v>
+        <v>10</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2305,19 +2327,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D71" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2325,19 +2345,17 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D72" s="1">
-        <v>1</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2345,17 +2363,17 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2363,17 +2381,17 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="2"/>
       <c r="E74" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2381,17 +2399,19 @@
         <v>168</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,19 +2419,19 @@
         <v>168</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2419,19 +2439,19 @@
         <v>168</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,17 +2459,19 @@
         <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2457,73 +2479,75 @@
         <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>170</v>
+      <c r="E82" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>174</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2531,17 +2555,17 @@
         <v>168</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>76</v>
+        <v>27</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2549,35 +2573,185 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>168</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>168</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>168</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>168</v>
+      </c>
+      <c r="B93" t="s">
         <v>153</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D93" t="s">
         <v>149</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Additional mappings for a couple of enums (#715)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25806"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25812"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC7B33-2245-4C78-9DA5-6ACDF0A65F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A51A6CD-04D3-4BD2-8105-1DBA6C164B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="184">
   <si>
     <t>Class</t>
   </si>
@@ -548,6 +548,30 @@
   </si>
   <si>
     <t>getAllSettings</t>
+  </si>
+  <si>
+    <t>DocumentPropertyType</t>
+  </si>
+  <si>
+    <t>CustomProperty</t>
+  </si>
+  <si>
+    <t>imageFormat</t>
+  </si>
+  <si>
+    <t>ImageFormat</t>
+  </si>
+  <si>
+    <t>inlinePictures</t>
+  </si>
+  <si>
+    <t>insertImage</t>
+  </si>
+  <si>
+    <t>getLast</t>
+  </si>
+  <si>
+    <t>InlinePictureCollection</t>
   </si>
 </sst>
 </file>
@@ -596,13 +620,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +686,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F85" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F85" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F93" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F93" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -969,11 +997,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,20 +1206,21 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" t="s">
-        <v>86</v>
+      <c r="C11" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1199,16 +1228,16 @@
         <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>158</v>
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1216,16 +1245,16 @@
         <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
         <v>132</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>152</v>
+        <v>75</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1233,7 +1262,7 @@
         <v>168</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" t="s">
         <v>132</v>
@@ -1242,7 +1271,7 @@
         <v>152</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1250,19 +1279,16 @@
         <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>150</v>
-      </c>
-      <c r="F15" t="s">
-        <v>114</v>
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1273,7 +1299,7 @@
         <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1282,7 +1308,7 @@
         <v>150</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1293,7 +1319,7 @@
         <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1302,7 +1328,7 @@
         <v>150</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1313,13 +1339,16 @@
         <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>150</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1330,13 +1359,13 @@
         <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
         <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1344,19 +1373,16 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
         <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1367,13 +1393,16 @@
         <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1381,56 +1410,56 @@
         <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>168</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>46</v>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>168</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
-        <v>123</v>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1443,66 +1472,63 @@
       <c r="C25" t="s">
         <v>123</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F25" t="s">
-        <v>126</v>
+      <c r="F25" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>168</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>42</v>
+      <c r="C26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>168</v>
       </c>
-      <c r="B27" t="s">
-        <v>162</v>
-      </c>
-      <c r="D27" t="s">
-        <v>132</v>
-      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F27" t="s">
-        <v>46</v>
+      <c r="F27" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
+      <c r="B28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" t="s">
+        <v>132</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1510,17 +1536,19 @@
         <v>168</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1531,7 +1559,7 @@
         <v>128</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
@@ -1546,39 +1574,35 @@
         <v>168</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1</v>
+      <c r="A32" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1588,15 +1612,17 @@
       <c r="B33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="1"/>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
       <c r="E33" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1604,17 +1630,19 @@
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
       <c r="E34" s="2" t="s">
-        <v>152</v>
+        <v>73</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1622,35 +1650,35 @@
         <v>168</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D36" s="2"/>
+      <c r="C36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1658,53 +1686,53 @@
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>126</v>
+        <v>74</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>168</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D39" s="2"/>
+      <c r="A39" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E39" s="2" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1712,17 +1740,17 @@
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E40" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1730,14 +1758,12 @@
         <v>168</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
         <v>169</v>
       </c>
@@ -1750,17 +1776,17 @@
         <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1768,17 +1794,17 @@
         <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1786,19 +1812,19 @@
         <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="D44" s="2">
         <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1806,17 +1832,17 @@
         <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1824,57 +1850,53 @@
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>168</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1</v>
+      <c r="A47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="2"/>
+      <c r="A48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E48" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1882,72 +1904,73 @@
         <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
       <c r="E49" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>168</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>94</v>
+      <c r="A50" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1</v>
+      <c r="A51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>168</v>
       </c>
-      <c r="B52" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="B52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1955,19 +1978,19 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>79</v>
+      <c r="E53" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1975,19 +1998,19 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1995,19 +2018,17 @@
         <v>168</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2015,19 +2036,17 @@
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2035,19 +2054,17 @@
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,39 +2072,36 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>168</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1</v>
+      <c r="B59" t="s">
+        <v>161</v>
+      </c>
+      <c r="D59" t="s">
+        <v>132</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2097,17 +2111,17 @@
       <c r="B60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>83</v>
+      <c r="C60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2117,17 +2131,17 @@
       <c r="B61" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>6</v>
+      <c r="C61" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2138,14 +2152,16 @@
         <v>10</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
       <c r="E62" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2156,14 +2172,16 @@
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
       <c r="E63" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2174,14 +2192,16 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
       <c r="E64" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2192,14 +2212,16 @@
         <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
       <c r="E65" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2210,14 +2232,16 @@
         <v>10</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2225,19 +2249,19 @@
         <v>168</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D67" s="1">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2245,19 +2269,19 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2265,19 +2289,19 @@
         <v>168</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2285,19 +2309,17 @@
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D70" s="1">
-        <v>1</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>150</v>
+        <v>10</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2305,19 +2327,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D71" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2325,19 +2345,17 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D72" s="1">
-        <v>1</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2345,17 +2363,17 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2363,17 +2381,17 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="2"/>
       <c r="E74" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2381,17 +2399,19 @@
         <v>168</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,19 +2419,19 @@
         <v>168</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2419,19 +2439,19 @@
         <v>168</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,17 +2459,19 @@
         <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2457,73 +2479,75 @@
         <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>170</v>
+      <c r="E82" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>174</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2531,17 +2555,17 @@
         <v>168</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>76</v>
+        <v>27</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2549,35 +2573,185 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>168</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>168</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>168</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>168</v>
+      </c>
+      <c r="B93" t="s">
         <v>153</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D93" t="s">
         <v>149</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Add manage-custom-xml-part snippet (#713)
* [Word] Add manage-custom-xml-part snippet

* Apply suggestions from code review

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>

* Updates based on feedback

* [Word] Additional mappings for a couple of enums (#715)

* Reset metadata file

* Re-add metadata

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25812"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A51A6CD-04D3-4BD2-8105-1DBA6C164B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1EF916-3E9F-45DD-9441-C86AE95B2D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="195">
   <si>
     <t>Class</t>
   </si>
@@ -572,6 +572,39 @@
   </si>
   <si>
     <t>InlinePictureCollection</t>
+  </si>
+  <si>
+    <t>CustomXmlPart</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>word-document-manage-custom-xml-part</t>
+  </si>
+  <si>
+    <t>addCustomXmlPart</t>
+  </si>
+  <si>
+    <t>deleteCustomXmlPart</t>
+  </si>
+  <si>
+    <t>getXml</t>
+  </si>
+  <si>
+    <t>insertAttribute</t>
+  </si>
+  <si>
+    <t>insertElement</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>getItem</t>
+  </si>
+  <si>
+    <t>CustomXmlPartCollection</t>
   </si>
 </sst>
 </file>
@@ -620,17 +653,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,8 +715,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F93" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F93" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F101" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F101" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -997,11 +1026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,14 +1241,14 @@
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1591,10 +1620,10 @@
       <c r="A32" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
         <v>149</v>
       </c>
@@ -1664,39 +1693,43 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>65</v>
+        <v>184</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
       <c r="E36" s="2" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>121</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
       <c r="E37" s="2" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1704,107 +1737,117 @@
         <v>168</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D38" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
       <c r="E38" s="2" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="2" t="s">
-        <v>132</v>
+      <c r="B39" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>63</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
-        <v>132</v>
+        <v>184</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>126</v>
+        <v>186</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D41" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="2" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>141</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D42" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
       <c r="E42" s="2" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D43" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
       <c r="E43" s="2" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1812,19 +1855,17 @@
         <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D44" s="2">
-        <v>1</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="2" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1832,71 +1873,71 @@
         <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>169</v>
+        <v>74</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>78</v>
+        <v>170</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C47" s="5"/>
+      <c r="B47" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="2" t="s">
-        <v>149</v>
+      <c r="A48" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>181</v>
+        <v>124</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1904,55 +1945,53 @@
         <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>178</v>
+      <c r="A50" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="2" t="s">
-        <v>149</v>
-      </c>
+      <c r="A51" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1960,17 +1999,19 @@
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1978,19 +2019,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1998,55 +2037,53 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E55" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>105</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D56" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E56" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>93</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2054,54 +2091,55 @@
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
       <c r="E57" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D58" s="2">
-        <v>1</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>168</v>
-      </c>
-      <c r="B59" t="s">
-        <v>161</v>
-      </c>
-      <c r="D59" t="s">
-        <v>132</v>
+      <c r="A59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2109,19 +2147,17 @@
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D60" s="2">
-        <v>1</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>79</v>
+        <v>159</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>12</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2129,19 +2165,19 @@
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>182</v>
+        <v>91</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>181</v>
+        <v>151</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2149,19 +2185,19 @@
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="D62" s="2">
         <v>1</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2169,19 +2205,17 @@
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2189,19 +2223,17 @@
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2209,19 +2241,17 @@
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2229,39 +2259,36 @@
         <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="D66" s="2">
         <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>168</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D67" s="2">
-        <v>1</v>
+      <c r="B67" t="s">
+        <v>161</v>
+      </c>
+      <c r="D67" t="s">
+        <v>132</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2271,17 +2298,17 @@
       <c r="B68" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="1">
-        <v>1</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>83</v>
+      <c r="C68" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2292,16 +2319,16 @@
         <v>10</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>6</v>
+        <v>182</v>
       </c>
       <c r="D69" s="2">
         <v>1</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>66</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2312,14 +2339,16 @@
         <v>10</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D70" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
       <c r="E70" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2330,14 +2359,16 @@
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D71" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
       <c r="E71" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2348,14 +2379,16 @@
         <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D72" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
       <c r="E72" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2366,14 +2399,16 @@
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D73" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
       <c r="E73" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2384,14 +2419,16 @@
         <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,19 +2436,19 @@
         <v>168</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D75" s="1">
+        <v>10</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D75" s="2">
         <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2419,19 +2456,19 @@
         <v>168</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,19 +2476,19 @@
         <v>168</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="1">
-        <v>1</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,19 +2496,17 @@
         <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D78" s="1">
-        <v>1</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>150</v>
+        <v>10</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2479,19 +2514,17 @@
         <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D79" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2499,19 +2532,17 @@
         <v>168</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D80" s="1">
-        <v>1</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2519,17 +2550,17 @@
         <v>168</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2537,17 +2568,17 @@
         <v>168</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="2"/>
       <c r="E82" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2555,17 +2586,19 @@
         <v>168</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2573,19 +2606,19 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2593,19 +2626,19 @@
         <v>168</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D85" s="2">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" s="1">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2613,17 +2646,19 @@
         <v>168</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2631,73 +2666,75 @@
         <v>168</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D87" s="1">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D88" s="1">
+        <v>1</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D89" s="2">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2" t="s">
-        <v>170</v>
+      <c r="E90" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2705,17 +2742,17 @@
         <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>76</v>
+        <v>27</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2723,35 +2760,185 @@
         <v>168</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D92" s="1">
         <v>1</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>168</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>168</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>168</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>168</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D100" s="1">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>168</v>
+      </c>
+      <c r="B101" t="s">
         <v>153</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D101" t="s">
         <v>149</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="E101" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Update existing sample to show BodyType
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25815"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1EF916-3E9F-45DD-9441-C86AE95B2D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ABEC1F-7157-4090-9DA1-02419862132D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="196">
   <si>
     <t>Class</t>
   </si>
@@ -605,6 +605,9 @@
   </si>
   <si>
     <t>CustomXmlPartCollection</t>
+  </si>
+  <si>
+    <t>BodyType</t>
   </si>
 </sst>
 </file>
@@ -715,8 +718,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F101" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F101" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F103" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F103" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1026,11 +1029,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,37 +1273,37 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>158</v>
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>168</v>
-      </c>
-      <c r="B14" t="s">
-        <v>130</v>
+      <c r="A14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="D14" t="s">
         <v>132</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>121</v>
+      <c r="E14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1308,16 +1311,16 @@
         <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
         <v>132</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>152</v>
+        <v>75</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1325,19 +1328,16 @@
         <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>150</v>
-      </c>
-      <c r="F16" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1345,19 +1345,16 @@
         <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1368,7 +1365,7 @@
         <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1377,7 +1374,7 @@
         <v>150</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1388,13 +1385,16 @@
         <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1405,13 +1405,16 @@
         <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1419,19 +1422,16 @@
         <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E21" t="s">
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1439,16 +1439,16 @@
         <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1456,39 +1456,36 @@
         <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>46</v>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1499,48 +1496,53 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>124</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>125</v>
+      <c r="F25" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>168</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C26" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" t="s">
-        <v>126</v>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>168</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="2"/>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
       <c r="E27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>42</v>
+        <v>124</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1548,16 +1550,16 @@
         <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" t="s">
+        <v>124</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1565,37 +1567,34 @@
         <v>168</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="1"/>
+      <c r="B30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" t="s">
+        <v>132</v>
+      </c>
       <c r="E30" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>126</v>
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1603,35 +1602,37 @@
         <v>168</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="2" t="s">
+      <c r="C32" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1639,39 +1640,35 @@
         <v>168</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="2">
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1681,55 +1678,55 @@
       <c r="B35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="1"/>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
       <c r="E35" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1740,7 +1737,7 @@
         <v>184</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>190</v>
+        <v>97</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -1749,7 +1746,7 @@
         <v>186</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1760,7 +1757,7 @@
         <v>184</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
@@ -1769,7 +1766,7 @@
         <v>186</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1780,7 +1777,7 @@
         <v>184</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -1789,7 +1786,7 @@
         <v>186</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,14 +1797,16 @@
         <v>184</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D41" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1815,10 +1814,10 @@
         <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1827,7 +1826,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1835,127 +1834,129 @@
         <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2" t="s">
+      <c r="D48" s="2"/>
+      <c r="E48" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B47" s="1" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2" t="s">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>168</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1963,17 +1964,17 @@
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D50" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E50" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>139</v>
+        <v>124</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1984,7 +1985,7 @@
         <v>137</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
@@ -1999,19 +2000,17 @@
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2019,17 +2018,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2037,67 +2036,67 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>181</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
+        <v>179</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>70</v>
@@ -2113,27 +2112,29 @@
       <c r="B58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E58" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>149</v>
+        <v>25</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>70</v>
@@ -2143,41 +2144,39 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1</v>
+        <v>183</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2185,19 +2184,17 @@
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2208,14 +2205,16 @@
         <v>91</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2226,14 +2225,16 @@
         <v>91</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
       <c r="E64" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2244,14 +2245,14 @@
         <v>91</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2259,31 +2260,30 @@
         <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D66" s="2"/>
       <c r="E66" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>168</v>
       </c>
-      <c r="B67" t="s">
-        <v>161</v>
-      </c>
-      <c r="D67" t="s">
-        <v>132</v>
-      </c>
+      <c r="B67" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
         <v>151</v>
       </c>
@@ -2296,39 +2296,36 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>79</v>
+      <c r="E68" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>168</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
+      <c r="B69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D69" t="s">
+        <v>132</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2339,16 +2336,16 @@
         <v>10</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D70" s="2">
         <v>1</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>75</v>
+      <c r="E70" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2359,16 +2356,16 @@
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>13</v>
+        <v>182</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2379,16 +2376,16 @@
         <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,16 +2396,16 @@
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2419,16 +2416,16 @@
         <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D74" s="2">
         <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,16 +2436,16 @@
         <v>10</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D75" s="2">
         <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2458,17 +2455,17 @@
       <c r="B76" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="1">
+      <c r="C76" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D76" s="2">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2479,16 +2476,16 @@
         <v>10</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2498,15 +2495,17 @@
       <c r="B78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" s="2"/>
+      <c r="C78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
       <c r="E78" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2517,14 +2516,16 @@
         <v>10</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D79" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
       <c r="E79" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2535,14 +2536,14 @@
         <v>10</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2553,14 +2554,14 @@
         <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2571,14 +2572,14 @@
         <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D82" s="2"/>
-      <c r="E82" s="1" t="s">
-        <v>79</v>
+      <c r="E82" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2586,19 +2587,17 @@
         <v>168</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D83" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="2"/>
       <c r="E83" s="2" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,19 +2605,17 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D84" s="1">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>152</v>
+        <v>10</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2629,16 +2626,16 @@
         <v>5</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="D85" s="1">
         <v>1</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>79</v>
+      <c r="E85" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2649,16 +2646,16 @@
         <v>5</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D86" s="1">
         <v>1</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>150</v>
+      <c r="E86" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2669,16 +2666,16 @@
         <v>5</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D87" s="1">
         <v>1</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>82</v>
+      <c r="E87" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2689,16 +2686,16 @@
         <v>5</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="D88" s="1">
         <v>1</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2709,14 +2706,16 @@
         <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1" t="s">
-        <v>151</v>
+        <v>36</v>
+      </c>
+      <c r="D89" s="1">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2724,17 +2723,19 @@
         <v>168</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1" t="s">
-        <v>132</v>
+        <v>5</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2742,17 +2743,17 @@
         <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1" t="s">
-        <v>149</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2760,19 +2761,17 @@
         <v>168</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D92" s="1">
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>78</v>
+        <v>163</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2782,17 +2781,15 @@
       <c r="B93" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D93" s="2">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>78</v>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2800,17 +2797,19 @@
         <v>168</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2818,55 +2817,55 @@
         <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" s="2">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>174</v>
+        <v>49</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2876,69 +2875,107 @@
       <c r="B98" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E98" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F98" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" s="2">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>168</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D100" s="1">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>168</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>168</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D102" s="1">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>168</v>
+      </c>
+      <c r="B103" t="s">
         <v>153</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D103" t="s">
         <v>149</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E103" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Update existing sample to show BodyType (#719)
* [Word] Update existing sample to show BodyType

* Apply suggestions from code review

Co-authored-by: Alison McKay <almckay@microsoft.com>

* Update based on feedback

Co-authored-by: Alison McKay <almckay@microsoft.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25815"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1EF916-3E9F-45DD-9441-C86AE95B2D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ABEC1F-7157-4090-9DA1-02419862132D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="196">
   <si>
     <t>Class</t>
   </si>
@@ -605,6 +605,9 @@
   </si>
   <si>
     <t>CustomXmlPartCollection</t>
+  </si>
+  <si>
+    <t>BodyType</t>
   </si>
 </sst>
 </file>
@@ -715,8 +718,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F101" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F101" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F103" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F103" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1026,11 +1029,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,37 +1273,37 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>158</v>
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>168</v>
-      </c>
-      <c r="B14" t="s">
-        <v>130</v>
+      <c r="A14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="D14" t="s">
         <v>132</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>121</v>
+      <c r="E14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1308,16 +1311,16 @@
         <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
         <v>132</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>152</v>
+        <v>75</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1325,19 +1328,16 @@
         <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>150</v>
-      </c>
-      <c r="F16" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1345,19 +1345,16 @@
         <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1368,7 +1365,7 @@
         <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1377,7 +1374,7 @@
         <v>150</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1388,13 +1385,16 @@
         <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1405,13 +1405,16 @@
         <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1419,19 +1422,16 @@
         <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E21" t="s">
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1439,16 +1439,16 @@
         <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1456,39 +1456,36 @@
         <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>46</v>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1499,48 +1496,53 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>124</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>125</v>
+      <c r="F25" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>168</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C26" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" t="s">
-        <v>126</v>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>168</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="2"/>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
       <c r="E27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>42</v>
+        <v>124</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1548,16 +1550,16 @@
         <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" t="s">
+        <v>124</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1565,37 +1567,34 @@
         <v>168</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="1"/>
+      <c r="B30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" t="s">
+        <v>132</v>
+      </c>
       <c r="E30" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>126</v>
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1603,35 +1602,37 @@
         <v>168</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="2" t="s">
+      <c r="C32" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1639,39 +1640,35 @@
         <v>168</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="2">
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1681,55 +1678,55 @@
       <c r="B35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="1"/>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
       <c r="E35" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1740,7 +1737,7 @@
         <v>184</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>190</v>
+        <v>97</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -1749,7 +1746,7 @@
         <v>186</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1760,7 +1757,7 @@
         <v>184</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
@@ -1769,7 +1766,7 @@
         <v>186</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1780,7 +1777,7 @@
         <v>184</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -1789,7 +1786,7 @@
         <v>186</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,14 +1797,16 @@
         <v>184</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D41" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1815,10 +1814,10 @@
         <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1827,7 +1826,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1835,127 +1834,129 @@
         <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2" t="s">
+      <c r="D48" s="2"/>
+      <c r="E48" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B47" s="1" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2" t="s">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>168</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1963,17 +1964,17 @@
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D50" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E50" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>139</v>
+        <v>124</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1984,7 +1985,7 @@
         <v>137</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
@@ -1999,19 +2000,17 @@
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2019,17 +2018,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2037,67 +2036,67 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>181</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
+        <v>179</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>70</v>
@@ -2113,27 +2112,29 @@
       <c r="B58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E58" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>149</v>
+        <v>25</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>70</v>
@@ -2143,41 +2144,39 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1</v>
+        <v>183</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2185,19 +2184,17 @@
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2208,14 +2205,16 @@
         <v>91</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2226,14 +2225,16 @@
         <v>91</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
       <c r="E64" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2244,14 +2245,14 @@
         <v>91</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2259,31 +2260,30 @@
         <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D66" s="2"/>
       <c r="E66" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>168</v>
       </c>
-      <c r="B67" t="s">
-        <v>161</v>
-      </c>
-      <c r="D67" t="s">
-        <v>132</v>
-      </c>
+      <c r="B67" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
         <v>151</v>
       </c>
@@ -2296,39 +2296,36 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>79</v>
+      <c r="E68" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>168</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
+      <c r="B69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D69" t="s">
+        <v>132</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2339,16 +2336,16 @@
         <v>10</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D70" s="2">
         <v>1</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>75</v>
+      <c r="E70" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2359,16 +2356,16 @@
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>13</v>
+        <v>182</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2379,16 +2376,16 @@
         <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,16 +2396,16 @@
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2419,16 +2416,16 @@
         <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D74" s="2">
         <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,16 +2436,16 @@
         <v>10</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D75" s="2">
         <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2458,17 +2455,17 @@
       <c r="B76" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="1">
+      <c r="C76" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D76" s="2">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2479,16 +2476,16 @@
         <v>10</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2498,15 +2495,17 @@
       <c r="B78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" s="2"/>
+      <c r="C78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
       <c r="E78" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2517,14 +2516,16 @@
         <v>10</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D79" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
       <c r="E79" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2535,14 +2536,14 @@
         <v>10</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2553,14 +2554,14 @@
         <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2571,14 +2572,14 @@
         <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D82" s="2"/>
-      <c r="E82" s="1" t="s">
-        <v>79</v>
+      <c r="E82" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2586,19 +2587,17 @@
         <v>168</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D83" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="2"/>
       <c r="E83" s="2" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,19 +2605,17 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D84" s="1">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>152</v>
+        <v>10</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2629,16 +2626,16 @@
         <v>5</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="D85" s="1">
         <v>1</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>79</v>
+      <c r="E85" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2649,16 +2646,16 @@
         <v>5</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D86" s="1">
         <v>1</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>150</v>
+      <c r="E86" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2669,16 +2666,16 @@
         <v>5</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D87" s="1">
         <v>1</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>82</v>
+      <c r="E87" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2689,16 +2686,16 @@
         <v>5</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="D88" s="1">
         <v>1</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2709,14 +2706,16 @@
         <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1" t="s">
-        <v>151</v>
+        <v>36</v>
+      </c>
+      <c r="D89" s="1">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2724,17 +2723,19 @@
         <v>168</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1" t="s">
-        <v>132</v>
+        <v>5</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2742,17 +2743,17 @@
         <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1" t="s">
-        <v>149</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2760,19 +2761,17 @@
         <v>168</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D92" s="1">
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>78</v>
+        <v>163</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2782,17 +2781,15 @@
       <c r="B93" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D93" s="2">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>78</v>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2800,17 +2797,19 @@
         <v>168</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2818,55 +2817,55 @@
         <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" s="2">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>174</v>
+        <v>49</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2876,69 +2875,107 @@
       <c r="B98" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E98" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F98" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" s="2">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>168</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D100" s="1">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>168</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>168</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D102" s="1">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>168</v>
+      </c>
+      <c r="B103" t="s">
         <v>153</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D103" t="s">
         <v>149</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E103" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Fix mapping to ParagraphCollection.getLast
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ABEC1F-7157-4090-9DA1-02419862132D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3403DEC-340F-4B4C-BE7F-F1805E94596C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="197">
   <si>
     <t>Class</t>
   </si>
@@ -608,6 +608,9 @@
   </si>
   <si>
     <t>BodyType</t>
+  </si>
+  <si>
+    <t>ParagraphCollection</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1035,8 @@
   <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2356,16 +2359,16 @@
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>182</v>
+        <v>29</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>181</v>
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2376,16 +2379,16 @@
         <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2396,16 +2399,16 @@
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2425,7 +2428,7 @@
         <v>71</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2436,16 +2439,16 @@
         <v>10</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D75" s="2">
         <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2456,16 +2459,16 @@
         <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2475,17 +2478,17 @@
       <c r="B77" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D77" s="2">
+      <c r="C77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="1">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2495,17 +2498,17 @@
       <c r="B78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2516,16 +2519,14 @@
         <v>10</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2536,14 +2537,14 @@
         <v>10</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2554,14 +2555,14 @@
         <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2572,14 +2573,14 @@
         <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2590,14 +2591,14 @@
         <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D83" s="2"/>
-      <c r="E83" s="2" t="s">
-        <v>80</v>
+      <c r="E83" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2605,17 +2606,19 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>10</v>
+        <v>196</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="1" t="s">
-        <v>79</v>
+        <v>182</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Word] Fix mapping to ParagraphCollection.getLast (#724)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ABEC1F-7157-4090-9DA1-02419862132D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3403DEC-340F-4B4C-BE7F-F1805E94596C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="197">
   <si>
     <t>Class</t>
   </si>
@@ -608,6 +608,9 @@
   </si>
   <si>
     <t>BodyType</t>
+  </si>
+  <si>
+    <t>ParagraphCollection</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1035,8 @@
   <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2356,16 +2359,16 @@
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>182</v>
+        <v>29</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>181</v>
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2376,16 +2379,16 @@
         <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2396,16 +2399,16 @@
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2425,7 +2428,7 @@
         <v>71</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2436,16 +2439,16 @@
         <v>10</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D75" s="2">
         <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2456,16 +2459,16 @@
         <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2475,17 +2478,17 @@
       <c r="B77" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D77" s="2">
+      <c r="C77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="1">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2495,17 +2498,17 @@
       <c r="B78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2516,16 +2519,14 @@
         <v>10</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2536,14 +2537,14 @@
         <v>10</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2554,14 +2555,14 @@
         <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2572,14 +2573,14 @@
         <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2590,14 +2591,14 @@
         <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D83" s="2"/>
-      <c r="E83" s="2" t="s">
-        <v>80</v>
+      <c r="E83" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2605,17 +2606,19 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>10</v>
+        <v>196</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="1" t="s">
-        <v>79</v>
+        <v>182</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Word] Add snippet that shows how to get various table formatting (#720)
* [Word] Add snippets that shows how to get various table borders

* Update to provide an example of using a string literal

* Merge with other table formatting snippets

* Updates based on feedback

* Metadata mappings
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25819"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3403DEC-340F-4B4C-BE7F-F1805E94596C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DA643A-9CAB-40AA-B57A-333E3F630C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="221">
   <si>
     <t>Class</t>
   </si>
@@ -611,6 +611,78 @@
   </si>
   <si>
     <t>ParagraphCollection</t>
+  </si>
+  <si>
+    <t>tables</t>
+  </si>
+  <si>
+    <t>TableCollection</t>
+  </si>
+  <si>
+    <t>word-tables-manage-formatting</t>
+  </si>
+  <si>
+    <t>getTableAlignment</t>
+  </si>
+  <si>
+    <t>horizontalAlignment</t>
+  </si>
+  <si>
+    <t>verticalAlignment</t>
+  </si>
+  <si>
+    <t>BorderLocation</t>
+  </si>
+  <si>
+    <t>getTableBorder</t>
+  </si>
+  <si>
+    <t>getBorder</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>CellPaddingLocation</t>
+  </si>
+  <si>
+    <t>getTableCellPadding</t>
+  </si>
+  <si>
+    <t>getCellPadding</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>getTableRowAlignment</t>
+  </si>
+  <si>
+    <t>TableRowCollection</t>
+  </si>
+  <si>
+    <t>getTableRowBorder</t>
+  </si>
+  <si>
+    <t>TableRow</t>
+  </si>
+  <si>
+    <t>TableBorder</t>
+  </si>
+  <si>
+    <t>getTableRowCellPadding</t>
+  </si>
+  <si>
+    <t>getTableCellAlignment</t>
+  </si>
+  <si>
+    <t>getTableCellBorder</t>
+  </si>
+  <si>
+    <t>getTableCellCellPadding</t>
   </si>
 </sst>
 </file>
@@ -721,8 +793,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F103" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F103" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F126" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F126" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1032,18 +1104,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
@@ -1279,28 +1351,28 @@
       <c r="A13" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>197</v>
       </c>
       <c r="E13" t="s">
-        <v>151</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D14" t="s">
-        <v>132</v>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
       </c>
       <c r="E14" t="s">
         <v>151</v>
@@ -1310,37 +1382,37 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B15" t="s">
-        <v>157</v>
+      <c r="A15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="D15" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>158</v>
+      <c r="E15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" t="s">
-        <v>130</v>
+      <c r="A16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="D16" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>121</v>
+      <c r="E16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1348,36 +1420,33 @@
         <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>152</v>
+        <v>75</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>150</v>
-      </c>
-      <c r="F18" t="s">
-        <v>114</v>
+      <c r="A18" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1385,19 +1454,16 @@
         <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>150</v>
-      </c>
-      <c r="F19" t="s">
-        <v>116</v>
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1405,19 +1471,16 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" t="s">
-        <v>119</v>
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1428,13 +1491,16 @@
         <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>97</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1445,13 +1511,16 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22" t="s">
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1459,10 +1528,10 @@
         <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1471,7 +1540,7 @@
         <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1479,16 +1548,16 @@
         <v>168</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="E24" t="s">
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1496,39 +1565,36 @@
         <v>168</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="E25" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>168</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>46</v>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1536,16 +1602,16 @@
         <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>125</v>
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1556,13 +1622,16 @@
         <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>97</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>124</v>
       </c>
       <c r="F28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1572,15 +1641,17 @@
       <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="2"/>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
       <c r="E29" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1588,36 +1659,33 @@
         <v>168</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
-      </c>
-      <c r="D30" t="s">
-        <v>132</v>
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" t="s">
-        <v>46</v>
+        <v>124</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>37</v>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1625,53 +1693,54 @@
         <v>168</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D32" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>126</v>
+        <v>43</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>168</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D33" s="1"/>
+      <c r="B33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" t="s">
+        <v>132</v>
+      </c>
       <c r="E33" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>126</v>
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>149</v>
+        <v>39</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1679,19 +1748,17 @@
         <v>168</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1699,32 +1766,30 @@
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>62</v>
+        <v>124</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="1"/>
+        <v>177</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="E37" s="2" t="s">
         <v>73</v>
       </c>
@@ -1733,63 +1798,61 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>168</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="1">
+        <v>61</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2">
         <v>1</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>186</v>
+        <v>73</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>168</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D39" s="1">
+        <v>61</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2">
         <v>1</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>186</v>
+        <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>187</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>184</v>
+        <v>61</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="2" t="s">
-        <v>186</v>
+        <v>73</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>190</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,7 +1863,7 @@
         <v>184</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>191</v>
+        <v>97</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1809,7 +1872,7 @@
         <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1820,7 +1883,7 @@
         <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1829,7 +1892,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1840,14 +1903,16 @@
         <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D43" s="1"/>
+        <v>190</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
       <c r="E43" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1855,10 +1920,10 @@
         <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>4</v>
+        <v>191</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1867,7 +1932,7 @@
         <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1875,10 +1940,10 @@
         <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -1891,39 +1956,41 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>65</v>
+        <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
       <c r="E47" s="2" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1931,35 +1998,37 @@
         <v>168</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="C49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1967,53 +2036,53 @@
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>126</v>
+        <v>74</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D52" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E52" s="2" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2021,17 +2090,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D53" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E53" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2039,14 +2108,12 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
         <v>169</v>
       </c>
@@ -2059,17 +2126,17 @@
         <v>168</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2077,53 +2144,55 @@
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2131,19 +2200,17 @@
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2151,12 +2218,12 @@
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D60" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E60" s="2" t="s">
         <v>70</v>
       </c>
@@ -2169,7 +2236,7 @@
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
@@ -2179,7 +2246,7 @@
         <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,57 +2254,55 @@
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2" t="s">
-        <v>132</v>
+        <v>25</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D63" s="2">
-        <v>1</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D64" s="2">
-        <v>1</v>
+        <v>183</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2245,17 +2310,17 @@
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D65" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E65" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2266,14 +2331,16 @@
         <v>91</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D66" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
       <c r="E66" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2284,14 +2351,16 @@
         <v>91</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D67" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
       <c r="E67" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2299,36 +2368,35 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D68" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>168</v>
       </c>
-      <c r="B69" t="s">
-        <v>161</v>
-      </c>
-      <c r="D69" t="s">
-        <v>132</v>
-      </c>
+      <c r="B69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="2"/>
       <c r="E69" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2336,19 +2404,17 @@
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D70" s="2">
-        <v>1</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2356,39 +2422,36 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>168</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="2">
-        <v>1</v>
+      <c r="B72" t="s">
+        <v>161</v>
+      </c>
+      <c r="D72" t="s">
+        <v>132</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,16 +2462,16 @@
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>71</v>
+      <c r="E73" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2419,16 +2482,16 @@
         <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D74" s="2">
         <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2439,16 +2502,16 @@
         <v>10</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D75" s="2">
         <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,16 +2522,16 @@
         <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2478,17 +2541,17 @@
       <c r="B77" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="1">
+      <c r="C77" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2499,16 +2562,16 @@
         <v>10</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="D78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2519,14 +2582,16 @@
         <v>10</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D79" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
       <c r="E79" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2536,15 +2601,17 @@
       <c r="B80" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D80" s="2"/>
+      <c r="C80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
       <c r="E80" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2555,14 +2622,16 @@
         <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D81" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
       <c r="E81" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2573,14 +2642,14 @@
         <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2591,14 +2660,14 @@
         <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D83" s="2"/>
-      <c r="E83" s="1" t="s">
-        <v>79</v>
+      <c r="E83" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,19 +2675,17 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D84" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D84" s="2"/>
       <c r="E84" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>181</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2626,19 +2693,17 @@
         <v>168</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D85" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="2"/>
       <c r="E85" s="2" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2646,19 +2711,17 @@
         <v>168</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D86" s="1">
-        <v>1</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>152</v>
+        <v>10</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2666,19 +2729,19 @@
         <v>168</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D87" s="1">
-        <v>1</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>79</v>
+        <v>196</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2689,16 +2752,16 @@
         <v>5</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D88" s="1">
         <v>1</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" s="2" t="s">
         <v>150</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2709,16 +2772,16 @@
         <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="D89" s="1">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2729,16 +2792,16 @@
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="D90" s="1">
         <v>1</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2749,14 +2812,16 @@
         <v>5</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D91" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1</v>
+      </c>
       <c r="E91" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2764,17 +2829,19 @@
         <v>168</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>79</v>
+        <v>5</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2782,17 +2849,19 @@
         <v>168</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1" t="s">
-        <v>149</v>
+        <v>5</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D93" s="1">
+        <v>1</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>146</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2800,19 +2869,17 @@
         <v>168</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D94" s="1">
-        <v>1</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
+      </c>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2820,19 +2887,17 @@
         <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D95" s="2">
-        <v>1</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>78</v>
+        <v>163</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2840,17 +2905,17 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="E96" s="1" t="s">
         <v>145</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2858,128 +2923,555 @@
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" s="1">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>168</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>168</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2" t="s">
+      <c r="C100" s="2"/>
+      <c r="D100" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="E100" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B98" s="1" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D99" s="2">
-        <v>1</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>168</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" s="2">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>168</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E104" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>168</v>
-      </c>
-      <c r="B102" s="1" t="s">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C105" s="2"/>
+      <c r="D105" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D106" s="2">
+        <v>1</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>168</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D102" s="1">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="s">
+      <c r="D107" s="1">
+        <v>1</v>
+      </c>
+      <c r="E107" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F107" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>168</v>
-      </c>
-      <c r="B103" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D108" s="1">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D109" s="1"/>
+      <c r="E109" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D112" s="1"/>
+      <c r="E112" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C113" t="s">
+        <v>206</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C114" t="s">
+        <v>94</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C115" t="s">
+        <v>207</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>168</v>
+      </c>
+      <c r="B116" t="s">
         <v>153</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D116" t="s">
         <v>149</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="E116" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F116" s="2" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C117" t="s">
+        <v>205</v>
+      </c>
+      <c r="D117">
+        <v>2</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C118" t="s">
+        <v>210</v>
+      </c>
+      <c r="D118">
+        <v>2</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>168</v>
+      </c>
+      <c r="B119" t="s">
+        <v>153</v>
+      </c>
+      <c r="C119" t="s">
+        <v>201</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>168</v>
+      </c>
+      <c r="B120" t="s">
+        <v>153</v>
+      </c>
+      <c r="C120" t="s">
+        <v>202</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D121" t="s">
+        <v>149</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C122" t="s">
+        <v>100</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C123" t="s">
+        <v>205</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C124" t="s">
+        <v>210</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D125" t="s">
+        <v>149</v>
+      </c>
+      <c r="E125" t="s">
+        <v>199</v>
+      </c>
+      <c r="F125" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C126" t="s">
+        <v>100</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126" t="s">
+        <v>199</v>
+      </c>
+      <c r="F126" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Word] (list) Tweak, additional mappings
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25819"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25820"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DA643A-9CAB-40AA-B57A-333E3F630C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD27B0-06E1-4BEB-AF0E-64C4C2A50267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="224">
   <si>
     <t>Class</t>
   </si>
@@ -683,6 +683,15 @@
   </si>
   <si>
     <t>getTableCellCellPadding</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>ListItem</t>
+  </si>
+  <si>
+    <t>level</t>
   </si>
 </sst>
 </file>
@@ -731,13 +740,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,8 +806,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F126" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F126" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F130" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F130" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1104,11 +1117,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2324,61 +2337,59 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>168</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>98</v>
+      <c r="A66" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>168</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>102</v>
+      <c r="A67" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>103</v>
+      <c r="E67" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>168</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>104</v>
+      <c r="A68" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="D68" s="2"/>
-      <c r="E68" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>105</v>
+      <c r="E68" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2389,14 +2400,16 @@
         <v>91</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D69" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
       <c r="E69" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2407,14 +2420,16 @@
         <v>91</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
       <c r="E70" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2422,36 +2437,35 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D71" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>168</v>
       </c>
-      <c r="B72" t="s">
-        <v>161</v>
-      </c>
-      <c r="D72" t="s">
-        <v>132</v>
-      </c>
+      <c r="B72" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" s="2"/>
       <c r="E72" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,19 +2473,17 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D73" s="2">
-        <v>1</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2479,39 +2491,36 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="D74" s="2">
         <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>168</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
+      <c r="B75" t="s">
+        <v>161</v>
+      </c>
+      <c r="D75" t="s">
+        <v>132</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2522,16 +2531,16 @@
         <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>71</v>
+      <c r="E76" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2542,16 +2551,16 @@
         <v>10</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2562,16 +2571,16 @@
         <v>10</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,16 +2591,16 @@
         <v>10</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D79" s="2">
         <v>1</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2601,17 +2610,17 @@
       <c r="B80" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="1">
+      <c r="C80" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D80" s="2">
         <v>1</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2622,16 +2631,16 @@
         <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="D81" s="2">
         <v>1</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2642,14 +2651,16 @@
         <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
       <c r="E82" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2659,15 +2670,17 @@
       <c r="B83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="2"/>
+      <c r="C83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
       <c r="E83" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2678,14 +2691,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
       <c r="E84" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2696,14 +2711,14 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2714,14 +2729,14 @@
         <v>10</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D86" s="2"/>
-      <c r="E86" s="1" t="s">
-        <v>79</v>
+      <c r="E86" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2729,19 +2744,17 @@
         <v>168</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D87" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D87" s="2"/>
       <c r="E87" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>181</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2749,19 +2762,17 @@
         <v>168</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D88" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" s="2"/>
       <c r="E88" s="2" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2769,19 +2780,17 @@
         <v>168</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D89" s="1">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>152</v>
+        <v>10</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2789,19 +2798,19 @@
         <v>168</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" s="1">
-        <v>1</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>79</v>
+        <v>196</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2809,19 +2818,17 @@
         <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D91" s="1">
-        <v>1</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>150</v>
+        <v>196</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2832,16 +2839,16 @@
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="D92" s="1">
         <v>1</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2852,16 +2859,16 @@
         <v>5</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D93" s="1">
         <v>1</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>151</v>
+      <c r="E93" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2872,14 +2879,16 @@
         <v>5</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D94" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1</v>
+      </c>
       <c r="E94" s="1" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2887,17 +2896,19 @@
         <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1" t="s">
-        <v>132</v>
+        <v>5</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2905,17 +2916,19 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D96" s="1">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>146</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2923,19 +2936,19 @@
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D97" s="1">
         <v>1</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>78</v>
+      <c r="E97" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2943,19 +2956,17 @@
         <v>168</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D98" s="2">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2963,17 +2974,17 @@
         <v>168</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>145</v>
+        <v>163</v>
+      </c>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>148</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2981,73 +2992,75 @@
         <v>168</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>71</v>
+        <v>27</v>
+      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>168</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>168</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D102" s="2">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>168</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D102" s="2">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D103" s="2"/>
       <c r="E103" s="2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3055,17 +3068,17 @@
         <v>168</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>134</v>
+        <v>49</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3073,17 +3086,17 @@
         <v>168</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3091,59 +3104,55 @@
         <v>168</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>205</v>
+        <v>4</v>
       </c>
       <c r="D106" s="2">
         <v>1</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D107" s="1">
-        <v>1</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D107" s="2"/>
       <c r="E107" s="2" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+      <c r="A108" t="s">
         <v>168</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D108" s="1">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>199</v>
+        <v>76</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>209</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3153,15 +3162,15 @@
       <c r="B109" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D109" s="1"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E109" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>200</v>
+        <v>53</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3171,33 +3180,37 @@
       <c r="B110" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D110" s="1"/>
+      <c r="C110" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D110" s="2">
+        <v>1</v>
+      </c>
       <c r="E110" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D111" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="D111" s="1">
+        <v>1</v>
+      </c>
       <c r="E111" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3208,14 +3221,16 @@
         <v>56</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D112" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1</v>
+      </c>
       <c r="E112" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3223,16 +3238,17 @@
         <v>168</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C113" t="s">
-        <v>206</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D113" s="1"/>
       <c r="E113" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,16 +3256,17 @@
         <v>168</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C114" t="s">
-        <v>94</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D114" s="1"/>
       <c r="E114" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3257,33 +3274,35 @@
         <v>168</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C115" t="s">
-        <v>207</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D115" s="1"/>
       <c r="E115" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>168</v>
-      </c>
-      <c r="B116" t="s">
-        <v>153</v>
-      </c>
-      <c r="D116" t="s">
-        <v>149</v>
-      </c>
+      <c r="A116" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D116" s="1"/>
       <c r="E116" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3291,19 +3310,16 @@
         <v>168</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="C117" t="s">
-        <v>205</v>
-      </c>
-      <c r="D117">
-        <v>2</v>
+        <v>206</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3311,36 +3327,33 @@
         <v>168</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="C118" t="s">
-        <v>210</v>
-      </c>
-      <c r="D118">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>168</v>
-      </c>
-      <c r="B119" t="s">
-        <v>153</v>
+      <c r="A119" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C119" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3350,14 +3363,14 @@
       <c r="B120" t="s">
         <v>153</v>
       </c>
-      <c r="C120" t="s">
-        <v>202</v>
+      <c r="D120" t="s">
+        <v>149</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>218</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3365,16 +3378,19 @@
         <v>168</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D121" t="s">
-        <v>149</v>
+        <v>153</v>
+      </c>
+      <c r="C121" t="s">
+        <v>205</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3382,59 +3398,53 @@
         <v>168</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="C122" t="s">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>215</v>
+      <c r="A123" t="s">
+        <v>168</v>
+      </c>
+      <c r="B123" t="s">
+        <v>153</v>
       </c>
       <c r="C123" t="s">
-        <v>205</v>
-      </c>
-      <c r="D123">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>215</v>
+      <c r="A124" t="s">
+        <v>168</v>
+      </c>
+      <c r="B124" t="s">
+        <v>153</v>
       </c>
       <c r="C124" t="s">
-        <v>210</v>
-      </c>
-      <c r="D124">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3442,16 +3452,16 @@
         <v>168</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D125" t="s">
         <v>149</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F125" t="s">
-        <v>212</v>
+      <c r="F125" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3459,7 +3469,7 @@
         <v>168</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C126" t="s">
         <v>100</v>
@@ -3467,10 +3477,87 @@
       <c r="D126">
         <v>1</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C127" t="s">
+        <v>205</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F126" t="s">
+      <c r="F127" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C128" t="s">
+        <v>210</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D129" t="s">
+        <v>149</v>
+      </c>
+      <c r="E129" t="s">
+        <v>199</v>
+      </c>
+      <c r="F129" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C130" t="s">
+        <v>100</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130" t="s">
+        <v>199</v>
+      </c>
+      <c r="F130" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (list) Tweak, additional mappings (#731)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25819"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25820"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DA643A-9CAB-40AA-B57A-333E3F630C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD27B0-06E1-4BEB-AF0E-64C4C2A50267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="224">
   <si>
     <t>Class</t>
   </si>
@@ -683,6 +683,15 @@
   </si>
   <si>
     <t>getTableCellCellPadding</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>ListItem</t>
+  </si>
+  <si>
+    <t>level</t>
   </si>
 </sst>
 </file>
@@ -731,13 +740,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,8 +806,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F126" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F126" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F130" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F130" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1104,11 +1117,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2324,61 +2337,59 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>168</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>98</v>
+      <c r="A66" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>168</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>102</v>
+      <c r="A67" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>103</v>
+      <c r="E67" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>168</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>104</v>
+      <c r="A68" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="D68" s="2"/>
-      <c r="E68" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>105</v>
+      <c r="E68" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2389,14 +2400,16 @@
         <v>91</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D69" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
       <c r="E69" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2407,14 +2420,16 @@
         <v>91</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
       <c r="E70" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2422,36 +2437,35 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D71" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>168</v>
       </c>
-      <c r="B72" t="s">
-        <v>161</v>
-      </c>
-      <c r="D72" t="s">
-        <v>132</v>
-      </c>
+      <c r="B72" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" s="2"/>
       <c r="E72" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,19 +2473,17 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D73" s="2">
-        <v>1</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2479,39 +2491,36 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="D74" s="2">
         <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>168</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
+      <c r="B75" t="s">
+        <v>161</v>
+      </c>
+      <c r="D75" t="s">
+        <v>132</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2522,16 +2531,16 @@
         <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>71</v>
+      <c r="E76" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2542,16 +2551,16 @@
         <v>10</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2562,16 +2571,16 @@
         <v>10</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,16 +2591,16 @@
         <v>10</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D79" s="2">
         <v>1</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2601,17 +2610,17 @@
       <c r="B80" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="1">
+      <c r="C80" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D80" s="2">
         <v>1</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2622,16 +2631,16 @@
         <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="D81" s="2">
         <v>1</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2642,14 +2651,16 @@
         <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
       <c r="E82" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2659,15 +2670,17 @@
       <c r="B83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="2"/>
+      <c r="C83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
       <c r="E83" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2678,14 +2691,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
       <c r="E84" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2696,14 +2711,14 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2714,14 +2729,14 @@
         <v>10</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D86" s="2"/>
-      <c r="E86" s="1" t="s">
-        <v>79</v>
+      <c r="E86" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2729,19 +2744,17 @@
         <v>168</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D87" s="2">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D87" s="2"/>
       <c r="E87" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>181</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2749,19 +2762,17 @@
         <v>168</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D88" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" s="2"/>
       <c r="E88" s="2" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2769,19 +2780,17 @@
         <v>168</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D89" s="1">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>152</v>
+        <v>10</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2789,19 +2798,19 @@
         <v>168</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" s="1">
-        <v>1</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>79</v>
+        <v>196</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2809,19 +2818,17 @@
         <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D91" s="1">
-        <v>1</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>150</v>
+        <v>196</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2832,16 +2839,16 @@
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="D92" s="1">
         <v>1</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2852,16 +2859,16 @@
         <v>5</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D93" s="1">
         <v>1</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>151</v>
+      <c r="E93" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2872,14 +2879,16 @@
         <v>5</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D94" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1</v>
+      </c>
       <c r="E94" s="1" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2887,17 +2896,19 @@
         <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1" t="s">
-        <v>132</v>
+        <v>5</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2905,17 +2916,19 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D96" s="1">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>146</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2923,19 +2936,19 @@
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D97" s="1">
         <v>1</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>78</v>
+      <c r="E97" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2943,19 +2956,17 @@
         <v>168</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D98" s="2">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2963,17 +2974,17 @@
         <v>168</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>145</v>
+        <v>163</v>
+      </c>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>148</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2981,73 +2992,75 @@
         <v>168</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>71</v>
+        <v>27</v>
+      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>168</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>168</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D102" s="2">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>168</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D102" s="2">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D103" s="2"/>
       <c r="E103" s="2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3055,17 +3068,17 @@
         <v>168</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>134</v>
+        <v>49</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3073,17 +3086,17 @@
         <v>168</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3091,59 +3104,55 @@
         <v>168</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>205</v>
+        <v>4</v>
       </c>
       <c r="D106" s="2">
         <v>1</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D107" s="1">
-        <v>1</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D107" s="2"/>
       <c r="E107" s="2" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+      <c r="A108" t="s">
         <v>168</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D108" s="1">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>199</v>
+        <v>76</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>209</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3153,15 +3162,15 @@
       <c r="B109" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D109" s="1"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E109" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>200</v>
+        <v>53</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3171,33 +3180,37 @@
       <c r="B110" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D110" s="1"/>
+      <c r="C110" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D110" s="2">
+        <v>1</v>
+      </c>
       <c r="E110" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D111" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="D111" s="1">
+        <v>1</v>
+      </c>
       <c r="E111" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3208,14 +3221,16 @@
         <v>56</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D112" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1</v>
+      </c>
       <c r="E112" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3223,16 +3238,17 @@
         <v>168</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C113" t="s">
-        <v>206</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D113" s="1"/>
       <c r="E113" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,16 +3256,17 @@
         <v>168</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C114" t="s">
-        <v>94</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D114" s="1"/>
       <c r="E114" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3257,33 +3274,35 @@
         <v>168</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C115" t="s">
-        <v>207</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D115" s="1"/>
       <c r="E115" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>168</v>
-      </c>
-      <c r="B116" t="s">
-        <v>153</v>
-      </c>
-      <c r="D116" t="s">
-        <v>149</v>
-      </c>
+      <c r="A116" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D116" s="1"/>
       <c r="E116" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3291,19 +3310,16 @@
         <v>168</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="C117" t="s">
-        <v>205</v>
-      </c>
-      <c r="D117">
-        <v>2</v>
+        <v>206</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3311,36 +3327,33 @@
         <v>168</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="C118" t="s">
-        <v>210</v>
-      </c>
-      <c r="D118">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>168</v>
-      </c>
-      <c r="B119" t="s">
-        <v>153</v>
+      <c r="A119" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C119" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3350,14 +3363,14 @@
       <c r="B120" t="s">
         <v>153</v>
       </c>
-      <c r="C120" t="s">
-        <v>202</v>
+      <c r="D120" t="s">
+        <v>149</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>218</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3365,16 +3378,19 @@
         <v>168</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D121" t="s">
-        <v>149</v>
+        <v>153</v>
+      </c>
+      <c r="C121" t="s">
+        <v>205</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3382,59 +3398,53 @@
         <v>168</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="C122" t="s">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>215</v>
+      <c r="A123" t="s">
+        <v>168</v>
+      </c>
+      <c r="B123" t="s">
+        <v>153</v>
       </c>
       <c r="C123" t="s">
-        <v>205</v>
-      </c>
-      <c r="D123">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>215</v>
+      <c r="A124" t="s">
+        <v>168</v>
+      </c>
+      <c r="B124" t="s">
+        <v>153</v>
       </c>
       <c r="C124" t="s">
-        <v>210</v>
-      </c>
-      <c r="D124">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3442,16 +3452,16 @@
         <v>168</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D125" t="s">
         <v>149</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F125" t="s">
-        <v>212</v>
+      <c r="F125" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3459,7 +3469,7 @@
         <v>168</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C126" t="s">
         <v>100</v>
@@ -3467,10 +3477,87 @@
       <c r="D126">
         <v>1</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C127" t="s">
+        <v>205</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F126" t="s">
+      <c r="F127" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C128" t="s">
+        <v>210</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D129" t="s">
+        <v>149</v>
+      </c>
+      <c r="E129" t="s">
+        <v>199</v>
+      </c>
+      <c r="F129" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C130" t="s">
+        <v>100</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130" t="s">
+        <v>199</v>
+      </c>
+      <c r="F130" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (list) Add snippet on organizing a list (#733)
* [Word] (list) Add snippet on formatting

* Updates based on feedback

* Apply suggestions from code review

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>

* Updates based on feedback

* Rename snippet

* rename function

* Add mappings

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25820"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25822"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD27B0-06E1-4BEB-AF0E-64C4C2A50267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E62E70-5EEC-4C49-AFDF-63710A621AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="232">
   <si>
     <t>Class</t>
   </si>
@@ -692,6 +692,30 @@
   </si>
   <si>
     <t>level</t>
+  </si>
+  <si>
+    <t>setLevelNumbering</t>
+  </si>
+  <si>
+    <t>word-lists-organize-list</t>
+  </si>
+  <si>
+    <t>insertOrganizeList</t>
+  </si>
+  <si>
+    <t>setLevelBullet</t>
+  </si>
+  <si>
+    <t>ListBullet</t>
+  </si>
+  <si>
+    <t>levelTypes</t>
+  </si>
+  <si>
+    <t>ListNumbering</t>
+  </si>
+  <si>
+    <t>ListLevelType</t>
   </si>
 </sst>
 </file>
@@ -806,8 +830,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F130" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F130" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F136" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F136" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1117,11 +1141,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <selection pane="bottomLeft" activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2340,17 +2364,17 @@
       <c r="A66" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C66" s="5"/>
+      <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2358,19 +2382,19 @@
       <c r="A67" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2379,148 +2403,149 @@
         <v>168</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C71" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>168</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>168</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D70" s="2">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>168</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>151</v>
+        <v>57</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>168</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>93</v>
+      <c r="A72" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>168</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>95</v>
+      <c r="A73" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>168</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D74" s="2">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>101</v>
+      <c r="A74" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>168</v>
       </c>
-      <c r="B75" t="s">
-        <v>161</v>
-      </c>
-      <c r="D75" t="s">
-        <v>132</v>
+      <c r="B75" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2528,19 +2553,19 @@
         <v>168</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
       </c>
-      <c r="E76" s="1" t="s">
-        <v>79</v>
+      <c r="E76" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2548,19 +2573,17 @@
         <v>168</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D77" s="2"/>
       <c r="E77" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2568,19 +2591,17 @@
         <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D78" s="2"/>
       <c r="E78" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2588,19 +2609,17 @@
         <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D79" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2608,39 +2627,36 @@
         <v>168</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="D80" s="2">
         <v>1</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>168</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+      <c r="D81" t="s">
+        <v>132</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2651,16 +2667,16 @@
         <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="D82" s="2">
         <v>1</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>57</v>
+      <c r="E82" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2670,17 +2686,17 @@
       <c r="B83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="1">
+      <c r="C83" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" s="2">
         <v>1</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2691,16 +2707,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2711,14 +2727,16 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D85" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
       <c r="E85" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2729,14 +2747,16 @@
         <v>10</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D86" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1</v>
+      </c>
       <c r="E86" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2747,14 +2767,16 @@
         <v>10</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D87" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
       <c r="E87" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2765,14 +2787,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D88" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1</v>
+      </c>
       <c r="E88" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2782,15 +2806,17 @@
       <c r="B89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" s="2"/>
-      <c r="E89" s="1" t="s">
-        <v>79</v>
+      <c r="C89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="1">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2798,19 +2824,19 @@
         <v>168</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>182</v>
+        <v>6</v>
       </c>
       <c r="D90" s="2">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>181</v>
+        <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2818,17 +2844,17 @@
         <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>67</v>
+        <v>10</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2836,19 +2862,17 @@
         <v>168</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D92" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" s="2"/>
       <c r="E92" s="2" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2856,19 +2880,17 @@
         <v>168</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D93" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>122</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2876,19 +2898,17 @@
         <v>168</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D94" s="1">
-        <v>1</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2896,19 +2916,17 @@
         <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D95" s="1">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="2"/>
       <c r="E95" s="1" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2916,19 +2934,19 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D96" s="1">
+        <v>196</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>35</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2936,19 +2954,17 @@
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D97" s="1">
-        <v>1</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>151</v>
+        <v>196</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2959,14 +2975,16 @@
         <v>5</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1" t="s">
-        <v>151</v>
+        <v>107</v>
+      </c>
+      <c r="D98" s="1">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2974,17 +2992,19 @@
         <v>168</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>79</v>
+        <v>5</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D99" s="1">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2992,17 +3012,19 @@
         <v>168</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1" t="s">
-        <v>149</v>
+        <v>5</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" s="1">
+        <v>1</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3010,19 +3032,19 @@
         <v>168</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>78</v>
+      <c r="E101" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3030,19 +3052,19 @@
         <v>168</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D102" s="2">
+        <v>5</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D102" s="1">
         <v>1</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3050,17 +3072,19 @@
         <v>168</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D103" s="1">
+        <v>1</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3068,73 +3092,73 @@
         <v>168</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2" t="s">
+      <c r="E105" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D106" s="2">
-        <v>1</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>170</v>
+      <c r="E106" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
+      <c r="A107" t="s">
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D107" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D107" s="1">
+        <v>1</v>
+      </c>
       <c r="E107" s="2" t="s">
-        <v>170</v>
+        <v>78</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3142,75 +3166,73 @@
         <v>168</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D108" s="2">
+        <v>1</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>134</v>
+        <v>40</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+      <c r="A109" t="s">
         <v>168</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+      <c r="A110" t="s">
         <v>168</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D110" s="2">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>199</v>
+        <v>71</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>204</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D111" s="1">
-        <v>1</v>
+        <v>173</v>
+      </c>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>54</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3218,19 +3240,19 @@
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D112" s="1">
+        <v>173</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" s="2">
         <v>1</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>209</v>
+        <v>174</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3238,35 +3260,35 @@
         <v>168</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D113" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D113" s="2"/>
       <c r="E113" s="2" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+      <c r="A114" t="s">
         <v>168</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D114" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E114" s="2" t="s">
-        <v>199</v>
+        <v>76</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>200</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3276,15 +3298,15 @@
       <c r="B115" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D115" s="1"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E115" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>212</v>
+        <v>53</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3294,32 +3316,37 @@
       <c r="B116" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D116" s="1"/>
+      <c r="C116" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D116" s="2">
+        <v>1</v>
+      </c>
       <c r="E116" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+      <c r="A117" t="s">
         <v>168</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C117" t="s">
-        <v>206</v>
+        <v>56</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>204</v>
+        <v>54</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3327,16 +3354,19 @@
         <v>168</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C118" t="s">
-        <v>94</v>
+        <v>56</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D118" s="1">
+        <v>1</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3344,33 +3374,35 @@
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C119" t="s">
-        <v>207</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D119" s="1"/>
       <c r="E119" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>168</v>
-      </c>
-      <c r="B120" t="s">
-        <v>153</v>
-      </c>
-      <c r="D120" t="s">
-        <v>149</v>
-      </c>
+      <c r="A120" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D120" s="1"/>
       <c r="E120" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3378,19 +3410,17 @@
         <v>168</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C121" t="s">
-        <v>205</v>
-      </c>
-      <c r="D121">
-        <v>2</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D121" s="1"/>
       <c r="E121" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3398,53 +3428,51 @@
         <v>168</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C122" t="s">
-        <v>210</v>
-      </c>
-      <c r="D122">
-        <v>2</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D122" s="1"/>
       <c r="E122" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>168</v>
-      </c>
-      <c r="B123" t="s">
-        <v>153</v>
+      <c r="A123" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C123" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>168</v>
-      </c>
-      <c r="B124" t="s">
-        <v>153</v>
+      <c r="A124" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C124" t="s">
-        <v>202</v>
+        <v>94</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3452,30 +3480,27 @@
         <v>168</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D125" t="s">
-        <v>149</v>
+        <v>216</v>
+      </c>
+      <c r="C125" t="s">
+        <v>207</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C126" t="s">
-        <v>100</v>
-      </c>
-      <c r="D126">
-        <v>1</v>
+      <c r="A126" t="s">
+        <v>168</v>
+      </c>
+      <c r="B126" t="s">
+        <v>153</v>
+      </c>
+      <c r="D126" t="s">
+        <v>149</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>52</v>
@@ -3489,19 +3514,19 @@
         <v>168</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>215</v>
+        <v>153</v>
       </c>
       <c r="C127" t="s">
         <v>205</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3509,55 +3534,166 @@
         <v>168</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>215</v>
+        <v>153</v>
       </c>
       <c r="C128" t="s">
         <v>210</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F128" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>168</v>
+      </c>
+      <c r="B129" t="s">
+        <v>153</v>
+      </c>
+      <c r="C129" t="s">
+        <v>201</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>168</v>
+      </c>
+      <c r="B130" t="s">
+        <v>153</v>
+      </c>
+      <c r="C130" t="s">
+        <v>202</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D131" t="s">
+        <v>149</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C132" t="s">
+        <v>100</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C133" t="s">
+        <v>205</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C134" t="s">
+        <v>210</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F134" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B129" s="1" t="s">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D135" t="s">
         <v>149</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E135" t="s">
         <v>199</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F135" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B130" s="1" t="s">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C136" t="s">
         <v>100</v>
       </c>
-      <c r="D130">
-        <v>1</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136" t="s">
         <v>199</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F136" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (range) Add metadata mappings for compare locations snippet (#735)
* [Word] (range) Add snippet to compare range locations

* Add metadata mappings
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25822"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E62E70-5EEC-4C49-AFDF-63710A621AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E279FA4-F754-4385-83E7-AB51BE59FCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-6180" yWindow="-19035" windowWidth="17250" windowHeight="8865" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="236">
   <si>
     <t>Class</t>
   </si>
@@ -716,6 +716,18 @@
   </si>
   <si>
     <t>ListLevelType</t>
+  </si>
+  <si>
+    <t>LocationRelation</t>
+  </si>
+  <si>
+    <t>word-ranges-compare-location</t>
+  </si>
+  <si>
+    <t>compareLocations</t>
+  </si>
+  <si>
+    <t>compareLocationWith</t>
   </si>
 </sst>
 </file>
@@ -830,8 +842,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F136" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F136" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F138" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F138" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1141,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E74" sqref="E74"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2402,19 +2414,19 @@
       <c r="A68" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="2" t="s">
         <v>227</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="2" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2422,19 +2434,19 @@
       <c r="A69" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="2" t="s">
         <v>224</v>
       </c>
       <c r="D69" s="2">
         <v>1</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="2" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2442,17 +2454,17 @@
       <c r="A70" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="2" t="s">
         <v>229</v>
       </c>
       <c r="D70" s="2"/>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="2" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2478,17 +2490,17 @@
       <c r="A72" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C72" s="5"/>
+      <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E72" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="2" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2496,17 +2508,17 @@
       <c r="A73" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C73" s="5"/>
+      <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E73" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="2" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2514,38 +2526,36 @@
       <c r="A74" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C74" s="5"/>
+      <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F74" s="2" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>98</v>
+      <c r="A75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2556,7 +2566,7 @@
         <v>91</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
@@ -2565,7 +2575,7 @@
         <v>151</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2576,14 +2586,16 @@
         <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D77" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
       <c r="E77" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2594,14 +2606,14 @@
         <v>91</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2612,14 +2624,14 @@
         <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2627,56 +2639,54 @@
         <v>168</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D80" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>168</v>
       </c>
-      <c r="B81" t="s">
-        <v>161</v>
-      </c>
-      <c r="D81" t="s">
-        <v>132</v>
+      <c r="B81" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>168</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>79</v>
+      <c r="B82" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82" t="s">
+        <v>132</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2687,16 +2697,16 @@
         <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>75</v>
+      <c r="E83" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2707,16 +2717,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2727,16 +2737,16 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,7 +2766,7 @@
         <v>71</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2767,16 +2777,16 @@
         <v>10</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D87" s="2">
         <v>1</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2787,16 +2797,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2806,17 +2816,17 @@
       <c r="B89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="1">
+      <c r="C89" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2826,17 +2836,17 @@
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="1">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2847,14 +2857,16 @@
         <v>10</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
       <c r="E91" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2865,14 +2877,14 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2883,14 +2895,14 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2901,14 +2913,14 @@
         <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2919,14 +2931,14 @@
         <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D95" s="2"/>
-      <c r="E95" s="1" t="s">
-        <v>79</v>
+      <c r="E95" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2934,19 +2946,17 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D96" s="2">
-        <v>1</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>70</v>
+        <v>8</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2957,14 +2967,16 @@
         <v>196</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D97" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
       <c r="E97" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>58</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2972,39 +2984,37 @@
         <v>168</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D98" s="1">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D99" s="1">
-        <v>1</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>122</v>
+      <c r="C99" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D99" s="2">
+        <v>1</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3015,16 +3025,16 @@
         <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="D100" s="1">
         <v>1</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>79</v>
+      <c r="E100" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3035,16 +3045,16 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>150</v>
+      <c r="E101" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3055,16 +3065,16 @@
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>82</v>
+      <c r="E102" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3075,16 +3085,16 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3095,14 +3105,16 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1" t="s">
-        <v>151</v>
+        <v>36</v>
+      </c>
+      <c r="D104" s="1">
+        <v>1</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3110,17 +3122,19 @@
         <v>168</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1" t="s">
-        <v>132</v>
+        <v>5</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D105" s="1">
+        <v>1</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3128,17 +3142,17 @@
         <v>168</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1" t="s">
-        <v>149</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3146,19 +3160,17 @@
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D107" s="1">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>78</v>
+        <v>163</v>
+      </c>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3168,17 +3180,15 @@
       <c r="B108" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D108" s="2">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>78</v>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3186,17 +3196,19 @@
         <v>168</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3204,55 +3216,55 @@
         <v>168</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2" t="s">
-        <v>132</v>
+        <v>27</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D110" s="2">
+        <v>1</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D112" s="2">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>174</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3262,33 +3274,35 @@
       <c r="B113" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E113" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C114" s="2"/>
-      <c r="D114" s="2" t="s">
-        <v>132</v>
+        <v>173</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D114" s="2">
+        <v>1</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>76</v>
+        <v>170</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3296,57 +3310,53 @@
         <v>168</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D115" s="2"/>
       <c r="E115" s="2" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
+      <c r="A116" t="s">
         <v>168</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D116" s="2">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>199</v>
+        <v>76</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D117" s="1">
-        <v>1</v>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3356,35 +3366,37 @@
       <c r="B118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D118" s="1">
+      <c r="C118" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D118" s="2">
         <v>1</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D119" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="D119" s="1">
+        <v>1</v>
+      </c>
       <c r="E119" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>200</v>
+        <v>54</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3395,14 +3407,16 @@
         <v>56</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D120" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1</v>
+      </c>
       <c r="E120" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3413,14 +3427,14 @@
         <v>56</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>211</v>
+        <v>21</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3431,7 +3445,7 @@
         <v>56</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="2" t="s">
@@ -3446,16 +3460,17 @@
         <v>168</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C123" t="s">
-        <v>206</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3463,16 +3478,17 @@
         <v>168</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C124" t="s">
-        <v>94</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D124" s="1"/>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3483,7 +3499,7 @@
         <v>216</v>
       </c>
       <c r="C125" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>199</v>
@@ -3493,20 +3509,20 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>168</v>
-      </c>
-      <c r="B126" t="s">
-        <v>153</v>
-      </c>
-      <c r="D126" t="s">
-        <v>149</v>
+      <c r="A126" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C126" t="s">
+        <v>94</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>54</v>
+        <v>204</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3514,110 +3530,107 @@
         <v>168</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="C127" t="s">
-        <v>205</v>
-      </c>
-      <c r="D127">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B128" s="1" t="s">
+      <c r="A128" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" t="s">
         <v>153</v>
       </c>
-      <c r="C128" t="s">
-        <v>210</v>
-      </c>
-      <c r="D128">
+      <c r="D128" t="s">
+        <v>149</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C129" t="s">
+        <v>205</v>
+      </c>
+      <c r="D129">
         <v>2</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>168</v>
-      </c>
-      <c r="B129" t="s">
-        <v>153</v>
-      </c>
-      <c r="C129" t="s">
-        <v>201</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>168</v>
-      </c>
-      <c r="B130" t="s">
+      <c r="A130" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C130" t="s">
-        <v>202</v>
+        <v>210</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D131" t="s">
-        <v>149</v>
+      <c r="A131" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" t="s">
+        <v>153</v>
+      </c>
+      <c r="C131" t="s">
+        <v>201</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>198</v>
+      <c r="A132" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" t="s">
+        <v>153</v>
       </c>
       <c r="C132" t="s">
-        <v>100</v>
-      </c>
-      <c r="D132">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>54</v>
+        <v>218</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3625,19 +3638,16 @@
         <v>168</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C133" t="s">
-        <v>205</v>
-      </c>
-      <c r="D133">
-        <v>1</v>
+        <v>198</v>
+      </c>
+      <c r="D133" t="s">
+        <v>149</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3645,19 +3655,19 @@
         <v>168</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C134" t="s">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="D134">
         <v>1</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>217</v>
+        <v>54</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3665,16 +3675,19 @@
         <v>168</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D135" t="s">
-        <v>149</v>
-      </c>
-      <c r="E135" t="s">
+        <v>215</v>
+      </c>
+      <c r="C135" t="s">
+        <v>205</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F135" t="s">
-        <v>212</v>
+      <c r="F135" s="2" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3682,18 +3695,55 @@
         <v>168</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C136" t="s">
+        <v>210</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D137" t="s">
+        <v>149</v>
+      </c>
+      <c r="E137" t="s">
+        <v>199</v>
+      </c>
+      <c r="F137" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C138" t="s">
         <v>100</v>
       </c>
-      <c r="D136">
-        <v>1</v>
-      </c>
-      <c r="E136" t="s">
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138" t="s">
         <v>199</v>
       </c>
-      <c r="F136" t="s">
+      <c r="F138" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (Body) Remove 3rd example from .search
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E279FA4-F754-4385-83E7-AB51BE59FCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04384470-42FA-4281-BDB9-CE6C01127C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-19035" windowWidth="17250" windowHeight="8865" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="236">
   <si>
     <t>Class</t>
   </si>
@@ -776,17 +776,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,8 +838,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F138" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F138" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F137" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F137" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1153,11 +1149,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,16 +1311,13 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1335,93 +1328,93 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F9" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" t="s">
-        <v>151</v>
-      </c>
-      <c r="F10" t="s">
-        <v>90</v>
+      <c r="C10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>168</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>23</v>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>168</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>94</v>
+      <c r="B14" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
       </c>
       <c r="E14" t="s">
         <v>151</v>
@@ -1435,67 +1428,67 @@
         <v>168</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="D15" t="s">
         <v>132</v>
       </c>
       <c r="E15" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>203</v>
+      <c r="A16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" t="s">
+        <v>157</v>
       </c>
       <c r="D16" t="s">
         <v>132</v>
       </c>
-      <c r="E16" t="s">
-        <v>199</v>
-      </c>
-      <c r="F16" t="s">
-        <v>204</v>
+      <c r="E16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" t="s">
-        <v>157</v>
+      <c r="A17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>75</v>
+        <v>199</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>158</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>208</v>
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
+        <v>130</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>209</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1503,7 +1496,7 @@
         <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
@@ -1512,7 +1505,7 @@
         <v>152</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1520,16 +1513,19 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1540,7 +1536,7 @@
         <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1549,7 +1545,7 @@
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1560,7 +1556,7 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1569,7 +1565,7 @@
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1580,16 +1576,13 @@
         <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E23" t="s">
         <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1600,13 +1593,13 @@
         <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E24" t="s">
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1614,16 +1607,19 @@
         <v>168</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1634,16 +1630,13 @@
         <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,56 +1644,56 @@
         <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>97</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>168</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>124</v>
-      </c>
-      <c r="F28" t="s">
-        <v>127</v>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
+      <c r="C29" t="s">
+        <v>123</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>46</v>
+        <v>124</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1713,63 +1706,66 @@
       <c r="C30" t="s">
         <v>123</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" t="s">
         <v>124</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>125</v>
+      <c r="F30" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>168</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C31" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" t="s">
-        <v>124</v>
-      </c>
-      <c r="F31" t="s">
-        <v>126</v>
+      <c r="C31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="2"/>
+      <c r="B32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" t="s">
+        <v>132</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>42</v>
+      <c r="F32" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>168</v>
       </c>
-      <c r="B33" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" t="s">
-        <v>132</v>
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" t="s">
-        <v>46</v>
+        <v>82</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1777,19 +1773,17 @@
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>37</v>
+        <v>124</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,7 +1794,7 @@
         <v>128</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
@@ -1811,39 +1805,41 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>177</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="E36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>126</v>
+        <v>73</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>149</v>
+        <v>61</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1863,7 +1859,7 @@
         <v>73</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1873,35 +1869,35 @@
       <c r="B39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="2">
-        <v>1</v>
-      </c>
+      <c r="C39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>61</v>
+        <v>184</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
       <c r="E40" s="2" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>63</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1912,7 +1908,7 @@
         <v>184</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>97</v>
+        <v>189</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1921,7 +1917,7 @@
         <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1932,7 +1928,7 @@
         <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1941,7 +1937,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1952,7 +1948,7 @@
         <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1961,7 +1957,7 @@
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1972,7 +1968,7 @@
         <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1981,7 +1977,7 @@
         <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1992,16 +1988,14 @@
         <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2009,12 +2003,14 @@
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D46" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
       <c r="E46" s="2" t="s">
         <v>186</v>
       </c>
@@ -2030,7 +2026,7 @@
         <v>194</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -2039,27 +2035,25 @@
         <v>186</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>168</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>194</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="2" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2069,33 +2063,33 @@
       <c r="B49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D49" s="1"/>
+      <c r="C49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>152</v>
+        <v>74</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2103,35 +2097,35 @@
         <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D51" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E51" s="2" t="s">
-        <v>170</v>
+        <v>73</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>175</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>63</v>
+        <v>124</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2139,17 +2133,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>126</v>
+        <v>169</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2160,14 +2154,14 @@
         <v>137</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2178,14 +2172,14 @@
         <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2193,12 +2187,14 @@
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D56" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
       <c r="E56" s="2" t="s">
         <v>169</v>
       </c>
@@ -2214,16 +2210,14 @@
         <v>144</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2231,35 +2225,35 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E58" s="2" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>136</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2267,50 +2261,50 @@
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>179</v>
+        <v>25</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
-        <v>149</v>
+      <c r="C61" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
         <v>70</v>
       </c>
@@ -2323,12 +2317,12 @@
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>183</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>70</v>
       </c>
@@ -2337,39 +2331,39 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>70</v>
+        <v>145</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>159</v>
+        <v>221</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>160</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2379,9 +2373,11 @@
       <c r="B66" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2" t="s">
-        <v>149</v>
+      <c r="C66" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>57</v>
@@ -2398,16 +2394,16 @@
         <v>221</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>57</v>
+        <v>225</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2418,7 +2414,7 @@
         <v>221</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
@@ -2438,11 +2434,9 @@
         <v>221</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="D69" s="2"/>
       <c r="E69" s="2" t="s">
         <v>225</v>
       </c>
@@ -2455,17 +2449,17 @@
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2473,17 +2467,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D71" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E71" s="2" t="s">
-        <v>57</v>
+        <v>225</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2491,7 +2485,7 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
@@ -2509,7 +2503,7 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -2527,35 +2521,37 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>234</v>
+      <c r="A75" t="s">
+        <v>168</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2566,7 +2562,7 @@
         <v>91</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
@@ -2575,7 +2571,7 @@
         <v>151</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2586,16 +2582,14 @@
         <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D77" s="2"/>
       <c r="E77" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,14 +2600,14 @@
         <v>91</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2624,14 +2618,14 @@
         <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2639,54 +2633,56 @@
         <v>168</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D80" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
       <c r="E80" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>168</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+      <c r="D81" t="s">
+        <v>132</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>168</v>
       </c>
-      <c r="B82" t="s">
-        <v>161</v>
-      </c>
-      <c r="D82" t="s">
-        <v>132</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>151</v>
+      <c r="B82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2697,16 +2693,16 @@
         <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>79</v>
+      <c r="E83" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2717,16 +2713,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2737,16 +2733,16 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2766,7 +2762,7 @@
         <v>71</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2777,16 +2773,16 @@
         <v>10</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D87" s="2">
         <v>1</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2797,16 +2793,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2816,17 +2812,17 @@
       <c r="B89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D89" s="2">
+      <c r="C89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="1">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2836,17 +2832,17 @@
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="2">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2857,16 +2853,14 @@
         <v>10</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D91" s="2"/>
       <c r="E91" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2877,14 +2871,14 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2895,14 +2889,14 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2913,14 +2907,14 @@
         <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2931,14 +2925,14 @@
         <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D95" s="2"/>
-      <c r="E95" s="2" t="s">
-        <v>80</v>
+      <c r="E95" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2946,17 +2940,19 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>10</v>
+        <v>196</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" s="2"/>
-      <c r="E96" s="1" t="s">
-        <v>79</v>
+        <v>182</v>
+      </c>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2967,54 +2963,54 @@
         <v>196</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D97" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D97" s="2"/>
       <c r="E97" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>181</v>
+        <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>196</v>
+        <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D98" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
       <c r="E98" s="2" t="s">
-        <v>57</v>
+        <v>233</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="4" t="s">
+      <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="D99" s="2">
-        <v>1</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>234</v>
+      <c r="C99" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D99" s="1">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3025,16 +3021,16 @@
         <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="D100" s="1">
         <v>1</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3045,16 +3041,16 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>152</v>
+      <c r="E101" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3065,16 +3061,16 @@
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3085,16 +3081,16 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>150</v>
+      <c r="E103" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3105,16 +3101,16 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>82</v>
+      <c r="E104" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3125,16 +3121,14 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D105" s="1">
-        <v>1</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D105" s="1"/>
       <c r="E105" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3142,17 +3136,17 @@
         <v>168</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D106" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E106" s="1" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3160,17 +3154,17 @@
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>163</v>
+        <v>27</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3180,15 +3174,17 @@
       <c r="B108" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>145</v>
+      <c r="C108" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D108" s="1">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,17 +3194,17 @@
       <c r="B109" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D109" s="1">
+      <c r="C109" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D109" s="2">
         <v>1</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3216,19 +3212,17 @@
         <v>168</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D110" s="2">
-        <v>1</v>
+        <v>147</v>
+      </c>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>40</v>
+        <v>148</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3236,35 +3230,35 @@
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>49</v>
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3274,15 +3268,17 @@
       <c r="B113" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2" t="s">
-        <v>149</v>
+      <c r="C113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" s="2">
+        <v>1</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3293,52 +3289,50 @@
         <v>173</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D114" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D114" s="2"/>
       <c r="E114" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+      <c r="A115" t="s">
         <v>168</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D115" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E115" s="2" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>133</v>
+        <v>56</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3348,55 +3342,57 @@
       <c r="B117" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2" t="s">
-        <v>149</v>
+      <c r="C117" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D117" s="2">
+        <v>1</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>53</v>
+        <v>204</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>168</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D118" s="2">
+      <c r="C118" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D118" s="1">
         <v>1</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>204</v>
+        <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>54</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3407,16 +3403,14 @@
         <v>56</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D120" s="1">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D120" s="1"/>
       <c r="E120" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3427,7 +3421,7 @@
         <v>56</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="2" t="s">
@@ -3445,14 +3439,14 @@
         <v>56</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3463,14 +3457,14 @@
         <v>56</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3478,17 +3472,16 @@
         <v>168</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D124" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="C124" t="s">
+        <v>206</v>
+      </c>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3499,7 +3492,7 @@
         <v>216</v>
       </c>
       <c r="C125" t="s">
-        <v>206</v>
+        <v>94</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>199</v>
@@ -3516,7 +3509,7 @@
         <v>216</v>
       </c>
       <c r="C126" t="s">
-        <v>94</v>
+        <v>207</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>199</v>
@@ -3526,37 +3519,40 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C127" t="s">
-        <v>207</v>
+      <c r="A127" t="s">
+        <v>168</v>
+      </c>
+      <c r="B127" t="s">
+        <v>153</v>
+      </c>
+      <c r="D127" t="s">
+        <v>149</v>
       </c>
       <c r="E127" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C128" t="s">
+        <v>205</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+      <c r="E128" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F127" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>168</v>
-      </c>
-      <c r="B128" t="s">
-        <v>153</v>
-      </c>
-      <c r="D128" t="s">
-        <v>149</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="F128" s="2" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3567,7 +3563,7 @@
         <v>153</v>
       </c>
       <c r="C129" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D129">
         <v>2</v>
@@ -3576,27 +3572,24 @@
         <v>199</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B130" s="1" t="s">
+      <c r="A130" t="s">
+        <v>168</v>
+      </c>
+      <c r="B130" t="s">
         <v>153</v>
       </c>
       <c r="C130" t="s">
-        <v>210</v>
-      </c>
-      <c r="D130">
-        <v>2</v>
+        <v>201</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3607,7 +3600,7 @@
         <v>153</v>
       </c>
       <c r="C131" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>199</v>
@@ -3617,20 +3610,20 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>168</v>
-      </c>
-      <c r="B132" t="s">
-        <v>153</v>
-      </c>
-      <c r="C132" t="s">
-        <v>202</v>
+      <c r="A132" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D132" t="s">
+        <v>149</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3640,14 +3633,17 @@
       <c r="B133" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D133" t="s">
-        <v>149</v>
+      <c r="C133" t="s">
+        <v>100</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>200</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3655,19 +3651,19 @@
         <v>168</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="C134" t="s">
-        <v>100</v>
+        <v>205</v>
       </c>
       <c r="D134">
         <v>1</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>54</v>
+        <v>214</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3678,7 +3674,7 @@
         <v>215</v>
       </c>
       <c r="C135" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -3687,7 +3683,7 @@
         <v>199</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3695,19 +3691,16 @@
         <v>168</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C136" t="s">
-        <v>210</v>
-      </c>
-      <c r="D136">
-        <v>1</v>
-      </c>
-      <c r="E136" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D136" t="s">
+        <v>149</v>
+      </c>
+      <c r="E136" t="s">
         <v>199</v>
       </c>
-      <c r="F136" s="2" t="s">
-        <v>217</v>
+      <c r="F136" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3717,33 +3710,16 @@
       <c r="B137" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D137" t="s">
-        <v>149</v>
+      <c r="C137" t="s">
+        <v>100</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
       </c>
       <c r="E137" t="s">
         <v>199</v>
       </c>
       <c r="F137" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C138" t="s">
-        <v>100</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
-      </c>
-      <c r="E138" t="s">
-        <v>199</v>
-      </c>
-      <c r="F138" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (Body) Remove 3rd example from .search (#755)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E279FA4-F754-4385-83E7-AB51BE59FCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04384470-42FA-4281-BDB9-CE6C01127C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-19035" windowWidth="17250" windowHeight="8865" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="236">
   <si>
     <t>Class</t>
   </si>
@@ -776,17 +776,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,8 +838,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F138" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F138" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F137" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F137" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1153,11 +1149,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,16 +1311,13 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1335,93 +1328,93 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F9" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" t="s">
-        <v>151</v>
-      </c>
-      <c r="F10" t="s">
-        <v>90</v>
+      <c r="C10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>168</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>23</v>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>168</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>94</v>
+      <c r="B14" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
       </c>
       <c r="E14" t="s">
         <v>151</v>
@@ -1435,67 +1428,67 @@
         <v>168</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="D15" t="s">
         <v>132</v>
       </c>
       <c r="E15" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>203</v>
+      <c r="A16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" t="s">
+        <v>157</v>
       </c>
       <c r="D16" t="s">
         <v>132</v>
       </c>
-      <c r="E16" t="s">
-        <v>199</v>
-      </c>
-      <c r="F16" t="s">
-        <v>204</v>
+      <c r="E16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" t="s">
-        <v>157</v>
+      <c r="A17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>75</v>
+        <v>199</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>158</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>208</v>
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
+        <v>130</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>209</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1503,7 +1496,7 @@
         <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
@@ -1512,7 +1505,7 @@
         <v>152</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1520,16 +1513,19 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1540,7 +1536,7 @@
         <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1549,7 +1545,7 @@
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1560,7 +1556,7 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1569,7 +1565,7 @@
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1580,16 +1576,13 @@
         <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E23" t="s">
         <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1600,13 +1593,13 @@
         <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E24" t="s">
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1614,16 +1607,19 @@
         <v>168</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1634,16 +1630,13 @@
         <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,56 +1644,56 @@
         <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>97</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>168</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>124</v>
-      </c>
-      <c r="F28" t="s">
-        <v>127</v>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
+      <c r="C29" t="s">
+        <v>123</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>46</v>
+        <v>124</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1713,63 +1706,66 @@
       <c r="C30" t="s">
         <v>123</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" t="s">
         <v>124</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>125</v>
+      <c r="F30" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>168</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C31" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" t="s">
-        <v>124</v>
-      </c>
-      <c r="F31" t="s">
-        <v>126</v>
+      <c r="C31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="2"/>
+      <c r="B32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" t="s">
+        <v>132</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>42</v>
+      <c r="F32" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>168</v>
       </c>
-      <c r="B33" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" t="s">
-        <v>132</v>
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" t="s">
-        <v>46</v>
+        <v>82</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1777,19 +1773,17 @@
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>37</v>
+        <v>124</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,7 +1794,7 @@
         <v>128</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
@@ -1811,39 +1805,41 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>177</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="E36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>126</v>
+        <v>73</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>149</v>
+        <v>61</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1863,7 +1859,7 @@
         <v>73</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1873,35 +1869,35 @@
       <c r="B39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="2">
-        <v>1</v>
-      </c>
+      <c r="C39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>61</v>
+        <v>184</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
       <c r="E40" s="2" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>63</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1912,7 +1908,7 @@
         <v>184</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>97</v>
+        <v>189</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1921,7 +1917,7 @@
         <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1932,7 +1928,7 @@
         <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1941,7 +1937,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1952,7 +1948,7 @@
         <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1961,7 +1957,7 @@
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1972,7 +1968,7 @@
         <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1981,7 +1977,7 @@
         <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1992,16 +1988,14 @@
         <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2009,12 +2003,14 @@
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D46" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
       <c r="E46" s="2" t="s">
         <v>186</v>
       </c>
@@ -2030,7 +2026,7 @@
         <v>194</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -2039,27 +2035,25 @@
         <v>186</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>168</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>194</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="2" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2069,33 +2063,33 @@
       <c r="B49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D49" s="1"/>
+      <c r="C49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>152</v>
+        <v>74</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2103,35 +2097,35 @@
         <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D51" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E51" s="2" t="s">
-        <v>170</v>
+        <v>73</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>175</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>63</v>
+        <v>124</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2139,17 +2133,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>126</v>
+        <v>169</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2160,14 +2154,14 @@
         <v>137</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2178,14 +2172,14 @@
         <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2193,12 +2187,14 @@
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D56" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
       <c r="E56" s="2" t="s">
         <v>169</v>
       </c>
@@ -2214,16 +2210,14 @@
         <v>144</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2231,35 +2225,35 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E58" s="2" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>136</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2267,50 +2261,50 @@
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>179</v>
+        <v>25</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
-        <v>149</v>
+      <c r="C61" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
         <v>70</v>
       </c>
@@ -2323,12 +2317,12 @@
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>183</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>70</v>
       </c>
@@ -2337,39 +2331,39 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>70</v>
+        <v>145</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>159</v>
+        <v>221</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>160</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2379,9 +2373,11 @@
       <c r="B66" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2" t="s">
-        <v>149</v>
+      <c r="C66" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>57</v>
@@ -2398,16 +2394,16 @@
         <v>221</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>57</v>
+        <v>225</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2418,7 +2414,7 @@
         <v>221</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
@@ -2438,11 +2434,9 @@
         <v>221</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="D69" s="2"/>
       <c r="E69" s="2" t="s">
         <v>225</v>
       </c>
@@ -2455,17 +2449,17 @@
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2473,17 +2467,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D71" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E71" s="2" t="s">
-        <v>57</v>
+        <v>225</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2491,7 +2485,7 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
@@ -2509,7 +2503,7 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -2527,35 +2521,37 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>234</v>
+      <c r="A75" t="s">
+        <v>168</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2566,7 +2562,7 @@
         <v>91</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
@@ -2575,7 +2571,7 @@
         <v>151</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2586,16 +2582,14 @@
         <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D77" s="2"/>
       <c r="E77" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,14 +2600,14 @@
         <v>91</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2624,14 +2618,14 @@
         <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2639,54 +2633,56 @@
         <v>168</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D80" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
       <c r="E80" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>168</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+      <c r="D81" t="s">
+        <v>132</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>168</v>
       </c>
-      <c r="B82" t="s">
-        <v>161</v>
-      </c>
-      <c r="D82" t="s">
-        <v>132</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>151</v>
+      <c r="B82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2697,16 +2693,16 @@
         <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>79</v>
+      <c r="E83" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2717,16 +2713,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2737,16 +2733,16 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2766,7 +2762,7 @@
         <v>71</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2777,16 +2773,16 @@
         <v>10</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D87" s="2">
         <v>1</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2797,16 +2793,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2816,17 +2812,17 @@
       <c r="B89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D89" s="2">
+      <c r="C89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="1">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2836,17 +2832,17 @@
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="2">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2857,16 +2853,14 @@
         <v>10</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="2">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D91" s="2"/>
       <c r="E91" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2877,14 +2871,14 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2895,14 +2889,14 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2913,14 +2907,14 @@
         <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2931,14 +2925,14 @@
         <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D95" s="2"/>
-      <c r="E95" s="2" t="s">
-        <v>80</v>
+      <c r="E95" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2946,17 +2940,19 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>10</v>
+        <v>196</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" s="2"/>
-      <c r="E96" s="1" t="s">
-        <v>79</v>
+        <v>182</v>
+      </c>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2967,54 +2963,54 @@
         <v>196</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D97" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D97" s="2"/>
       <c r="E97" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>181</v>
+        <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>196</v>
+        <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D98" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
       <c r="E98" s="2" t="s">
-        <v>57</v>
+        <v>233</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="4" t="s">
+      <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="D99" s="2">
-        <v>1</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>234</v>
+      <c r="C99" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D99" s="1">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3025,16 +3021,16 @@
         <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="D100" s="1">
         <v>1</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3045,16 +3041,16 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>152</v>
+      <c r="E101" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3065,16 +3061,16 @@
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3085,16 +3081,16 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>150</v>
+      <c r="E103" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3105,16 +3101,16 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>82</v>
+      <c r="E104" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3125,16 +3121,14 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D105" s="1">
-        <v>1</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D105" s="1"/>
       <c r="E105" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3142,17 +3136,17 @@
         <v>168</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D106" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E106" s="1" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3160,17 +3154,17 @@
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>163</v>
+        <v>27</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3180,15 +3174,17 @@
       <c r="B108" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>145</v>
+      <c r="C108" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D108" s="1">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,17 +3194,17 @@
       <c r="B109" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D109" s="1">
+      <c r="C109" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D109" s="2">
         <v>1</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3216,19 +3212,17 @@
         <v>168</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D110" s="2">
-        <v>1</v>
+        <v>147</v>
+      </c>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>40</v>
+        <v>148</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3236,35 +3230,35 @@
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>49</v>
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3274,15 +3268,17 @@
       <c r="B113" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2" t="s">
-        <v>149</v>
+      <c r="C113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" s="2">
+        <v>1</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3293,52 +3289,50 @@
         <v>173</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D114" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D114" s="2"/>
       <c r="E114" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+      <c r="A115" t="s">
         <v>168</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D115" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E115" s="2" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>133</v>
+        <v>56</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3348,55 +3342,57 @@
       <c r="B117" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2" t="s">
-        <v>149</v>
+      <c r="C117" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D117" s="2">
+        <v>1</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>53</v>
+        <v>204</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>168</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D118" s="2">
+      <c r="C118" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D118" s="1">
         <v>1</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>204</v>
+        <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>54</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3407,16 +3403,14 @@
         <v>56</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D120" s="1">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D120" s="1"/>
       <c r="E120" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3427,7 +3421,7 @@
         <v>56</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="2" t="s">
@@ -3445,14 +3439,14 @@
         <v>56</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3463,14 +3457,14 @@
         <v>56</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3478,17 +3472,16 @@
         <v>168</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D124" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="C124" t="s">
+        <v>206</v>
+      </c>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3499,7 +3492,7 @@
         <v>216</v>
       </c>
       <c r="C125" t="s">
-        <v>206</v>
+        <v>94</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>199</v>
@@ -3516,7 +3509,7 @@
         <v>216</v>
       </c>
       <c r="C126" t="s">
-        <v>94</v>
+        <v>207</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>199</v>
@@ -3526,37 +3519,40 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C127" t="s">
-        <v>207</v>
+      <c r="A127" t="s">
+        <v>168</v>
+      </c>
+      <c r="B127" t="s">
+        <v>153</v>
+      </c>
+      <c r="D127" t="s">
+        <v>149</v>
       </c>
       <c r="E127" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C128" t="s">
+        <v>205</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+      <c r="E128" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F127" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>168</v>
-      </c>
-      <c r="B128" t="s">
-        <v>153</v>
-      </c>
-      <c r="D128" t="s">
-        <v>149</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="F128" s="2" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3567,7 +3563,7 @@
         <v>153</v>
       </c>
       <c r="C129" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D129">
         <v>2</v>
@@ -3576,27 +3572,24 @@
         <v>199</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B130" s="1" t="s">
+      <c r="A130" t="s">
+        <v>168</v>
+      </c>
+      <c r="B130" t="s">
         <v>153</v>
       </c>
       <c r="C130" t="s">
-        <v>210</v>
-      </c>
-      <c r="D130">
-        <v>2</v>
+        <v>201</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3607,7 +3600,7 @@
         <v>153</v>
       </c>
       <c r="C131" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>199</v>
@@ -3617,20 +3610,20 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>168</v>
-      </c>
-      <c r="B132" t="s">
-        <v>153</v>
-      </c>
-      <c r="C132" t="s">
-        <v>202</v>
+      <c r="A132" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D132" t="s">
+        <v>149</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3640,14 +3633,17 @@
       <c r="B133" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D133" t="s">
-        <v>149</v>
+      <c r="C133" t="s">
+        <v>100</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>200</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3655,19 +3651,19 @@
         <v>168</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="C134" t="s">
-        <v>100</v>
+        <v>205</v>
       </c>
       <c r="D134">
         <v>1</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>54</v>
+        <v>214</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3678,7 +3674,7 @@
         <v>215</v>
       </c>
       <c r="C135" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -3687,7 +3683,7 @@
         <v>199</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3695,19 +3691,16 @@
         <v>168</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C136" t="s">
-        <v>210</v>
-      </c>
-      <c r="D136">
-        <v>1</v>
-      </c>
-      <c r="E136" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D136" t="s">
+        <v>149</v>
+      </c>
+      <c r="E136" t="s">
         <v>199</v>
       </c>
-      <c r="F136" s="2" t="s">
-        <v>217</v>
+      <c r="F136" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3717,33 +3710,16 @@
       <c r="B137" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D137" t="s">
-        <v>149</v>
+      <c r="C137" t="s">
+        <v>100</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
       </c>
       <c r="E137" t="s">
         <v>199</v>
       </c>
       <c r="F137" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C138" t="s">
-        <v>100</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
-      </c>
-      <c r="E138" t="s">
-        <v>199</v>
-      </c>
-      <c r="F138" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (Footer) Remap sample
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26202"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04384470-42FA-4281-BDB9-CE6C01127C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877AC9A9-5FE0-4186-AF33-094BB6AA1F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -1152,8 +1152,8 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3198,7 +3198,7 @@
         <v>41</v>
       </c>
       <c r="D109" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
[Word] (Footer) Remap sample (#759)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26202"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04384470-42FA-4281-BDB9-CE6C01127C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877AC9A9-5FE0-4186-AF33-094BB6AA1F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -1152,8 +1152,8 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3198,7 +3198,7 @@
         <v>41</v>
       </c>
       <c r="D109" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
[Word] (preview) Update Style to BuiltInStyleName
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26207"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877AC9A9-5FE0-4186-AF33-094BB6AA1F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC01AE-16DB-4BDA-BFA2-AFE22B4DDDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="238">
   <si>
     <t>Class</t>
   </si>
@@ -728,6 +728,12 @@
   </si>
   <si>
     <t>compareLocationWith</t>
+  </si>
+  <si>
+    <t>BuiltInStyleName</t>
+  </si>
+  <si>
+    <t>word-insert-formatted-text</t>
   </si>
 </sst>
 </file>
@@ -838,8 +844,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F137" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F137" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F138" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F138" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1149,11 +1155,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1458,37 +1464,38 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>168</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="D17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" t="s">
-        <v>130</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1496,7 +1503,7 @@
         <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
@@ -1505,7 +1512,7 @@
         <v>152</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,19 +1520,16 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1536,7 +1540,7 @@
         <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1545,7 +1549,7 @@
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1556,7 +1560,7 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1565,7 +1569,7 @@
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1576,13 +1580,16 @@
         <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23" t="s">
         <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1593,13 +1600,13 @@
         <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E24" t="s">
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1607,19 +1614,16 @@
         <v>168</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="E25" t="s">
         <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1630,13 +1634,16 @@
         <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1644,56 +1651,56 @@
         <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>46</v>
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>124</v>
+      </c>
+      <c r="F28" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>168</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C29" t="s">
-        <v>123</v>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1706,66 +1713,63 @@
       <c r="C30" t="s">
         <v>123</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F30" t="s">
-        <v>126</v>
+      <c r="F30" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>42</v>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" t="s">
-        <v>162</v>
-      </c>
-      <c r="D32" t="s">
-        <v>132</v>
-      </c>
+      <c r="B32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F32" t="s">
-        <v>46</v>
+      <c r="F32" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>168</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
+      <c r="B33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" t="s">
+        <v>132</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1773,17 +1777,19 @@
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
       <c r="E34" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1794,7 +1800,7 @@
         <v>128</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
@@ -1805,41 +1811,39 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>168</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1859,7 +1863,7 @@
         <v>73</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1869,35 +1873,35 @@
       <c r="B39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="1"/>
+      <c r="C39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
       <c r="E39" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1908,7 +1912,7 @@
         <v>184</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>189</v>
+        <v>97</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1917,7 +1921,7 @@
         <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1928,7 +1932,7 @@
         <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1937,7 +1941,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1948,7 +1952,7 @@
         <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1957,7 +1961,7 @@
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1968,7 +1972,7 @@
         <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1977,7 +1981,7 @@
         <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1988,14 +1992,16 @@
         <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D45" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
       <c r="E45" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2003,14 +2009,12 @@
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
         <v>186</v>
       </c>
@@ -2026,7 +2030,7 @@
         <v>194</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>193</v>
+        <v>4</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -2035,25 +2039,27 @@
         <v>186</v>
       </c>
       <c r="F47" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2063,33 +2069,33 @@
       <c r="B49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="2"/>
+      <c r="C49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>170</v>
+        <v>74</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2097,35 +2103,35 @@
         <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>168</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2133,17 +2139,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E53" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2154,14 +2160,14 @@
         <v>137</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2172,14 +2178,14 @@
         <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,14 +2193,12 @@
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
         <v>169</v>
       </c>
@@ -2210,14 +2214,16 @@
         <v>144</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
       <c r="E57" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2225,35 +2231,35 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2261,50 +2267,50 @@
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1</v>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D62" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
       <c r="E62" s="2" t="s">
         <v>70</v>
       </c>
@@ -2317,12 +2323,12 @@
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
         <v>70</v>
       </c>
@@ -2331,39 +2337,39 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>221</v>
+        <v>159</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2373,11 +2379,9 @@
       <c r="B66" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>57</v>
@@ -2394,16 +2398,16 @@
         <v>221</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>227</v>
+        <v>30</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2414,7 +2418,7 @@
         <v>221</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
@@ -2434,9 +2438,11 @@
         <v>221</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D69" s="2"/>
+        <v>224</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
       <c r="E69" s="2" t="s">
         <v>225</v>
       </c>
@@ -2449,17 +2455,17 @@
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
-        <v>57</v>
+        <v>225</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2467,17 +2473,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2485,7 +2491,7 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
@@ -2503,7 +2509,7 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -2521,37 +2527,35 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E74" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2562,7 +2566,7 @@
         <v>91</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
@@ -2571,7 +2575,7 @@
         <v>151</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,14 +2586,16 @@
         <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D77" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
       <c r="E77" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2600,14 +2606,14 @@
         <v>91</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2618,14 +2624,14 @@
         <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2633,56 +2639,54 @@
         <v>168</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D80" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>168</v>
       </c>
-      <c r="B81" t="s">
-        <v>161</v>
-      </c>
-      <c r="D81" t="s">
-        <v>132</v>
+      <c r="B81" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>168</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>79</v>
+      <c r="B82" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82" t="s">
+        <v>132</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2693,16 +2697,16 @@
         <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>75</v>
+      <c r="E83" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2713,16 +2717,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2733,16 +2737,16 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2762,7 +2766,7 @@
         <v>71</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2773,16 +2777,16 @@
         <v>10</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D87" s="2">
         <v>1</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2793,16 +2797,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2812,17 +2816,17 @@
       <c r="B89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="1">
+      <c r="C89" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2832,17 +2836,17 @@
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="1">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2853,14 +2857,16 @@
         <v>10</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
       <c r="E91" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2871,14 +2877,14 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2889,14 +2895,14 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2907,14 +2913,14 @@
         <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2925,14 +2931,14 @@
         <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D95" s="2"/>
-      <c r="E95" s="1" t="s">
-        <v>79</v>
+      <c r="E95" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2940,19 +2946,17 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D96" s="2">
-        <v>1</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>70</v>
+        <v>8</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2963,54 +2967,54 @@
         <v>196</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>168</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2" t="s">
+      <c r="D98" s="2"/>
+      <c r="E98" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D98" s="2">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D99" s="1">
+      <c r="C99" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D99" s="2">
         <v>1</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>150</v>
+        <v>233</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>108</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3021,16 +3025,16 @@
         <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D100" s="1">
         <v>1</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3041,16 +3045,16 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>79</v>
+      <c r="E101" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3061,16 +3065,16 @@
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3081,16 +3085,16 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>82</v>
+      <c r="E103" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3101,16 +3105,16 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
       </c>
-      <c r="E104" s="1" t="s">
-        <v>151</v>
+      <c r="E104" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3121,14 +3125,16 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D105" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="D105" s="1">
+        <v>1</v>
+      </c>
       <c r="E105" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3136,17 +3142,17 @@
         <v>168</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3154,17 +3160,17 @@
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3174,17 +3180,15 @@
       <c r="B108" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D108" s="1">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>78</v>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3194,17 +3198,17 @@
       <c r="B109" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D109" s="2">
-        <v>2</v>
+      <c r="C109" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3212,17 +3216,19 @@
         <v>168</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D110" s="2">
+        <v>2</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>148</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3230,35 +3236,35 @@
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3268,17 +3274,15 @@
       <c r="B113" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D113" s="2">
-        <v>1</v>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3289,50 +3293,52 @@
         <v>173</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D114" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D114" s="2">
+        <v>1</v>
+      </c>
       <c r="E114" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F114" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>168</v>
-      </c>
-      <c r="B115" s="1" t="s">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>168</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3342,57 +3348,55 @@
       <c r="B117" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C117" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D117" s="2">
-        <v>1</v>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>204</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D118" s="1">
+      <c r="C118" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D118" s="2">
         <v>1</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>54</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>210</v>
+        <v>55</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>209</v>
+        <v>54</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3403,14 +3407,16 @@
         <v>56</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D120" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1</v>
+      </c>
       <c r="E120" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3421,7 +3427,7 @@
         <v>56</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>201</v>
+        <v>21</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="2" t="s">
@@ -3439,14 +3445,14 @@
         <v>56</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3457,14 +3463,14 @@
         <v>56</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3472,16 +3478,17 @@
         <v>168</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C124" t="s">
-        <v>206</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D124" s="1"/>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3492,7 +3499,7 @@
         <v>216</v>
       </c>
       <c r="C125" t="s">
-        <v>94</v>
+        <v>206</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>199</v>
@@ -3509,7 +3516,7 @@
         <v>216</v>
       </c>
       <c r="C126" t="s">
-        <v>207</v>
+        <v>94</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>199</v>
@@ -3519,40 +3526,37 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>168</v>
-      </c>
-      <c r="B127" t="s">
+      <c r="A127" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C127" t="s">
+        <v>207</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" t="s">
         <v>153</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D128" t="s">
         <v>149</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="E128" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="F128" s="2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C128" t="s">
-        <v>205</v>
-      </c>
-      <c r="D128">
-        <v>2</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3563,7 +3567,7 @@
         <v>153</v>
       </c>
       <c r="C129" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D129">
         <v>2</v>
@@ -3572,24 +3576,27 @@
         <v>199</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>168</v>
-      </c>
-      <c r="B130" t="s">
+      <c r="A130" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C130" t="s">
-        <v>201</v>
+        <v>210</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3600,7 +3607,7 @@
         <v>153</v>
       </c>
       <c r="C131" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>199</v>
@@ -3610,20 +3617,20 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D132" t="s">
-        <v>149</v>
+      <c r="A132" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" t="s">
+        <v>153</v>
+      </c>
+      <c r="C132" t="s">
+        <v>202</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3633,17 +3640,14 @@
       <c r="B133" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C133" t="s">
-        <v>100</v>
-      </c>
-      <c r="D133">
-        <v>1</v>
+      <c r="D133" t="s">
+        <v>149</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3651,19 +3655,19 @@
         <v>168</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C134" t="s">
-        <v>205</v>
+        <v>100</v>
       </c>
       <c r="D134">
         <v>1</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>214</v>
+        <v>54</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3674,7 +3678,7 @@
         <v>215</v>
       </c>
       <c r="C135" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -3683,7 +3687,7 @@
         <v>199</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3691,16 +3695,19 @@
         <v>168</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D136" t="s">
-        <v>149</v>
-      </c>
-      <c r="E136" t="s">
+        <v>215</v>
+      </c>
+      <c r="C136" t="s">
+        <v>210</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F136" t="s">
-        <v>212</v>
+      <c r="F136" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3710,16 +3717,33 @@
       <c r="B137" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C137" t="s">
-        <v>100</v>
-      </c>
-      <c r="D137">
-        <v>1</v>
+      <c r="D137" t="s">
+        <v>149</v>
       </c>
       <c r="E137" t="s">
         <v>199</v>
       </c>
       <c r="F137" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C138" t="s">
+        <v>100</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138" t="s">
+        <v>199</v>
+      </c>
+      <c r="F138" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] (preview) Update Style to BuiltInStyleName (#761)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26207"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877AC9A9-5FE0-4186-AF33-094BB6AA1F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC01AE-16DB-4BDA-BFA2-AFE22B4DDDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="238">
   <si>
     <t>Class</t>
   </si>
@@ -728,6 +728,12 @@
   </si>
   <si>
     <t>compareLocationWith</t>
+  </si>
+  <si>
+    <t>BuiltInStyleName</t>
+  </si>
+  <si>
+    <t>word-insert-formatted-text</t>
   </si>
 </sst>
 </file>
@@ -838,8 +844,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F137" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F137" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F138" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F138" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1149,11 +1155,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1458,37 +1464,38 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>168</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="D17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" t="s">
-        <v>130</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1496,7 +1503,7 @@
         <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
@@ -1505,7 +1512,7 @@
         <v>152</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,19 +1520,16 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1536,7 +1540,7 @@
         <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1545,7 +1549,7 @@
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1556,7 +1560,7 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1565,7 +1569,7 @@
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1576,13 +1580,16 @@
         <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23" t="s">
         <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1593,13 +1600,13 @@
         <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E24" t="s">
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1607,19 +1614,16 @@
         <v>168</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="E25" t="s">
         <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1630,13 +1634,16 @@
         <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1644,56 +1651,56 @@
         <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>46</v>
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>124</v>
+      </c>
+      <c r="F28" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>168</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C29" t="s">
-        <v>123</v>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1706,66 +1713,63 @@
       <c r="C30" t="s">
         <v>123</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F30" t="s">
-        <v>126</v>
+      <c r="F30" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>42</v>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" t="s">
-        <v>162</v>
-      </c>
-      <c r="D32" t="s">
-        <v>132</v>
-      </c>
+      <c r="B32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F32" t="s">
-        <v>46</v>
+      <c r="F32" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>168</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
+      <c r="B33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" t="s">
+        <v>132</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1773,17 +1777,19 @@
         <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
       <c r="E34" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1794,7 +1800,7 @@
         <v>128</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
@@ -1805,41 +1811,39 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>168</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1859,7 +1863,7 @@
         <v>73</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1869,35 +1873,35 @@
       <c r="B39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="1"/>
+      <c r="C39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
       <c r="E39" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1908,7 +1912,7 @@
         <v>184</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>189</v>
+        <v>97</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1917,7 +1921,7 @@
         <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1928,7 +1932,7 @@
         <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1937,7 +1941,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1948,7 +1952,7 @@
         <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1957,7 +1961,7 @@
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1968,7 +1972,7 @@
         <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1977,7 +1981,7 @@
         <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1988,14 +1992,16 @@
         <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D45" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
       <c r="E45" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2003,14 +2009,12 @@
         <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
         <v>186</v>
       </c>
@@ -2026,7 +2030,7 @@
         <v>194</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>193</v>
+        <v>4</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -2035,25 +2039,27 @@
         <v>186</v>
       </c>
       <c r="F47" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2063,33 +2069,33 @@
       <c r="B49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="2"/>
+      <c r="C49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>170</v>
+        <v>74</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2097,35 +2103,35 @@
         <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>168</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2133,17 +2139,17 @@
         <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E53" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2154,14 +2160,14 @@
         <v>137</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2172,14 +2178,14 @@
         <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,14 +2193,12 @@
         <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
         <v>169</v>
       </c>
@@ -2210,14 +2214,16 @@
         <v>144</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
       <c r="E57" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2225,35 +2231,35 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2261,50 +2267,50 @@
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1</v>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D62" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
       <c r="E62" s="2" t="s">
         <v>70</v>
       </c>
@@ -2317,12 +2323,12 @@
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
         <v>70</v>
       </c>
@@ -2331,39 +2337,39 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>221</v>
+        <v>159</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2373,11 +2379,9 @@
       <c r="B66" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>57</v>
@@ -2394,16 +2398,16 @@
         <v>221</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>227</v>
+        <v>30</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2414,7 +2418,7 @@
         <v>221</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
@@ -2434,9 +2438,11 @@
         <v>221</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D69" s="2"/>
+        <v>224</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
       <c r="E69" s="2" t="s">
         <v>225</v>
       </c>
@@ -2449,17 +2455,17 @@
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
-        <v>57</v>
+        <v>225</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2467,17 +2473,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2485,7 +2491,7 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
@@ -2503,7 +2509,7 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -2521,37 +2527,35 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E74" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2562,7 +2566,7 @@
         <v>91</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
@@ -2571,7 +2575,7 @@
         <v>151</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,14 +2586,16 @@
         <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D77" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
       <c r="E77" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2600,14 +2606,14 @@
         <v>91</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2618,14 +2624,14 @@
         <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2633,56 +2639,54 @@
         <v>168</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D80" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>168</v>
       </c>
-      <c r="B81" t="s">
-        <v>161</v>
-      </c>
-      <c r="D81" t="s">
-        <v>132</v>
+      <c r="B81" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>168</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>79</v>
+      <c r="B82" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82" t="s">
+        <v>132</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2693,16 +2697,16 @@
         <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>75</v>
+      <c r="E83" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2713,16 +2717,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2733,16 +2737,16 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2762,7 +2766,7 @@
         <v>71</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2773,16 +2777,16 @@
         <v>10</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D87" s="2">
         <v>1</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2793,16 +2797,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2812,17 +2816,17 @@
       <c r="B89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="1">
+      <c r="C89" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2832,17 +2836,17 @@
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="1">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2853,14 +2857,16 @@
         <v>10</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
       <c r="E91" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2871,14 +2877,14 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2889,14 +2895,14 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2907,14 +2913,14 @@
         <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2925,14 +2931,14 @@
         <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D95" s="2"/>
-      <c r="E95" s="1" t="s">
-        <v>79</v>
+      <c r="E95" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2940,19 +2946,17 @@
         <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D96" s="2">
-        <v>1</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>70</v>
+        <v>8</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2963,54 +2967,54 @@
         <v>196</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>168</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2" t="s">
+      <c r="D98" s="2"/>
+      <c r="E98" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D98" s="2">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D99" s="1">
+      <c r="C99" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D99" s="2">
         <v>1</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>150</v>
+        <v>233</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>108</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3021,16 +3025,16 @@
         <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D100" s="1">
         <v>1</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3041,16 +3045,16 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>79</v>
+      <c r="E101" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3061,16 +3065,16 @@
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3081,16 +3085,16 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>82</v>
+      <c r="E103" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3101,16 +3105,16 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
       </c>
-      <c r="E104" s="1" t="s">
-        <v>151</v>
+      <c r="E104" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3121,14 +3125,16 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D105" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="D105" s="1">
+        <v>1</v>
+      </c>
       <c r="E105" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3136,17 +3142,17 @@
         <v>168</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3154,17 +3160,17 @@
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3174,17 +3180,15 @@
       <c r="B108" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D108" s="1">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>78</v>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3194,17 +3198,17 @@
       <c r="B109" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D109" s="2">
-        <v>2</v>
+      <c r="C109" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3212,17 +3216,19 @@
         <v>168</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D110" s="2">
+        <v>2</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>148</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3230,35 +3236,35 @@
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3268,17 +3274,15 @@
       <c r="B113" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D113" s="2">
-        <v>1</v>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3289,50 +3293,52 @@
         <v>173</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D114" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D114" s="2">
+        <v>1</v>
+      </c>
       <c r="E114" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F114" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>168</v>
-      </c>
-      <c r="B115" s="1" t="s">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>168</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3342,57 +3348,55 @@
       <c r="B117" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C117" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D117" s="2">
-        <v>1</v>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>204</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D118" s="1">
+      <c r="C118" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D118" s="2">
         <v>1</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>54</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>210</v>
+        <v>55</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>209</v>
+        <v>54</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3403,14 +3407,16 @@
         <v>56</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D120" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1</v>
+      </c>
       <c r="E120" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3421,7 +3427,7 @@
         <v>56</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>201</v>
+        <v>21</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="2" t="s">
@@ -3439,14 +3445,14 @@
         <v>56</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3457,14 +3463,14 @@
         <v>56</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3472,16 +3478,17 @@
         <v>168</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C124" t="s">
-        <v>206</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D124" s="1"/>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3492,7 +3499,7 @@
         <v>216</v>
       </c>
       <c r="C125" t="s">
-        <v>94</v>
+        <v>206</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>199</v>
@@ -3509,7 +3516,7 @@
         <v>216</v>
       </c>
       <c r="C126" t="s">
-        <v>207</v>
+        <v>94</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>199</v>
@@ -3519,40 +3526,37 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>168</v>
-      </c>
-      <c r="B127" t="s">
+      <c r="A127" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C127" t="s">
+        <v>207</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" t="s">
         <v>153</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D128" t="s">
         <v>149</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="E128" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="F128" s="2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C128" t="s">
-        <v>205</v>
-      </c>
-      <c r="D128">
-        <v>2</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3563,7 +3567,7 @@
         <v>153</v>
       </c>
       <c r="C129" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D129">
         <v>2</v>
@@ -3572,24 +3576,27 @@
         <v>199</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>168</v>
-      </c>
-      <c r="B130" t="s">
+      <c r="A130" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C130" t="s">
-        <v>201</v>
+        <v>210</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3600,7 +3607,7 @@
         <v>153</v>
       </c>
       <c r="C131" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>199</v>
@@ -3610,20 +3617,20 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D132" t="s">
-        <v>149</v>
+      <c r="A132" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" t="s">
+        <v>153</v>
+      </c>
+      <c r="C132" t="s">
+        <v>202</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3633,17 +3640,14 @@
       <c r="B133" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C133" t="s">
-        <v>100</v>
-      </c>
-      <c r="D133">
-        <v>1</v>
+      <c r="D133" t="s">
+        <v>149</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3651,19 +3655,19 @@
         <v>168</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C134" t="s">
-        <v>205</v>
+        <v>100</v>
       </c>
       <c r="D134">
         <v>1</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>214</v>
+        <v>54</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3674,7 +3678,7 @@
         <v>215</v>
       </c>
       <c r="C135" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -3683,7 +3687,7 @@
         <v>199</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3691,16 +3695,19 @@
         <v>168</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D136" t="s">
-        <v>149</v>
-      </c>
-      <c r="E136" t="s">
+        <v>215</v>
+      </c>
+      <c r="C136" t="s">
+        <v>210</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F136" t="s">
-        <v>212</v>
+      <c r="F136" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3710,16 +3717,33 @@
       <c r="B137" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C137" t="s">
-        <v>100</v>
-      </c>
-      <c r="D137">
-        <v>1</v>
+      <c r="D137" t="s">
+        <v>149</v>
       </c>
       <c r="E137" t="s">
         <v>199</v>
       </c>
       <c r="F137" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C138" t="s">
+        <v>100</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138" t="s">
+        <v>199</v>
+      </c>
+      <c r="F138" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Map additional samples
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26223"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC01AE-16DB-4BDA-BFA2-AFE22B4DDDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D31D42-3421-411B-A33B-2DD852975A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="240">
   <si>
     <t>Class</t>
   </si>
@@ -734,6 +734,12 @@
   </si>
   <si>
     <t>word-insert-formatted-text</t>
+  </si>
+  <si>
+    <t>BorderType</t>
+  </si>
+  <si>
+    <t>VerticalAlignment</t>
   </si>
 </sst>
 </file>
@@ -782,13 +788,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,8 +852,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F138" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F138" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F140" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F140" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1155,11 +1163,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,72 +1455,72 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" t="s">
-        <v>157</v>
+      <c r="A16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D16" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>158</v>
+      <c r="E16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F16" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="D18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" t="s">
-        <v>130</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1520,7 +1528,7 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
         <v>132</v>
@@ -1529,7 +1537,7 @@
         <v>152</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1537,19 +1545,16 @@
         <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>150</v>
-      </c>
-      <c r="F21" t="s">
-        <v>114</v>
+        <v>131</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1560,7 +1565,7 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1569,7 +1574,7 @@
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1580,7 +1585,7 @@
         <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1589,7 +1594,7 @@
         <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1600,13 +1605,16 @@
         <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1617,13 +1625,13 @@
         <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E25" t="s">
         <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1631,19 +1639,16 @@
         <v>168</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1654,13 +1659,16 @@
         <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>100</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1668,56 +1676,56 @@
         <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>46</v>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>168</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C30" t="s">
-        <v>123</v>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1730,66 +1738,63 @@
       <c r="C31" t="s">
         <v>123</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F31" t="s">
-        <v>126</v>
+      <c r="F31" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>42</v>
+      <c r="C32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>168</v>
       </c>
-      <c r="B33" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" t="s">
-        <v>132</v>
-      </c>
+      <c r="B33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F33" t="s">
-        <v>46</v>
+      <c r="F33" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>168</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1</v>
+      <c r="B34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" t="s">
+        <v>132</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="F34" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1797,17 +1802,19 @@
         <v>168</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
       <c r="E35" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1818,7 +1825,7 @@
         <v>128</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
@@ -1829,41 +1836,39 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1883,7 +1888,7 @@
         <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1893,35 +1898,35 @@
       <c r="B40" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="1"/>
+      <c r="C40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
       <c r="E40" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F40" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1932,7 +1937,7 @@
         <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>189</v>
+        <v>97</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1941,7 +1946,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1952,7 +1957,7 @@
         <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1961,7 +1966,7 @@
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1972,7 +1977,7 @@
         <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1981,7 +1986,7 @@
         <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1992,7 +1997,7 @@
         <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -2001,7 +2006,7 @@
         <v>186</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2012,14 +2017,16 @@
         <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D46" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
       <c r="E46" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,14 +2034,12 @@
         <v>168</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
         <v>186</v>
       </c>
@@ -2050,7 +2055,7 @@
         <v>194</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>193</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
@@ -2059,25 +2064,27 @@
         <v>186</v>
       </c>
       <c r="F48" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>168</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2087,33 +2094,33 @@
       <c r="B50" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="2"/>
+      <c r="C50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="2" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>170</v>
+        <v>74</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2121,35 +2128,35 @@
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2157,17 +2164,17 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D54" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E54" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2178,14 +2185,14 @@
         <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2196,14 +2203,14 @@
         <v>137</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2211,14 +2218,12 @@
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
         <v>169</v>
       </c>
@@ -2234,14 +2239,16 @@
         <v>144</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
       <c r="E58" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2249,35 +2256,35 @@
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2285,50 +2292,50 @@
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>70</v>
       </c>
@@ -2341,12 +2348,12 @@
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
         <v>70</v>
       </c>
@@ -2355,39 +2362,39 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>221</v>
+        <v>159</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2397,11 +2404,9 @@
       <c r="B67" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D67" s="2">
-        <v>1</v>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>57</v>
@@ -2418,16 +2423,16 @@
         <v>221</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>227</v>
+        <v>30</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2438,7 +2443,7 @@
         <v>221</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D69" s="2">
         <v>1</v>
@@ -2458,9 +2463,11 @@
         <v>221</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D70" s="2"/>
+        <v>224</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
       <c r="E70" s="2" t="s">
         <v>225</v>
       </c>
@@ -2473,17 +2480,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>57</v>
+        <v>225</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2491,17 +2498,17 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D72" s="2"/>
       <c r="E72" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2509,7 +2516,7 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -2527,7 +2534,7 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
@@ -2545,37 +2552,35 @@
         <v>168</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>168</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D76" s="2">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2586,7 +2591,7 @@
         <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
@@ -2595,7 +2600,7 @@
         <v>151</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,14 +2611,16 @@
         <v>91</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D78" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
       <c r="E78" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2624,14 +2631,14 @@
         <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2642,14 +2649,14 @@
         <v>91</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2657,56 +2664,54 @@
         <v>168</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>168</v>
       </c>
-      <c r="B82" t="s">
-        <v>161</v>
-      </c>
-      <c r="D82" t="s">
-        <v>132</v>
+      <c r="B82" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>168</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>79</v>
+      <c r="B83" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83" t="s">
+        <v>132</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2717,16 +2722,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>75</v>
+      <c r="E84" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2737,16 +2742,16 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2757,16 +2762,16 @@
         <v>10</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D86" s="2">
         <v>1</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2786,7 +2791,7 @@
         <v>71</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2797,16 +2802,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2817,16 +2822,16 @@
         <v>10</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2836,17 +2841,17 @@
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="1">
+      <c r="C90" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D90" s="2">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2856,17 +2861,17 @@
       <c r="B91" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="1">
         <v>1</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2877,14 +2882,16 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D92" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1</v>
+      </c>
       <c r="E92" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2895,14 +2902,14 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2913,14 +2920,14 @@
         <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2931,14 +2938,14 @@
         <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2949,14 +2956,14 @@
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D96" s="2"/>
-      <c r="E96" s="1" t="s">
-        <v>79</v>
+      <c r="E96" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2964,19 +2971,17 @@
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D97" s="2">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>70</v>
+        <v>8</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2987,54 +2992,54 @@
         <v>196</v>
       </c>
       <c r="C98" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2" t="s">
+      <c r="D99" s="2"/>
+      <c r="E99" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D99" s="2">
-        <v>1</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D100" s="1">
+      <c r="C100" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D100" s="2">
         <v>1</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>150</v>
+        <v>233</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>108</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3045,16 +3050,16 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3065,16 +3070,16 @@
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>79</v>
+      <c r="E102" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3085,16 +3090,16 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3105,16 +3110,16 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>82</v>
+      <c r="E104" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3125,16 +3130,16 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="D105" s="1">
         <v>1</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>151</v>
+      <c r="E105" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3145,14 +3150,16 @@
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D106" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1</v>
+      </c>
       <c r="E106" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3160,17 +3167,17 @@
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D107" s="1"/>
       <c r="E107" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3178,17 +3185,17 @@
         <v>168</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,17 +3205,15 @@
       <c r="B109" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D109" s="1">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>78</v>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3218,17 +3223,17 @@
       <c r="B110" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D110" s="2">
-        <v>2</v>
+      <c r="C110" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D110" s="1">
+        <v>1</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3236,17 +3241,19 @@
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D111" s="2">
+        <v>2</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>148</v>
+        <v>40</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,35 +3261,35 @@
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+      <c r="A113" t="s">
         <v>168</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3292,17 +3299,15 @@
       <c r="B114" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D114" s="2">
-        <v>1</v>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3313,50 +3318,52 @@
         <v>173</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D115" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D115" s="2">
+        <v>1</v>
+      </c>
       <c r="E115" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F115" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F116" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>168</v>
-      </c>
-      <c r="B116" s="1" t="s">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>168</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3366,57 +3373,55 @@
       <c r="B118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D118" s="2">
-        <v>1</v>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>204</v>
+        <v>53</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D119" s="1">
+      <c r="C119" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D119" s="2">
         <v>1</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>54</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+      <c r="A120" t="s">
         <v>168</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>210</v>
+        <v>55</v>
       </c>
       <c r="D120" s="1">
         <v>1</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>209</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3427,14 +3432,16 @@
         <v>56</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D121" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D121" s="1">
+        <v>1</v>
+      </c>
       <c r="E121" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3445,7 +3452,7 @@
         <v>56</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>201</v>
+        <v>21</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="2" t="s">
@@ -3463,14 +3470,14 @@
         <v>56</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3481,14 +3488,14 @@
         <v>56</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3496,16 +3503,17 @@
         <v>168</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C125" t="s">
-        <v>206</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D125" s="1"/>
       <c r="E125" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3516,7 +3524,7 @@
         <v>216</v>
       </c>
       <c r="C126" t="s">
-        <v>94</v>
+        <v>206</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>199</v>
@@ -3533,7 +3541,7 @@
         <v>216</v>
       </c>
       <c r="C127" t="s">
-        <v>207</v>
+        <v>94</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>199</v>
@@ -3543,40 +3551,37 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>168</v>
-      </c>
-      <c r="B128" t="s">
+      <c r="A128" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C128" t="s">
+        <v>207</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>168</v>
+      </c>
+      <c r="B129" t="s">
         <v>153</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D129" t="s">
         <v>149</v>
       </c>
-      <c r="E128" s="2" t="s">
+      <c r="E129" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="F129" s="2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C129" t="s">
-        <v>205</v>
-      </c>
-      <c r="D129">
-        <v>2</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3587,7 +3592,7 @@
         <v>153</v>
       </c>
       <c r="C130" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D130">
         <v>2</v>
@@ -3596,24 +3601,27 @@
         <v>199</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>168</v>
-      </c>
-      <c r="B131" t="s">
+      <c r="A131" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C131" t="s">
-        <v>201</v>
+        <v>210</v>
+      </c>
+      <c r="D131">
+        <v>2</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3624,7 +3632,7 @@
         <v>153</v>
       </c>
       <c r="C132" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>199</v>
@@ -3634,20 +3642,20 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D133" t="s">
-        <v>149</v>
+      <c r="A133" t="s">
+        <v>168</v>
+      </c>
+      <c r="B133" t="s">
+        <v>153</v>
+      </c>
+      <c r="C133" t="s">
+        <v>202</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3657,17 +3665,14 @@
       <c r="B134" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C134" t="s">
-        <v>100</v>
-      </c>
-      <c r="D134">
-        <v>1</v>
+      <c r="D134" t="s">
+        <v>149</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3675,19 +3680,19 @@
         <v>168</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C135" t="s">
-        <v>205</v>
+        <v>100</v>
       </c>
       <c r="D135">
         <v>1</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>214</v>
+        <v>54</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3698,7 +3703,7 @@
         <v>215</v>
       </c>
       <c r="C136" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -3707,7 +3712,7 @@
         <v>199</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3715,16 +3720,19 @@
         <v>168</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D137" t="s">
-        <v>149</v>
-      </c>
-      <c r="E137" t="s">
+        <v>215</v>
+      </c>
+      <c r="C137" t="s">
+        <v>210</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F137" t="s">
-        <v>212</v>
+      <c r="F137" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3734,17 +3742,52 @@
       <c r="B138" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C138" t="s">
-        <v>100</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
+      <c r="D138" t="s">
+        <v>149</v>
       </c>
       <c r="E138" t="s">
         <v>199</v>
       </c>
       <c r="F138" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C139" t="s">
+        <v>100</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="E139" t="s">
+        <v>199</v>
+      </c>
+      <c r="F139" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C140" s="5"/>
+      <c r="D140" t="s">
+        <v>132</v>
+      </c>
+      <c r="E140" t="s">
+        <v>199</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Word] Map additional samples (#763)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26223"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC01AE-16DB-4BDA-BFA2-AFE22B4DDDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D31D42-3421-411B-A33B-2DD852975A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="240">
   <si>
     <t>Class</t>
   </si>
@@ -734,6 +734,12 @@
   </si>
   <si>
     <t>word-insert-formatted-text</t>
+  </si>
+  <si>
+    <t>BorderType</t>
+  </si>
+  <si>
+    <t>VerticalAlignment</t>
   </si>
 </sst>
 </file>
@@ -782,13 +788,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,8 +852,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F138" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F138" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F140" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F140" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1155,11 +1163,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,72 +1455,72 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" t="s">
-        <v>157</v>
+      <c r="A16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D16" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>158</v>
+      <c r="E16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F16" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="D18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" t="s">
-        <v>130</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1520,7 +1528,7 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
         <v>132</v>
@@ -1529,7 +1537,7 @@
         <v>152</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1537,19 +1545,16 @@
         <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>150</v>
-      </c>
-      <c r="F21" t="s">
-        <v>114</v>
+        <v>131</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1560,7 +1565,7 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1569,7 +1574,7 @@
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1580,7 +1585,7 @@
         <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1589,7 +1594,7 @@
         <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1600,13 +1605,16 @@
         <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1617,13 +1625,13 @@
         <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E25" t="s">
         <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1631,19 +1639,16 @@
         <v>168</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1654,13 +1659,16 @@
         <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>100</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1668,56 +1676,56 @@
         <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>46</v>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>168</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C30" t="s">
-        <v>123</v>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1730,66 +1738,63 @@
       <c r="C31" t="s">
         <v>123</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F31" t="s">
-        <v>126</v>
+      <c r="F31" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>42</v>
+      <c r="C32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>168</v>
       </c>
-      <c r="B33" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" t="s">
-        <v>132</v>
-      </c>
+      <c r="B33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F33" t="s">
-        <v>46</v>
+      <c r="F33" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>168</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1</v>
+      <c r="B34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" t="s">
+        <v>132</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="F34" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1797,17 +1802,19 @@
         <v>168</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
       <c r="E35" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1818,7 +1825,7 @@
         <v>128</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
@@ -1829,41 +1836,39 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1883,7 +1888,7 @@
         <v>73</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1893,35 +1898,35 @@
       <c r="B40" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="1"/>
+      <c r="C40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
       <c r="E40" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F40" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1932,7 +1937,7 @@
         <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>189</v>
+        <v>97</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1941,7 +1946,7 @@
         <v>186</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1952,7 +1957,7 @@
         <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1961,7 +1966,7 @@
         <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1972,7 +1977,7 @@
         <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1981,7 +1986,7 @@
         <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1992,7 +1997,7 @@
         <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -2001,7 +2006,7 @@
         <v>186</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2012,14 +2017,16 @@
         <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D46" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
       <c r="E46" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,14 +2034,12 @@
         <v>168</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
         <v>186</v>
       </c>
@@ -2050,7 +2055,7 @@
         <v>194</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>193</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
@@ -2059,25 +2064,27 @@
         <v>186</v>
       </c>
       <c r="F48" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>168</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2087,33 +2094,33 @@
       <c r="B50" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="2"/>
+      <c r="C50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="2" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>170</v>
+        <v>74</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2121,35 +2128,35 @@
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2157,17 +2164,17 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D54" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E54" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2178,14 +2185,14 @@
         <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2196,14 +2203,14 @@
         <v>137</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2211,14 +2218,12 @@
         <v>168</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
         <v>169</v>
       </c>
@@ -2234,14 +2239,16 @@
         <v>144</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
       <c r="E58" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2249,35 +2256,35 @@
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2285,50 +2292,50 @@
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>70</v>
       </c>
@@ -2341,12 +2348,12 @@
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
         <v>70</v>
       </c>
@@ -2355,39 +2362,39 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>221</v>
+        <v>159</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2397,11 +2404,9 @@
       <c r="B67" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D67" s="2">
-        <v>1</v>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>57</v>
@@ -2418,16 +2423,16 @@
         <v>221</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>227</v>
+        <v>30</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2438,7 +2443,7 @@
         <v>221</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D69" s="2">
         <v>1</v>
@@ -2458,9 +2463,11 @@
         <v>221</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D70" s="2"/>
+        <v>224</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
       <c r="E70" s="2" t="s">
         <v>225</v>
       </c>
@@ -2473,17 +2480,17 @@
         <v>168</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>57</v>
+        <v>225</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2491,17 +2498,17 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D72" s="2"/>
       <c r="E72" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2509,7 +2516,7 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -2527,7 +2534,7 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
@@ -2545,37 +2552,35 @@
         <v>168</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>168</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D76" s="2">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2586,7 +2591,7 @@
         <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
@@ -2595,7 +2600,7 @@
         <v>151</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,14 +2611,16 @@
         <v>91</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D78" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
       <c r="E78" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2624,14 +2631,14 @@
         <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2642,14 +2649,14 @@
         <v>91</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2657,56 +2664,54 @@
         <v>168</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>168</v>
       </c>
-      <c r="B82" t="s">
-        <v>161</v>
-      </c>
-      <c r="D82" t="s">
-        <v>132</v>
+      <c r="B82" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>168</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>79</v>
+      <c r="B83" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83" t="s">
+        <v>132</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2717,16 +2722,16 @@
         <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>75</v>
+      <c r="E84" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2737,16 +2742,16 @@
         <v>10</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2757,16 +2762,16 @@
         <v>10</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D86" s="2">
         <v>1</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2786,7 +2791,7 @@
         <v>71</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2797,16 +2802,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2817,16 +2822,16 @@
         <v>10</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2836,17 +2841,17 @@
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="1">
+      <c r="C90" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D90" s="2">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2856,17 +2861,17 @@
       <c r="B91" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="1">
         <v>1</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2877,14 +2882,16 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D92" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1</v>
+      </c>
       <c r="E92" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2895,14 +2902,14 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2913,14 +2920,14 @@
         <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2931,14 +2938,14 @@
         <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2949,14 +2956,14 @@
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D96" s="2"/>
-      <c r="E96" s="1" t="s">
-        <v>79</v>
+      <c r="E96" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2964,19 +2971,17 @@
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D97" s="2">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>70</v>
+        <v>8</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2987,54 +2992,54 @@
         <v>196</v>
       </c>
       <c r="C98" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2" t="s">
+      <c r="D99" s="2"/>
+      <c r="E99" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D99" s="2">
-        <v>1</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D100" s="1">
+      <c r="C100" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D100" s="2">
         <v>1</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>150</v>
+        <v>233</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>108</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3045,16 +3050,16 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3065,16 +3070,16 @@
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>79</v>
+      <c r="E102" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3085,16 +3090,16 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3105,16 +3110,16 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>82</v>
+      <c r="E104" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3125,16 +3130,16 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="D105" s="1">
         <v>1</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>151</v>
+      <c r="E105" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3145,14 +3150,16 @@
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D106" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1</v>
+      </c>
       <c r="E106" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3160,17 +3167,17 @@
         <v>168</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D107" s="1"/>
       <c r="E107" s="1" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3178,17 +3185,17 @@
         <v>168</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,17 +3205,15 @@
       <c r="B109" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D109" s="1">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>78</v>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3218,17 +3223,17 @@
       <c r="B110" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D110" s="2">
-        <v>2</v>
+      <c r="C110" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D110" s="1">
+        <v>1</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3236,17 +3241,19 @@
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D111" s="2">
+        <v>2</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>148</v>
+        <v>40</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,35 +3261,35 @@
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+      <c r="A113" t="s">
         <v>168</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3292,17 +3299,15 @@
       <c r="B114" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D114" s="2">
-        <v>1</v>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3313,50 +3318,52 @@
         <v>173</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D115" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D115" s="2">
+        <v>1</v>
+      </c>
       <c r="E115" s="2" t="s">
         <v>170</v>
       </c>
       <c r="F115" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F116" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>168</v>
-      </c>
-      <c r="B116" s="1" t="s">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>168</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3366,57 +3373,55 @@
       <c r="B118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D118" s="2">
-        <v>1</v>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>204</v>
+        <v>53</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D119" s="1">
+      <c r="C119" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D119" s="2">
         <v>1</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>54</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+      <c r="A120" t="s">
         <v>168</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>210</v>
+        <v>55</v>
       </c>
       <c r="D120" s="1">
         <v>1</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>209</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3427,14 +3432,16 @@
         <v>56</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D121" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D121" s="1">
+        <v>1</v>
+      </c>
       <c r="E121" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3445,7 +3452,7 @@
         <v>56</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>201</v>
+        <v>21</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="2" t="s">
@@ -3463,14 +3470,14 @@
         <v>56</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3481,14 +3488,14 @@
         <v>56</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3496,16 +3503,17 @@
         <v>168</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C125" t="s">
-        <v>206</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D125" s="1"/>
       <c r="E125" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3516,7 +3524,7 @@
         <v>216</v>
       </c>
       <c r="C126" t="s">
-        <v>94</v>
+        <v>206</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>199</v>
@@ -3533,7 +3541,7 @@
         <v>216</v>
       </c>
       <c r="C127" t="s">
-        <v>207</v>
+        <v>94</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>199</v>
@@ -3543,40 +3551,37 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>168</v>
-      </c>
-      <c r="B128" t="s">
+      <c r="A128" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C128" t="s">
+        <v>207</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>168</v>
+      </c>
+      <c r="B129" t="s">
         <v>153</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D129" t="s">
         <v>149</v>
       </c>
-      <c r="E128" s="2" t="s">
+      <c r="E129" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="F129" s="2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C129" t="s">
-        <v>205</v>
-      </c>
-      <c r="D129">
-        <v>2</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3587,7 +3592,7 @@
         <v>153</v>
       </c>
       <c r="C130" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D130">
         <v>2</v>
@@ -3596,24 +3601,27 @@
         <v>199</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>168</v>
-      </c>
-      <c r="B131" t="s">
+      <c r="A131" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C131" t="s">
-        <v>201</v>
+        <v>210</v>
+      </c>
+      <c r="D131">
+        <v>2</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3624,7 +3632,7 @@
         <v>153</v>
       </c>
       <c r="C132" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>199</v>
@@ -3634,20 +3642,20 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D133" t="s">
-        <v>149</v>
+      <c r="A133" t="s">
+        <v>168</v>
+      </c>
+      <c r="B133" t="s">
+        <v>153</v>
+      </c>
+      <c r="C133" t="s">
+        <v>202</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3657,17 +3665,14 @@
       <c r="B134" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C134" t="s">
-        <v>100</v>
-      </c>
-      <c r="D134">
-        <v>1</v>
+      <c r="D134" t="s">
+        <v>149</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3675,19 +3680,19 @@
         <v>168</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C135" t="s">
-        <v>205</v>
+        <v>100</v>
       </c>
       <c r="D135">
         <v>1</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>214</v>
+        <v>54</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3698,7 +3703,7 @@
         <v>215</v>
       </c>
       <c r="C136" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -3707,7 +3712,7 @@
         <v>199</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3715,16 +3720,19 @@
         <v>168</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D137" t="s">
-        <v>149</v>
-      </c>
-      <c r="E137" t="s">
+        <v>215</v>
+      </c>
+      <c r="C137" t="s">
+        <v>210</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F137" t="s">
-        <v>212</v>
+      <c r="F137" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3734,17 +3742,52 @@
       <c r="B138" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C138" t="s">
-        <v>100</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
+      <c r="D138" t="s">
+        <v>149</v>
       </c>
       <c r="E138" t="s">
         <v>199</v>
       </c>
       <c r="F138" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C139" t="s">
+        <v>100</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="E139" t="s">
+        <v>199</v>
+      </c>
+      <c r="F139" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C140" s="5"/>
+      <c r="D140" t="s">
+        <v>132</v>
+      </c>
+      <c r="E140" t="s">
+        <v>199</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Word] Add snippet showing how to insert a document
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D31D42-3421-411B-A33B-2DD852975A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8B44A5-EA22-4D36-BD3B-02A9CD4FB5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="246">
   <si>
     <t>Class</t>
   </si>
@@ -740,6 +740,24 @@
   </si>
   <si>
     <t>VerticalAlignment</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>createDocument</t>
+  </si>
+  <si>
+    <t>word-document-insert-external-document</t>
+  </si>
+  <si>
+    <t>insertDocument</t>
+  </si>
+  <si>
+    <t>getBase64</t>
+  </si>
+  <si>
+    <t>DocumentCreated</t>
   </si>
 </sst>
 </file>
@@ -788,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -797,6 +815,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,8 +873,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F140" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F140" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F144" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F144" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1163,11 +1184,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1218,63 +1239,63 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>107</v>
+      <c r="A3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" t="s">
-        <v>107</v>
+      <c r="E3" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>68</v>
+      <c r="A4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>168</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>53</v>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1285,16 +1306,16 @@
         <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1304,69 +1325,74 @@
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>168</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F8" t="s">
-        <v>136</v>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>168</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" t="s">
-        <v>151</v>
-      </c>
-      <c r="F9" t="s">
-        <v>90</v>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>168</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>23</v>
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1377,47 +1403,48 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="F11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>197</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" t="s">
-        <v>54</v>
+      <c r="C12" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>168</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1425,33 +1452,33 @@
         <v>168</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D14" t="s">
-        <v>132</v>
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>151</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D15" t="s">
-        <v>132</v>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
       </c>
       <c r="E15" t="s">
-        <v>199</v>
+        <v>151</v>
       </c>
       <c r="F15" t="s">
-        <v>204</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1459,102 +1486,102 @@
         <v>168</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>238</v>
+        <v>195</v>
       </c>
       <c r="D16" t="s">
         <v>132</v>
       </c>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>151</v>
       </c>
       <c r="F16" t="s">
-        <v>219</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" t="s">
-        <v>157</v>
+      <c r="A17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>158</v>
+      <c r="E17" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D18" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>134</v>
+      <c r="E18" t="s">
+        <v>199</v>
+      </c>
+      <c r="F18" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>208</v>
+      <c r="A19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" t="s">
+        <v>157</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>199</v>
+        <v>75</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>209</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>168</v>
       </c>
-      <c r="B20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B20" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>152</v>
+        <v>237</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" t="s">
-        <v>131</v>
+      <c r="A21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="D21" t="s">
         <v>132</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>122</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1562,19 +1589,16 @@
         <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>150</v>
-      </c>
-      <c r="F22" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1582,19 +1606,16 @@
         <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>150</v>
-      </c>
-      <c r="F23" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="D23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1605,7 +1626,7 @@
         <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1614,7 +1635,7 @@
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1625,13 +1646,16 @@
         <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1642,13 +1666,16 @@
         <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1656,19 +1683,16 @@
         <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E27" t="s">
         <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1676,16 +1700,16 @@
         <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="E28" t="s">
         <v>150</v>
       </c>
       <c r="F28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1693,39 +1717,36 @@
         <v>168</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>46</v>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1736,48 +1757,53 @@
         <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>125</v>
+      <c r="F31" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C32" t="s">
-        <v>123</v>
-      </c>
-      <c r="E32" t="s">
-        <v>124</v>
-      </c>
-      <c r="F32" t="s">
-        <v>126</v>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>168</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="2"/>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
       <c r="E33" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>42</v>
+        <v>124</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1785,16 +1811,16 @@
         <v>168</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
-      </c>
-      <c r="D34" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" t="s">
+        <v>124</v>
       </c>
       <c r="F34" t="s">
-        <v>46</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1802,37 +1828,34 @@
         <v>168</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="1"/>
+      <c r="B36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" t="s">
+        <v>132</v>
+      </c>
       <c r="E36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>126</v>
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1840,35 +1863,37 @@
         <v>168</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2" t="s">
+      <c r="C38" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1876,39 +1901,35 @@
         <v>168</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="2">
-        <v>1</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>60</v>
+        <v>124</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1918,55 +1939,55 @@
       <c r="B41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="1"/>
+      <c r="C41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>168</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1977,7 +1998,7 @@
         <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>190</v>
+        <v>97</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1986,7 +2007,7 @@
         <v>186</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1997,7 +2018,7 @@
         <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -2006,7 +2027,7 @@
         <v>186</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2017,7 +2038,7 @@
         <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -2026,7 +2047,7 @@
         <v>186</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2037,14 +2058,16 @@
         <v>184</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D47" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
       <c r="E47" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2052,10 +2075,10 @@
         <v>168</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
@@ -2064,7 +2087,7 @@
         <v>186</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2072,163 +2095,165 @@
         <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F49" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>168</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2" t="s">
+      <c r="D54" s="2"/>
+      <c r="E54" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" s="1" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>168</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>168</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>168</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>168</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2236,19 +2261,17 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D58" s="2">
-        <v>1</v>
+        <v>166</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2256,17 +2279,17 @@
         <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2274,53 +2297,55 @@
         <v>168</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2328,37 +2353,35 @@
         <v>168</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D63" s="2">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>168</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E64" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2366,11 +2389,11 @@
         <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>70</v>
@@ -2380,39 +2403,41 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>168</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2" t="s">
-        <v>149</v>
+        <v>25</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2420,19 +2445,17 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>221</v>
+        <v>25</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D68" s="2">
-        <v>1</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2440,39 +2463,35 @@
         <v>168</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
+        <v>183</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>225</v>
+        <v>70</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>226</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D70" s="2">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>225</v>
+        <v>145</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>226</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2482,15 +2501,15 @@
       <c r="B71" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E71" s="2" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2498,12 +2517,14 @@
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D72" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
       <c r="E72" s="2" t="s">
         <v>57</v>
       </c>
@@ -2516,11 +2537,13 @@
         <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2" t="s">
-        <v>132</v>
+        <v>221</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>225</v>
@@ -2534,11 +2557,13 @@
         <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2" t="s">
-        <v>132</v>
+        <v>221</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>225</v>
@@ -2552,12 +2577,12 @@
         <v>168</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D75" s="2"/>
       <c r="E75" s="2" t="s">
         <v>225</v>
       </c>
@@ -2570,93 +2595,89 @@
         <v>168</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2" t="s">
+      <c r="C80" s="2"/>
+      <c r="D80" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>168</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>168</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>168</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2667,14 +2688,16 @@
         <v>91</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D81" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
       <c r="E81" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2682,10 +2705,10 @@
         <v>168</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D82" s="2">
         <v>1</v>
@@ -2694,24 +2717,25 @@
         <v>151</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>168</v>
       </c>
-      <c r="B83" t="s">
-        <v>161</v>
-      </c>
-      <c r="D83" t="s">
-        <v>132</v>
-      </c>
+      <c r="B83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D83" s="2"/>
       <c r="E83" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2719,19 +2743,17 @@
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D84" s="2">
-        <v>1</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2739,19 +2761,17 @@
         <v>168</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D85" s="2">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D85" s="2"/>
       <c r="E85" s="2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2759,39 +2779,36 @@
         <v>168</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="D86" s="2">
         <v>1</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>168</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D87" s="2">
-        <v>1</v>
+      <c r="B87" t="s">
+        <v>161</v>
+      </c>
+      <c r="D87" t="s">
+        <v>132</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2802,16 +2819,16 @@
         <v>10</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>71</v>
+      <c r="E88" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2822,16 +2839,16 @@
         <v>10</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2842,16 +2859,16 @@
         <v>10</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D90" s="2">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2861,17 +2878,17 @@
       <c r="B91" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="1">
+      <c r="C91" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D91" s="2">
         <v>1</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2882,16 +2899,16 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D92" s="2">
         <v>1</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2902,14 +2919,16 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D93" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1</v>
+      </c>
       <c r="E93" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2920,14 +2939,16 @@
         <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D94" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1</v>
+      </c>
       <c r="E94" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2937,15 +2958,17 @@
       <c r="B95" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D95" s="2"/>
+      <c r="C95" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1</v>
+      </c>
       <c r="E95" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2956,14 +2979,16 @@
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D96" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
       <c r="E96" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2974,14 +2999,14 @@
         <v>10</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D97" s="2"/>
-      <c r="E97" s="1" t="s">
-        <v>79</v>
+      <c r="E97" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2989,19 +3014,17 @@
         <v>168</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D98" s="2">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D98" s="2"/>
       <c r="E98" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>181</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -3009,37 +3032,35 @@
         <v>168</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+      <c r="A100" t="s">
         <v>168</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D100" s="2">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D100" s="2"/>
       <c r="E100" s="2" t="s">
-        <v>233</v>
+        <v>80</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>234</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3047,19 +3068,17 @@
         <v>168</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D101" s="1">
-        <v>1</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>150</v>
+        <v>10</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3067,19 +3086,19 @@
         <v>168</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D102" s="1">
+        <v>196</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D102" s="2">
         <v>1</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3087,39 +3106,37 @@
         <v>168</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D103" s="1">
-        <v>1</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>79</v>
+        <v>196</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="A104" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D104" s="1">
-        <v>1</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>150</v>
+      <c r="C104" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D104" s="2">
+        <v>1</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>106</v>
+        <v>234</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3130,16 +3147,16 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="D105" s="1">
         <v>1</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3150,16 +3167,16 @@
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D106" s="1">
         <v>1</v>
       </c>
-      <c r="E106" s="1" t="s">
-        <v>151</v>
+      <c r="E106" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3170,14 +3187,16 @@
         <v>5</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D107" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D107" s="1">
+        <v>1</v>
+      </c>
       <c r="E107" s="1" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3185,17 +3204,19 @@
         <v>168</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1" t="s">
-        <v>132</v>
+        <v>5</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D108" s="1">
+        <v>1</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3203,17 +3224,19 @@
         <v>168</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>145</v>
+        <v>5</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>146</v>
+        <v>35</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3221,19 +3244,19 @@
         <v>168</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D110" s="1">
         <v>1</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>78</v>
+      <c r="E110" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3241,19 +3264,17 @@
         <v>168</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D111" s="2">
-        <v>2</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3261,17 +3282,17 @@
         <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>145</v>
+        <v>163</v>
+      </c>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>148</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3279,73 +3300,75 @@
         <v>168</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>71</v>
+        <v>27</v>
+      </c>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+      <c r="A114" t="s">
         <v>168</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C114" s="2"/>
-      <c r="D114" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>168</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D115" s="2">
+        <v>2</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>168</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D115" s="2">
-        <v>1</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D116" s="2"/>
       <c r="E116" s="2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3353,17 +3376,17 @@
         <v>168</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>134</v>
+        <v>49</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3371,17 +3394,17 @@
         <v>168</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3389,59 +3412,55 @@
         <v>168</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>205</v>
+        <v>4</v>
       </c>
       <c r="D119" s="2">
         <v>1</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D120" s="1">
-        <v>1</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D120" s="2"/>
       <c r="E120" s="2" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
+      <c r="A121" t="s">
         <v>168</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D121" s="1">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>199</v>
+        <v>76</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>209</v>
+        <v>134</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3451,15 +3470,15 @@
       <c r="B122" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D122" s="1"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E122" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>200</v>
+        <v>53</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3469,33 +3488,37 @@
       <c r="B123" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D123" s="1"/>
+      <c r="C123" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D123" s="2">
+        <v>1</v>
+      </c>
       <c r="E123" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+      <c r="A124" t="s">
         <v>168</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D124" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="D124" s="1">
+        <v>1</v>
+      </c>
       <c r="E124" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3506,14 +3529,16 @@
         <v>56</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D125" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D125" s="1">
+        <v>1</v>
+      </c>
       <c r="E125" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3521,16 +3546,17 @@
         <v>168</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C126" t="s">
-        <v>206</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D126" s="1"/>
       <c r="E126" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3538,16 +3564,17 @@
         <v>168</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C127" t="s">
-        <v>94</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D127" s="1"/>
       <c r="E127" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3555,33 +3582,35 @@
         <v>168</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C128" t="s">
-        <v>207</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D128" s="1"/>
       <c r="E128" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>168</v>
-      </c>
-      <c r="B129" t="s">
-        <v>153</v>
-      </c>
-      <c r="D129" t="s">
-        <v>149</v>
-      </c>
+      <c r="A129" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D129" s="1"/>
       <c r="E129" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3589,19 +3618,16 @@
         <v>168</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="C130" t="s">
-        <v>205</v>
-      </c>
-      <c r="D130">
-        <v>2</v>
+        <v>206</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3609,36 +3635,33 @@
         <v>168</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="C131" t="s">
-        <v>210</v>
-      </c>
-      <c r="D131">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>168</v>
-      </c>
-      <c r="B132" t="s">
-        <v>153</v>
+      <c r="A132" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C132" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3648,14 +3671,14 @@
       <c r="B133" t="s">
         <v>153</v>
       </c>
-      <c r="C133" t="s">
-        <v>202</v>
+      <c r="D133" t="s">
+        <v>149</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>218</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3663,16 +3686,19 @@
         <v>168</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D134" t="s">
-        <v>149</v>
+        <v>153</v>
+      </c>
+      <c r="C134" t="s">
+        <v>205</v>
+      </c>
+      <c r="D134">
+        <v>2</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3680,59 +3706,53 @@
         <v>168</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="C135" t="s">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="D135">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>215</v>
+      <c r="A136" t="s">
+        <v>168</v>
+      </c>
+      <c r="B136" t="s">
+        <v>153</v>
       </c>
       <c r="C136" t="s">
-        <v>205</v>
-      </c>
-      <c r="D136">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>215</v>
+      <c r="A137" t="s">
+        <v>168</v>
+      </c>
+      <c r="B137" t="s">
+        <v>153</v>
       </c>
       <c r="C137" t="s">
-        <v>210</v>
-      </c>
-      <c r="D137">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>199</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3740,16 +3760,16 @@
         <v>168</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D138" t="s">
         <v>149</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E138" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F138" t="s">
-        <v>212</v>
+      <c r="F138" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3757,7 +3777,7 @@
         <v>168</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C139" t="s">
         <v>100</v>
@@ -3765,28 +3785,104 @@
       <c r="D139">
         <v>1</v>
       </c>
-      <c r="E139" t="s">
-        <v>199</v>
-      </c>
-      <c r="F139" t="s">
-        <v>214</v>
+      <c r="E139" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C140" t="s">
+        <v>205</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C141" t="s">
+        <v>210</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D142" t="s">
+        <v>149</v>
+      </c>
+      <c r="E142" t="s">
+        <v>199</v>
+      </c>
+      <c r="F142" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C143" t="s">
+        <v>100</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143" t="s">
+        <v>199</v>
+      </c>
+      <c r="F143" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C140" s="5"/>
-      <c r="D140" t="s">
+      <c r="D144" t="s">
         <v>132</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E144" t="s">
         <v>199</v>
       </c>
-      <c r="F140" s="5" t="s">
+      <c r="F144" t="s">
         <v>212</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Word] Add snippet showing how to insert a document (#772)
* [Word] Add snippet showing how to insert a document

* Apply suggestions from code review

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>

* Updates based on feedback

---------

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/word.xlsx
+++ b/snippet-extractor-metadata/word.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D31D42-3421-411B-A33B-2DD852975A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2DC27C-FFC8-4CB7-99A0-4AB100ABF134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="245">
   <si>
     <t>Class</t>
   </si>
@@ -740,6 +740,21 @@
   </si>
   <si>
     <t>VerticalAlignment</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>createDocument</t>
+  </si>
+  <si>
+    <t>word-document-insert-external-document</t>
+  </si>
+  <si>
+    <t>insertDocument</t>
+  </si>
+  <si>
+    <t>DocumentCreated</t>
   </si>
 </sst>
 </file>
@@ -788,15 +803,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,8 +865,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F140" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F140" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F142" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F142" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{1DA12987-AB2C-4056-A643-B1229DC856C5}" name="Package" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1163,11 +1176,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2"